<commit_message>
modeling the combined data mills 6,7,8
</commit_message>
<xml_diff>
--- a/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
+++ b/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
@@ -3,14 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F271A7F6-0866-4D37-A078-FD1B7F2FCB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7821C385-163F-4051-ADD6-1EF91D4DCF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Юни" sheetId="6" r:id="rId1"/>
     <sheet name="Юли" sheetId="7" r:id="rId2"/>
+    <sheet name="Август" sheetId="8" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -620,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="70">
   <si>
     <t xml:space="preserve">Подадена руда
  от МГТЛ 
@@ -864,6 +868,18 @@
   <si>
     <t>Смилане 
  класа     + 0,20мм</t>
+  </si>
+  <si>
+    <t>Класа 
+ +12,5мм.</t>
+  </si>
+  <si>
+    <t>Смилане 
+ класа         +0,20мм</t>
+  </si>
+  <si>
+    <t>Меден 
+концентра, автомобилна везна</t>
   </si>
 </sst>
 </file>
@@ -1672,9 +1688,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1682,9 +1695,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1705,6 +1715,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1722,6 +1738,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Януари "/>
+      <sheetName val="Февруари"/>
+      <sheetName val="Март"/>
+      <sheetName val="Април"/>
+      <sheetName val="Май"/>
+      <sheetName val="Юни"/>
+      <sheetName val="Юли"/>
+      <sheetName val="Август"/>
+      <sheetName val="Септември"/>
+      <sheetName val="Октомври"/>
+      <sheetName val="Ноември"/>
+      <sheetName val="Декември"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
+        <row r="127">
+          <cell r="AU127">
+            <v>1478.34</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2014,7 +2074,7 @@
   <dimension ref="A1:BA132"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="P1" sqref="P1:P1048576"/>
@@ -2079,13 +2139,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="189" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="187" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="187" t="s">
+      <c r="C1" s="185" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -2214,19 +2274,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="182" t="s">
+      <c r="AX1" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="182"/>
-      <c r="AZ1" s="182" t="s">
+      <c r="AY1" s="191"/>
+      <c r="AZ1" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="182"/>
+      <c r="BA1" s="191"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="192"/>
-      <c r="B2" s="190"/>
-      <c r="C2" s="188"/>
+      <c r="A2" s="190"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -2417,7 +2477,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="183">
+      <c r="A4" s="182">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -2579,7 +2639,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="184"/>
+      <c r="A5" s="183"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -2739,7 +2799,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="184"/>
+      <c r="A6" s="183"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -2899,7 +2959,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185"/>
+      <c r="A7" s="184"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -3070,7 +3130,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="183">
+      <c r="A8" s="182">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -3234,7 +3294,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="184"/>
+      <c r="A9" s="183"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -3394,7 +3454,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="184"/>
+      <c r="A10" s="183"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -3554,7 +3614,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="185"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -3725,7 +3785,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="183">
+      <c r="A12" s="182">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -3889,7 +3949,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="184"/>
+      <c r="A13" s="183"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -4049,7 +4109,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="184"/>
+      <c r="A14" s="183"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -4209,7 +4269,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="185"/>
+      <c r="A15" s="184"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -4380,7 +4440,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183">
+      <c r="A16" s="182">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -4544,7 +4604,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="184"/>
+      <c r="A17" s="183"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -4704,7 +4764,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="184"/>
+      <c r="A18" s="183"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -4864,7 +4924,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="185"/>
+      <c r="A19" s="184"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -5035,7 +5095,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183">
+      <c r="A20" s="182">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -5199,7 +5259,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="184"/>
+      <c r="A21" s="183"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -5359,7 +5419,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="184"/>
+      <c r="A22" s="183"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -5519,7 +5579,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="185"/>
+      <c r="A23" s="184"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -5690,7 +5750,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="183">
+      <c r="A24" s="182">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -5856,7 +5916,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="184"/>
+      <c r="A25" s="183"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -6016,7 +6076,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="184"/>
+      <c r="A26" s="183"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -6176,7 +6236,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="185"/>
+      <c r="A27" s="184"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -6347,7 +6407,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="183">
+      <c r="A28" s="182">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -6509,7 +6569,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="184"/>
+      <c r="A29" s="183"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -6669,7 +6729,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="184"/>
+      <c r="A30" s="183"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -6829,7 +6889,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="185"/>
+      <c r="A31" s="184"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -7000,7 +7060,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="183">
+      <c r="A32" s="182">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -7162,7 +7222,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="184"/>
+      <c r="A33" s="183"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -7322,7 +7382,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="184"/>
+      <c r="A34" s="183"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -7482,7 +7542,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="185"/>
+      <c r="A35" s="184"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -7653,7 +7713,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="183">
+      <c r="A36" s="182">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -7817,7 +7877,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="184"/>
+      <c r="A37" s="183"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -7977,7 +8037,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="184"/>
+      <c r="A38" s="183"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -8137,7 +8197,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="185"/>
+      <c r="A39" s="184"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -8308,7 +8368,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="183">
+      <c r="A40" s="182">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -8472,7 +8532,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="184"/>
+      <c r="A41" s="183"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -8632,7 +8692,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="184"/>
+      <c r="A42" s="183"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -8792,7 +8852,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="185"/>
+      <c r="A43" s="184"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -8963,7 +9023,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="183">
+      <c r="A44" s="182">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -9127,7 +9187,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="184"/>
+      <c r="A45" s="183"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -9287,7 +9347,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="184"/>
+      <c r="A46" s="183"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -9447,7 +9507,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="185"/>
+      <c r="A47" s="184"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -9618,7 +9678,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="183">
+      <c r="A48" s="182">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -9784,7 +9844,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="184"/>
+      <c r="A49" s="183"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -9944,7 +10004,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="184"/>
+      <c r="A50" s="183"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -10104,7 +10164,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="185"/>
+      <c r="A51" s="184"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -10275,7 +10335,7 @@
       <c r="BA51" s="57"/>
     </row>
     <row r="52" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="183">
+      <c r="A52" s="182">
         <v>13</v>
       </c>
       <c r="B52" s="22">
@@ -10439,7 +10499,7 @@
       <c r="BA52" s="19"/>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A53" s="184"/>
+      <c r="A53" s="183"/>
       <c r="B53" s="32">
         <v>2</v>
       </c>
@@ -10599,7 +10659,7 @@
       <c r="BA53" s="44"/>
     </row>
     <row r="54" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A54" s="184"/>
+      <c r="A54" s="183"/>
       <c r="B54" s="32">
         <v>3</v>
       </c>
@@ -10759,7 +10819,7 @@
       <c r="BA54" s="40"/>
     </row>
     <row r="55" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="185"/>
+      <c r="A55" s="184"/>
       <c r="B55" s="48" t="s">
         <v>35</v>
       </c>
@@ -10930,7 +10990,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="183">
+      <c r="A56" s="182">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -11092,7 +11152,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="184"/>
+      <c r="A57" s="183"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -11252,7 +11312,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="184"/>
+      <c r="A58" s="183"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -11412,7 +11472,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="185"/>
+      <c r="A59" s="184"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -11583,7 +11643,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="183">
+      <c r="A60" s="182">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -11745,7 +11805,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="184"/>
+      <c r="A61" s="183"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -11905,7 +11965,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="184"/>
+      <c r="A62" s="183"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -12065,7 +12125,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="185"/>
+      <c r="A63" s="184"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -12236,7 +12296,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="183">
+      <c r="A64" s="182">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -12400,7 +12460,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="184"/>
+      <c r="A65" s="183"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -12560,7 +12620,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="184"/>
+      <c r="A66" s="183"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -12720,7 +12780,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="185"/>
+      <c r="A67" s="184"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -12891,7 +12951,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="183">
+      <c r="A68" s="182">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -13055,7 +13115,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="184"/>
+      <c r="A69" s="183"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -13215,7 +13275,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="184"/>
+      <c r="A70" s="183"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -13375,7 +13435,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="185"/>
+      <c r="A71" s="184"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -13546,7 +13606,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="183">
+      <c r="A72" s="182">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -13712,7 +13772,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="184"/>
+      <c r="A73" s="183"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -13872,7 +13932,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="184"/>
+      <c r="A74" s="183"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -14032,7 +14092,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="185"/>
+      <c r="A75" s="184"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -14203,7 +14263,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="183">
+      <c r="A76" s="182">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -14367,7 +14427,7 @@
       <c r="BA76" s="175"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="184"/>
+      <c r="A77" s="183"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -14527,7 +14587,7 @@
       <c r="BA77" s="176"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="184"/>
+      <c r="A78" s="183"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -14687,7 +14747,7 @@
       <c r="BA78" s="177"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="185"/>
+      <c r="A79" s="184"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -14858,7 +14918,7 @@
       <c r="BA79" s="179"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="184">
+      <c r="A80" s="183">
         <v>20</v>
       </c>
       <c r="B80" s="32">
@@ -15024,7 +15084,7 @@
       <c r="BA80" s="168"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="184"/>
+      <c r="A81" s="183"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -15184,7 +15244,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="184"/>
+      <c r="A82" s="183"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -15344,7 +15404,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="185"/>
+      <c r="A83" s="184"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -15515,7 +15575,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="183">
+      <c r="A84" s="182">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -15677,7 +15737,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="184"/>
+      <c r="A85" s="183"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -15837,7 +15897,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="184"/>
+      <c r="A86" s="183"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -15997,7 +16057,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="185"/>
+      <c r="A87" s="184"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -16168,7 +16228,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="183">
+      <c r="A88" s="182">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -16330,7 +16390,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="184"/>
+      <c r="A89" s="183"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -16490,7 +16550,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="184"/>
+      <c r="A90" s="183"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -16650,7 +16710,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="185"/>
+      <c r="A91" s="184"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -16821,7 +16881,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="183">
+      <c r="A92" s="182">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -16985,7 +17045,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="184"/>
+      <c r="A93" s="183"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -17145,7 +17205,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="184"/>
+      <c r="A94" s="183"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -17305,7 +17365,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="185"/>
+      <c r="A95" s="184"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -17476,7 +17536,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="183">
+      <c r="A96" s="182">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -17642,7 +17702,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="184"/>
+      <c r="A97" s="183"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -17802,7 +17862,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="184"/>
+      <c r="A98" s="183"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -17962,7 +18022,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="185"/>
+      <c r="A99" s="184"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -18130,7 +18190,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="186">
+      <c r="A100" s="192">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -18296,7 +18356,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="186"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -18456,7 +18516,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="186"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -18616,7 +18676,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="186"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -18787,7 +18847,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="183">
+      <c r="A104" s="182">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -18953,7 +19013,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="184"/>
+      <c r="A105" s="183"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -19113,7 +19173,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="184"/>
+      <c r="A106" s="183"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -19273,7 +19333,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="185"/>
+      <c r="A107" s="184"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -19444,7 +19504,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="183">
+      <c r="A108" s="182">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -19610,7 +19670,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="184"/>
+      <c r="A109" s="183"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -19770,7 +19830,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="184"/>
+      <c r="A110" s="183"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -19930,7 +19990,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="185"/>
+      <c r="A111" s="184"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -20101,7 +20161,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="183">
+      <c r="A112" s="182">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -20263,7 +20323,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="184"/>
+      <c r="A113" s="183"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -20423,7 +20483,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="184"/>
+      <c r="A114" s="183"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -20583,7 +20643,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="185"/>
+      <c r="A115" s="184"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -20754,7 +20814,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="184">
+      <c r="A116" s="183">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -20916,7 +20976,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="184"/>
+      <c r="A117" s="183"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -21076,7 +21136,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="184"/>
+      <c r="A118" s="183"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -21236,7 +21296,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="185"/>
+      <c r="A119" s="184"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -21407,7 +21467,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="183">
+      <c r="A120" s="182">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -21573,7 +21633,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="184"/>
+      <c r="A121" s="183"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -21733,7 +21793,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="184"/>
+      <c r="A122" s="183"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -21893,7 +21953,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="185"/>
+      <c r="A123" s="184"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -22064,7 +22124,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="183">
+      <c r="A124" s="182">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -22174,7 +22234,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="184"/>
+      <c r="A125" s="183"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -22282,7 +22342,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="184"/>
+      <c r="A126" s="183"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -22390,7 +22450,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="185"/>
+      <c r="A127" s="184"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -22783,26 +22843,6 @@
     <protectedRange sqref="AB1" name="Range1_1_1_1_1_1_1_1_1_1_1"/>
   </protectedRanges>
   <mergeCells count="36">
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A100:A103"/>
@@ -22819,6 +22859,26 @@
     <mergeCell ref="A68:A71"/>
     <mergeCell ref="A84:A87"/>
     <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -22830,8 +22890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BA128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D122" sqref="D122"/>
@@ -22896,13 +22956,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="189" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="189" t="s">
+      <c r="B1" s="187" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="187" t="s">
+      <c r="C1" s="185" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -23031,19 +23091,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="182" t="s">
+      <c r="AX1" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="182"/>
-      <c r="AZ1" s="182" t="s">
+      <c r="AY1" s="191"/>
+      <c r="AZ1" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="182"/>
+      <c r="BA1" s="191"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="192"/>
-      <c r="B2" s="190"/>
-      <c r="C2" s="188"/>
+      <c r="A2" s="190"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="186"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -23234,7 +23294,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="183">
+      <c r="A4" s="182">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -23398,7 +23458,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="184"/>
+      <c r="A5" s="183"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -23557,7 +23617,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="184"/>
+      <c r="A6" s="183"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -23716,7 +23776,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185"/>
+      <c r="A7" s="184"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -23887,7 +23947,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="183">
+      <c r="A8" s="182">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -24051,7 +24111,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="184"/>
+      <c r="A9" s="183"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -24211,7 +24271,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="184"/>
+      <c r="A10" s="183"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -24371,7 +24431,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="185"/>
+      <c r="A11" s="184"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -24542,7 +24602,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="183">
+      <c r="A12" s="182">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -24704,7 +24764,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="184"/>
+      <c r="A13" s="183"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -24864,7 +24924,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="184"/>
+      <c r="A14" s="183"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -25024,7 +25084,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="185"/>
+      <c r="A15" s="184"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -25195,7 +25255,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183">
+      <c r="A16" s="182">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -25357,7 +25417,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="184"/>
+      <c r="A17" s="183"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -25517,7 +25577,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="184"/>
+      <c r="A18" s="183"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -25677,7 +25737,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="185"/>
+      <c r="A19" s="184"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -25848,7 +25908,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183">
+      <c r="A20" s="182">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -26010,7 +26070,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="184"/>
+      <c r="A21" s="183"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -26170,7 +26230,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="184"/>
+      <c r="A22" s="183"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -26330,7 +26390,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="185"/>
+      <c r="A23" s="184"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -26501,7 +26561,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="183">
+      <c r="A24" s="182">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -26663,7 +26723,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="184"/>
+      <c r="A25" s="183"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -26823,7 +26883,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="184"/>
+      <c r="A26" s="183"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -26983,7 +27043,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="185"/>
+      <c r="A27" s="184"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -27154,7 +27214,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="183">
+      <c r="A28" s="182">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -27318,7 +27378,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="184"/>
+      <c r="A29" s="183"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -27476,7 +27536,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="184"/>
+      <c r="A30" s="183"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -27634,7 +27694,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="185"/>
+      <c r="A31" s="184"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -27805,7 +27865,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="183">
+      <c r="A32" s="182">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -27969,7 +28029,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="184"/>
+      <c r="A33" s="183"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -28129,7 +28189,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="184"/>
+      <c r="A34" s="183"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -28289,7 +28349,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="185"/>
+      <c r="A35" s="184"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -28460,7 +28520,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="183">
+      <c r="A36" s="182">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -28624,7 +28684,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="184"/>
+      <c r="A37" s="183"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -28784,7 +28844,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="184"/>
+      <c r="A38" s="183"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -28944,7 +29004,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="185"/>
+      <c r="A39" s="184"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -29115,7 +29175,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="183">
+      <c r="A40" s="182">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -29279,7 +29339,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="184"/>
+      <c r="A41" s="183"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -29435,7 +29495,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="184"/>
+      <c r="A42" s="183"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -29583,7 +29643,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="185"/>
+      <c r="A43" s="184"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -29754,7 +29814,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="183">
+      <c r="A44" s="182">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -29916,7 +29976,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="184"/>
+      <c r="A45" s="183"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -30076,7 +30136,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="184"/>
+      <c r="A46" s="183"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -30236,7 +30296,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="185"/>
+      <c r="A47" s="184"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -30407,7 +30467,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="183">
+      <c r="A48" s="182">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -30569,7 +30629,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="184"/>
+      <c r="A49" s="183"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -30729,7 +30789,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="184"/>
+      <c r="A50" s="183"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -30889,7 +30949,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="185"/>
+      <c r="A51" s="184"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -31694,7 +31754,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="183">
+      <c r="A56" s="182">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -31858,7 +31918,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="184"/>
+      <c r="A57" s="183"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -32018,7 +32078,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="184"/>
+      <c r="A58" s="183"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -32178,7 +32238,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="185"/>
+      <c r="A59" s="184"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -32349,7 +32409,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="183">
+      <c r="A60" s="182">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -32513,7 +32573,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="184"/>
+      <c r="A61" s="183"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -32673,7 +32733,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="184"/>
+      <c r="A62" s="183"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -32833,7 +32893,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="185"/>
+      <c r="A63" s="184"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -33004,7 +33064,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="183">
+      <c r="A64" s="182">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -33170,7 +33230,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="184"/>
+      <c r="A65" s="183"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -33330,7 +33390,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="184"/>
+      <c r="A66" s="183"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -33490,7 +33550,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="185"/>
+      <c r="A67" s="184"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -33661,7 +33721,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="183">
+      <c r="A68" s="182">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -33825,7 +33885,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="184"/>
+      <c r="A69" s="183"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -33985,7 +34045,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="184"/>
+      <c r="A70" s="183"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -34145,7 +34205,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="185"/>
+      <c r="A71" s="184"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -34316,7 +34376,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="183">
+      <c r="A72" s="182">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -34480,7 +34540,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="184"/>
+      <c r="A73" s="183"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -34640,7 +34700,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="184"/>
+      <c r="A74" s="183"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -34800,7 +34860,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="185"/>
+      <c r="A75" s="184"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -34971,7 +35031,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="183">
+      <c r="A76" s="182">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -35133,7 +35193,7 @@
       <c r="BA76" s="19"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="184"/>
+      <c r="A77" s="183"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -35293,7 +35353,7 @@
       <c r="BA77" s="44"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="184"/>
+      <c r="A78" s="183"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -35453,7 +35513,7 @@
       <c r="BA78" s="40"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="185"/>
+      <c r="A79" s="184"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -35624,7 +35684,7 @@
       <c r="BA79" s="57"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="183">
+      <c r="A80" s="182">
         <v>20</v>
       </c>
       <c r="B80" s="22">
@@ -35786,7 +35846,7 @@
       <c r="BA80" s="19"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="184"/>
+      <c r="A81" s="183"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -35946,7 +36006,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="184"/>
+      <c r="A82" s="183"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -36106,7 +36166,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="185"/>
+      <c r="A83" s="184"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -36277,7 +36337,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="183">
+      <c r="A84" s="182">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -36441,7 +36501,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="184"/>
+      <c r="A85" s="183"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -36601,7 +36661,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="184"/>
+      <c r="A86" s="183"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -36761,7 +36821,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="185"/>
+      <c r="A87" s="184"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -36932,7 +36992,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="183">
+      <c r="A88" s="182">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -37096,7 +37156,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="184"/>
+      <c r="A89" s="183"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -37256,7 +37316,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="184"/>
+      <c r="A90" s="183"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -37416,7 +37476,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="185"/>
+      <c r="A91" s="184"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -37587,7 +37647,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="183">
+      <c r="A92" s="182">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -37751,7 +37811,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="184"/>
+      <c r="A93" s="183"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -37909,7 +37969,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="184"/>
+      <c r="A94" s="183"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -38063,7 +38123,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="185"/>
+      <c r="A95" s="184"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -38234,7 +38294,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="183">
+      <c r="A96" s="182">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -38398,7 +38458,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="184"/>
+      <c r="A97" s="183"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -38558,7 +38618,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="184"/>
+      <c r="A98" s="183"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -38718,7 +38778,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="185"/>
+      <c r="A99" s="184"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -38889,7 +38949,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="186">
+      <c r="A100" s="192">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -39053,7 +39113,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="186"/>
+      <c r="A101" s="192"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -39213,7 +39273,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="186"/>
+      <c r="A102" s="192"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -39373,7 +39433,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="186"/>
+      <c r="A103" s="192"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -39544,7 +39604,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="183">
+      <c r="A104" s="182">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -39706,7 +39766,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="184"/>
+      <c r="A105" s="183"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -39866,7 +39926,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="184"/>
+      <c r="A106" s="183"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -40026,7 +40086,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="185"/>
+      <c r="A107" s="184"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -40197,7 +40257,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="183">
+      <c r="A108" s="182">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -40359,7 +40419,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="184"/>
+      <c r="A109" s="183"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -40515,7 +40575,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="184"/>
+      <c r="A110" s="183"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -40665,7 +40725,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="185"/>
+      <c r="A111" s="184"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -40836,7 +40896,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="183">
+      <c r="A112" s="182">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -41000,7 +41060,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="184"/>
+      <c r="A113" s="183"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -41160,7 +41220,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="184"/>
+      <c r="A114" s="183"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -41320,7 +41380,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="185"/>
+      <c r="A115" s="184"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -41491,7 +41551,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="184">
+      <c r="A116" s="183">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -41655,7 +41715,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="184"/>
+      <c r="A117" s="183"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -41815,7 +41875,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="184"/>
+      <c r="A118" s="183"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -41975,7 +42035,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="185"/>
+      <c r="A119" s="184"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -42146,7 +42206,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="183">
+      <c r="A120" s="182">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -42310,7 +42370,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="184"/>
+      <c r="A121" s="183"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -42470,7 +42530,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="184"/>
+      <c r="A122" s="183"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -42630,7 +42690,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="185"/>
+      <c r="A123" s="184"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -42801,7 +42861,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="183">
+      <c r="A124" s="182">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -42965,7 +43025,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="184"/>
+      <c r="A125" s="183"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -43121,7 +43181,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="184"/>
+      <c r="A126" s="183"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -43271,7 +43331,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="185"/>
+      <c r="A127" s="184"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -43707,12 +43767,18 @@
     <protectedRange sqref="AB112:AB127" name="Range1_1_1_1_1_2_2_1_1_4"/>
   </protectedRanges>
   <mergeCells count="35">
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A56:A59"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A35"/>
@@ -43726,25 +43792,2348 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
     <mergeCell ref="A96:A99"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="A104:A107"/>
     <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="A84:A87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6555BB66-49A2-4157-88D4-D9BD7AEDD16F}">
+  <dimension ref="A1:BA15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="189" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="187" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="185" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="125" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="125" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="125" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="120" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="125" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="125" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="125"/>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="127" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" s="125" t="s">
+        <v>68</v>
+      </c>
+      <c r="V1" s="125"/>
+      <c r="W1" s="125" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="125"/>
+      <c r="AA1" s="149" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="127" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="125" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="125" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE1" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF1" s="125" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG1" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="111" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="125" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK1" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL1" s="125" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO1" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP1" s="125" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ1" s="127" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR1" s="125" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS1" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT1" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU1" s="92" t="s">
+        <v>37</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW1" s="125" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX1" s="191" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY1" s="191"/>
+      <c r="AZ1" s="191" t="s">
+        <v>26</v>
+      </c>
+      <c r="BA1" s="191"/>
+    </row>
+    <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="190"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="150" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH2" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AQ2" s="128"/>
+      <c r="AR2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS2" s="93" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT2" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU2" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="83"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="141"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="151"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="89"/>
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="113"/>
+      <c r="AI3" s="115"/>
+      <c r="AJ3" s="89"/>
+      <c r="AK3" s="89"/>
+      <c r="AL3" s="85"/>
+      <c r="AM3" s="86"/>
+      <c r="AN3" s="87"/>
+      <c r="AO3" s="87"/>
+      <c r="AP3" s="85"/>
+      <c r="AQ3" s="129"/>
+      <c r="AR3" s="85"/>
+      <c r="AS3" s="96"/>
+      <c r="AT3" s="119">
+        <f>[1]Юли!AU127</f>
+        <v>1478.34</v>
+      </c>
+      <c r="AU3" s="97"/>
+      <c r="AV3" s="88"/>
+      <c r="AW3" s="85"/>
+      <c r="AX3" s="85"/>
+      <c r="AY3" s="85"/>
+      <c r="AZ3" s="85"/>
+      <c r="BA3" s="85"/>
+    </row>
+    <row r="4" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="182">
+        <v>1</v>
+      </c>
+      <c r="B4" s="22">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="11">
+        <v>6500</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>11055</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="H4" s="12">
+        <v>7.9</v>
+      </c>
+      <c r="I4" s="11">
+        <v>10680</v>
+      </c>
+      <c r="J4" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="K4" s="11">
+        <v>16319</v>
+      </c>
+      <c r="L4" s="13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="M4" s="23">
+        <f>ROUND(K4*(1-L4),0)</f>
+        <v>15421</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="O4" s="24">
+        <f t="shared" ref="O4:O6" si="0">M4*N4</f>
+        <v>10887.225999999999</v>
+      </c>
+      <c r="P4" s="13">
+        <v>0.253</v>
+      </c>
+      <c r="Q4" s="24">
+        <f t="shared" ref="Q4:Q6" si="1">M4*P4</f>
+        <v>3901.5129999999999</v>
+      </c>
+      <c r="R4" s="15">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="S4" s="142">
+        <v>0.2097</v>
+      </c>
+      <c r="T4" s="24">
+        <f t="shared" ref="T4:T6" si="2">M4*R4</f>
+        <v>632.26100000000008</v>
+      </c>
+      <c r="U4" s="25">
+        <v>0.23</v>
+      </c>
+      <c r="V4" s="24">
+        <f t="shared" ref="V4:V6" si="3">M4*U4</f>
+        <v>3546.83</v>
+      </c>
+      <c r="W4" s="15">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="X4" s="24">
+        <f>M4*W4</f>
+        <v>7525.4479999999994</v>
+      </c>
+      <c r="Y4" s="15">
+        <v>0.43</v>
+      </c>
+      <c r="Z4" s="124">
+        <f t="shared" ref="Z4:Z6" si="4">Y4*M4</f>
+        <v>6631.03</v>
+      </c>
+      <c r="AA4" s="145">
+        <v>2.7100000000000002E-3</v>
+      </c>
+      <c r="AB4" s="18">
+        <f>M4*AA4</f>
+        <v>41.790910000000004</v>
+      </c>
+      <c r="AC4" s="16">
+        <v>2.6900000000000001E-3</v>
+      </c>
+      <c r="AD4" s="18">
+        <f>M4*AC4</f>
+        <v>41.482489999999999</v>
+      </c>
+      <c r="AE4" s="26">
+        <f>IF(M4&gt;0,(AG4+AP4)/M4,0)</f>
+        <v>2.7350149795733088E-3</v>
+      </c>
+      <c r="AF4" s="16">
+        <v>2.9E-4</v>
+      </c>
+      <c r="AG4" s="23">
+        <f t="shared" ref="AG4:AG6" si="5">AF4*M4</f>
+        <v>4.4720899999999997</v>
+      </c>
+      <c r="AH4" s="114">
+        <v>0.21149999999999999</v>
+      </c>
+      <c r="AI4" s="29">
+        <f>AL4*(1-AM4)*AH4</f>
+        <v>36.953279999999999</v>
+      </c>
+      <c r="AJ4" s="27">
+        <f>IF(AND(AH4&gt;0,AF4&gt;0,AC4&gt;0),((AC4-AF4)*AH4)/((AH4-AF4)*AC4),0)</f>
+        <v>0.89341832658664044</v>
+      </c>
+      <c r="AK4" s="59">
+        <f t="shared" ref="AK4:AK15" si="6">IF(AND(AE4&gt;0,AN4&gt;0,AF4&gt;0),((AN4*(AE4-AF4))/(AE4*(AN4-AF4))),0)</f>
+        <v>0.89517063729570767</v>
+      </c>
+      <c r="AL4" s="11">
+        <v>192</v>
+      </c>
+      <c r="AM4" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="AN4" s="14">
+        <v>0.21579999999999999</v>
+      </c>
+      <c r="AO4" s="130">
+        <v>0.21190000000000001</v>
+      </c>
+      <c r="AP4" s="29">
+        <f>AL4*(1-AM4)*AN4</f>
+        <v>37.704575999999996</v>
+      </c>
+      <c r="AQ4" s="131">
+        <f>AL4*(1-AM4)*AO4</f>
+        <v>37.023167999999998</v>
+      </c>
+      <c r="AR4" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="AS4" s="18">
+        <v>502.42</v>
+      </c>
+      <c r="AT4" s="110">
+        <f>AT3+AL4-AS4</f>
+        <v>1167.9199999999998</v>
+      </c>
+      <c r="AU4" s="99"/>
+      <c r="AV4" s="11"/>
+      <c r="AW4" s="30"/>
+      <c r="AX4" s="19"/>
+      <c r="AY4" s="19"/>
+      <c r="AZ4" s="19"/>
+      <c r="BA4" s="19"/>
+    </row>
+    <row r="5" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="183"/>
+      <c r="B5" s="32">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="33">
+        <v>19500</v>
+      </c>
+      <c r="E5" s="33">
+        <v>3</v>
+      </c>
+      <c r="F5" s="33">
+        <v>18972</v>
+      </c>
+      <c r="G5" s="34">
+        <v>1</v>
+      </c>
+      <c r="H5" s="34">
+        <v>8.1</v>
+      </c>
+      <c r="I5" s="33">
+        <v>18386</v>
+      </c>
+      <c r="J5" s="34">
+        <v>4.5</v>
+      </c>
+      <c r="K5" s="33">
+        <v>15725</v>
+      </c>
+      <c r="L5" s="35">
+        <v>0.06</v>
+      </c>
+      <c r="M5" s="36">
+        <f>ROUND(K5*(1-L5),0)</f>
+        <v>14782</v>
+      </c>
+      <c r="N5" s="37">
+        <v>0.71</v>
+      </c>
+      <c r="O5" s="24">
+        <f t="shared" si="0"/>
+        <v>10495.22</v>
+      </c>
+      <c r="P5" s="35">
+        <v>0.248</v>
+      </c>
+      <c r="Q5" s="24">
+        <f t="shared" si="1"/>
+        <v>3665.9360000000001</v>
+      </c>
+      <c r="R5" s="38">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="S5" s="134">
+        <v>0.18840000000000001</v>
+      </c>
+      <c r="T5" s="24">
+        <f t="shared" si="2"/>
+        <v>620.84400000000005</v>
+      </c>
+      <c r="U5" s="27">
+        <v>0.22</v>
+      </c>
+      <c r="V5" s="24">
+        <f t="shared" si="3"/>
+        <v>3252.04</v>
+      </c>
+      <c r="W5" s="38">
+        <v>0.46</v>
+      </c>
+      <c r="X5" s="24">
+        <f>M5*W5</f>
+        <v>6799.72</v>
+      </c>
+      <c r="Y5" s="38">
+        <v>0.42</v>
+      </c>
+      <c r="Z5" s="24">
+        <f t="shared" si="4"/>
+        <v>6208.44</v>
+      </c>
+      <c r="AA5" s="146">
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="AB5" s="18">
+        <f t="shared" ref="AB5:AB6" si="7">M5*AA5</f>
+        <v>37.102820000000001</v>
+      </c>
+      <c r="AC5" s="39">
+        <v>2.5899999999999999E-3</v>
+      </c>
+      <c r="AD5" s="17">
+        <f>M5*AC5</f>
+        <v>38.285379999999996</v>
+      </c>
+      <c r="AE5" s="26">
+        <f>IF(M5&gt;0,(AG5+AP5)/M5,0)</f>
+        <v>2.6494704370179953E-3</v>
+      </c>
+      <c r="AF5" s="39">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG5" s="36">
+        <f t="shared" si="5"/>
+        <v>3.9911400000000001</v>
+      </c>
+      <c r="AH5" s="27">
+        <v>0.22620000000000001</v>
+      </c>
+      <c r="AI5" s="40">
+        <f>AL5*(1-AM5)*AH5</f>
+        <v>35.392383000000002</v>
+      </c>
+      <c r="AJ5" s="27">
+        <f>IF(AND(AH5&gt;0,AF5&gt;0,AC5&gt;0),((AC5-AF5)*AH5)/((AH5-AF5)*AC5),0)</f>
+        <v>0.89682337458197237</v>
+      </c>
+      <c r="AK5" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89917281026480267</v>
+      </c>
+      <c r="AL5" s="33">
+        <v>171</v>
+      </c>
+      <c r="AM5" s="35">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN5" s="37">
+        <v>0.2248</v>
+      </c>
+      <c r="AO5" s="132">
+        <v>0.21759999999999999</v>
+      </c>
+      <c r="AP5" s="40">
+        <f>AL5*(1-AM5)*AN5</f>
+        <v>35.173332000000002</v>
+      </c>
+      <c r="AQ5" s="133">
+        <f t="shared" ref="AQ5:AQ6" si="8">AL5*(1-AM5)*AO5</f>
+        <v>34.046784000000002</v>
+      </c>
+      <c r="AR5" s="41">
+        <v>1.6</v>
+      </c>
+      <c r="AS5" s="41"/>
+      <c r="AT5" s="110">
+        <f>AT4+AL5-AS5</f>
+        <v>1338.9199999999998</v>
+      </c>
+      <c r="AU5" s="100"/>
+      <c r="AV5" s="42"/>
+      <c r="AW5" s="43"/>
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="44"/>
+      <c r="AZ5" s="44"/>
+      <c r="BA5" s="44"/>
+    </row>
+    <row r="6" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="183"/>
+      <c r="B6" s="32">
+        <v>3</v>
+      </c>
+      <c r="C6" s="180" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="42">
+        <v>17100</v>
+      </c>
+      <c r="E6" s="42">
+        <v>3</v>
+      </c>
+      <c r="F6" s="42">
+        <v>17836</v>
+      </c>
+      <c r="G6" s="36">
+        <v>0.7</v>
+      </c>
+      <c r="H6" s="36">
+        <v>6.5</v>
+      </c>
+      <c r="I6" s="42">
+        <v>16955</v>
+      </c>
+      <c r="J6" s="36">
+        <v>3.8</v>
+      </c>
+      <c r="K6" s="42">
+        <v>15464</v>
+      </c>
+      <c r="L6" s="38">
+        <v>0.06</v>
+      </c>
+      <c r="M6" s="36">
+        <f>ROUND(K6*(1-L6),0)</f>
+        <v>14536</v>
+      </c>
+      <c r="N6" s="27">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="O6" s="24">
+        <f t="shared" si="0"/>
+        <v>10422.312</v>
+      </c>
+      <c r="P6" s="38">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="Q6" s="24">
+        <f t="shared" si="1"/>
+        <v>3415.9599999999996</v>
+      </c>
+      <c r="R6" s="38">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="S6" s="134">
+        <v>0.1711</v>
+      </c>
+      <c r="T6" s="24">
+        <f t="shared" si="2"/>
+        <v>697.72800000000007</v>
+      </c>
+      <c r="U6" s="27">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="V6" s="24">
+        <f t="shared" si="3"/>
+        <v>2849.056</v>
+      </c>
+      <c r="W6" s="38">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="X6" s="24">
+        <f>M6*W6</f>
+        <v>7544.1840000000002</v>
+      </c>
+      <c r="Y6" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z6" s="24">
+        <f t="shared" si="4"/>
+        <v>5959.7599999999993</v>
+      </c>
+      <c r="AA6" s="147">
+        <v>2.4099999999999998E-3</v>
+      </c>
+      <c r="AB6" s="148">
+        <f t="shared" si="7"/>
+        <v>35.031759999999998</v>
+      </c>
+      <c r="AC6" s="46">
+        <v>2.49E-3</v>
+      </c>
+      <c r="AD6" s="17">
+        <f>M6*AC6</f>
+        <v>36.19464</v>
+      </c>
+      <c r="AE6" s="26">
+        <f>IF(M6&gt;0,(AG6+AP6)/M6,0)</f>
+        <v>2.907700880572372E-3</v>
+      </c>
+      <c r="AF6" s="46">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG6" s="36">
+        <f t="shared" si="5"/>
+        <v>3.9247200000000002</v>
+      </c>
+      <c r="AH6" s="27">
+        <v>0.21279999999999999</v>
+      </c>
+      <c r="AI6" s="40">
+        <f>AL6*(1-AM6)*AH6</f>
+        <v>35.785511999999997</v>
+      </c>
+      <c r="AJ6" s="27">
+        <f>IF(AND(AH6&gt;0,AF6&gt;0,AC6&gt;0),((AC6-AF6)*AH6)/((AH6-AF6)*AC6),0)</f>
+        <v>0.89269891876355945</v>
+      </c>
+      <c r="AK6" s="28">
+        <f t="shared" si="6"/>
+        <v>0.90821865300602855</v>
+      </c>
+      <c r="AL6" s="42">
+        <v>185</v>
+      </c>
+      <c r="AM6" s="38">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AN6" s="27">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="AO6" s="134">
+        <v>0.22189999999999999</v>
+      </c>
+      <c r="AP6" s="40">
+        <f>AL6*(1-AM6)*AN6</f>
+        <v>38.341619999999999</v>
+      </c>
+      <c r="AQ6" s="135">
+        <f t="shared" si="8"/>
+        <v>37.315813499999997</v>
+      </c>
+      <c r="AR6" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS6" s="17"/>
+      <c r="AT6" s="110">
+        <f>AT5+AL6-AS6</f>
+        <v>1523.9199999999998</v>
+      </c>
+      <c r="AU6" s="101"/>
+      <c r="AV6" s="42"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="40"/>
+      <c r="AY6" s="40"/>
+      <c r="AZ6" s="40"/>
+      <c r="BA6" s="40"/>
+    </row>
+    <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="184"/>
+      <c r="B7" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50">
+        <f>SUM(D4:D6)</f>
+        <v>43100</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50">
+        <f>SUM(F4:F6)</f>
+        <v>47863</v>
+      </c>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="50">
+        <f>SUM(I4:I6)</f>
+        <v>46021</v>
+      </c>
+      <c r="J7" s="51"/>
+      <c r="K7" s="50">
+        <f>SUM(K4:K6)</f>
+        <v>47508</v>
+      </c>
+      <c r="L7" s="20">
+        <f>IF(K7&gt;0,(K4*L4+K5*L5+K6*L6)/K7,0)</f>
+        <v>5.828249978950914E-2</v>
+      </c>
+      <c r="M7" s="51">
+        <f>M4+M5+M6</f>
+        <v>44739</v>
+      </c>
+      <c r="N7" s="52">
+        <f>IF(M7&gt;0,O7/M7,0)</f>
+        <v>0.71089559444779715</v>
+      </c>
+      <c r="O7" s="53">
+        <f>O4+O5+O6</f>
+        <v>31804.757999999994</v>
+      </c>
+      <c r="P7" s="20">
+        <f>IF(M7&gt;0,Q7/M7,0)</f>
+        <v>0.24549965354612305</v>
+      </c>
+      <c r="Q7" s="53">
+        <f>Q4+Q5+Q6</f>
+        <v>10983.409</v>
+      </c>
+      <c r="R7" s="20">
+        <f>IF(M7&gt;0,T7/M7,0)</f>
+        <v>4.360475200607971E-2</v>
+      </c>
+      <c r="S7" s="136"/>
+      <c r="T7" s="53">
+        <f>T4+T5+T6</f>
+        <v>1950.8330000000001</v>
+      </c>
+      <c r="U7" s="20">
+        <f>IF(M7&gt;0,V7/M7,0)</f>
+        <v>0.21564912045418985</v>
+      </c>
+      <c r="V7" s="53">
+        <f>V4+V5+V6</f>
+        <v>9647.9259999999995</v>
+      </c>
+      <c r="W7" s="20">
+        <f>IF(M7&gt;0,X7/M7,0)</f>
+        <v>0.4888207604103802</v>
+      </c>
+      <c r="X7" s="53">
+        <f>X4+X5+X6</f>
+        <v>21869.351999999999</v>
+      </c>
+      <c r="Y7" s="20">
+        <f>IF(M7&gt;0,Z7/M7,0)</f>
+        <v>0.42019781398779588</v>
+      </c>
+      <c r="Z7" s="53">
+        <f>Z4+Z5+Z6</f>
+        <v>18799.23</v>
+      </c>
+      <c r="AA7" s="152">
+        <f>IF(M7&gt;0,AB7/M7,0)</f>
+        <v>2.5464469478531037E-3</v>
+      </c>
+      <c r="AB7" s="55">
+        <f t="shared" ref="AB7" si="9">SUM(AB4:AB6)</f>
+        <v>113.92549</v>
+      </c>
+      <c r="AC7" s="54">
+        <f>IF(M7&gt;0,AD7/M7,0)</f>
+        <v>2.5919781398779586E-3</v>
+      </c>
+      <c r="AD7" s="55">
+        <f>SUM(AD4:AD6)</f>
+        <v>115.96250999999998</v>
+      </c>
+      <c r="AE7" s="54">
+        <f>IF(M7&gt;0,(AE4*M4+AE5*M5+AE6*M6)/M7,0)</f>
+        <v>2.7628574174657456E-3</v>
+      </c>
+      <c r="AF7" s="54">
+        <f>IF(K7&gt;0,(K4*AF4+K5*AF5+K6*AF6)/K7,0)</f>
+        <v>2.7687000084196346E-4</v>
+      </c>
+      <c r="AG7" s="51">
+        <f>SUM(AG4:AG6)</f>
+        <v>12.38795</v>
+      </c>
+      <c r="AH7" s="52">
+        <f>IF(K7&gt;0,(K4*AH4+K5*AH5+K6*AH6)/K7,0)</f>
+        <v>0.21678880820072408</v>
+      </c>
+      <c r="AI7" s="57">
+        <f>SUM(AI4:AI6)</f>
+        <v>108.131175</v>
+      </c>
+      <c r="AJ7" s="52">
+        <f>IF(AND(AD7&gt;0),((AD4*AJ4+AD5*AJ5+AD6*AJ6)/AD7),0)</f>
+        <v>0.89431796949062681</v>
+      </c>
+      <c r="AK7" s="56">
+        <f t="shared" si="6"/>
+        <v>0.90090832599054893</v>
+      </c>
+      <c r="AL7" s="50">
+        <f>SUM(AL4:AL6)</f>
+        <v>548</v>
+      </c>
+      <c r="AM7" s="20">
+        <f>IF(AL7&gt;0,(AM4*AL4+AM5*AL5+AM6*AL6)/AL7,0)</f>
+        <v>8.8777372262773727E-2</v>
+      </c>
+      <c r="AN7" s="52">
+        <f>IF(K7&gt;0,(AN4*K4+AN5*K5+AN6*K6)/K7,0)</f>
+        <v>0.22275010945524962</v>
+      </c>
+      <c r="AO7" s="136">
+        <f>IF(K7&gt;0,(AO4*K4+AO5*K5+AO6*K6)/K7,0)</f>
+        <v>0.21704171297465691</v>
+      </c>
+      <c r="AP7" s="57">
+        <f>SUM(AP4:AP6)</f>
+        <v>111.219528</v>
+      </c>
+      <c r="AQ7" s="137">
+        <f t="shared" ref="AQ7" si="10">SUM(AQ4:AQ6)</f>
+        <v>108.38576549999999</v>
+      </c>
+      <c r="AR7" s="55"/>
+      <c r="AS7" s="55">
+        <f>SUM(AS4:AS6)</f>
+        <v>502.42</v>
+      </c>
+      <c r="AT7" s="102"/>
+      <c r="AU7" s="103">
+        <f>AT6</f>
+        <v>1523.9199999999998</v>
+      </c>
+      <c r="AV7" s="50">
+        <f>SUM(AV4:AV6)</f>
+        <v>0</v>
+      </c>
+      <c r="AW7" s="58"/>
+      <c r="AX7" s="57"/>
+      <c r="AY7" s="57"/>
+      <c r="AZ7" s="57"/>
+      <c r="BA7" s="57"/>
+    </row>
+    <row r="8" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="182">
+        <v>2</v>
+      </c>
+      <c r="B8" s="22">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="11">
+        <v>17000</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>18048</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="H8" s="12">
+        <v>6.3</v>
+      </c>
+      <c r="I8" s="11">
+        <v>17595</v>
+      </c>
+      <c r="J8" s="12">
+        <v>2.9</v>
+      </c>
+      <c r="K8" s="11">
+        <v>15448</v>
+      </c>
+      <c r="L8" s="13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M8" s="23">
+        <f>ROUND(K8*(1-L8),0)</f>
+        <v>14614</v>
+      </c>
+      <c r="N8" s="14">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="O8" s="24">
+        <f t="shared" ref="O8:O10" si="11">M8*N8</f>
+        <v>10010.59</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q8" s="24">
+        <f t="shared" ref="Q8:Q10" si="12">M8*P8</f>
+        <v>4091.9200000000005</v>
+      </c>
+      <c r="R8" s="15">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="S8" s="143">
+        <v>0.1749</v>
+      </c>
+      <c r="T8" s="24">
+        <f t="shared" ref="T8:T10" si="13">M8*R8</f>
+        <v>511.49000000000007</v>
+      </c>
+      <c r="U8" s="25">
+        <v>0.191</v>
+      </c>
+      <c r="V8" s="24">
+        <f t="shared" ref="V8:V10" si="14">M8*U8</f>
+        <v>2791.2739999999999</v>
+      </c>
+      <c r="W8" s="15">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="X8" s="24">
+        <f t="shared" ref="X8:X10" si="15">M8*W8</f>
+        <v>7482.3680000000004</v>
+      </c>
+      <c r="Y8" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="Z8" s="24">
+        <f t="shared" ref="Z8:Z10" si="16">Y8*M8</f>
+        <v>5845.6</v>
+      </c>
+      <c r="AA8" s="145">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="AB8" s="18">
+        <f>M8*AA8</f>
+        <v>36.973420000000004</v>
+      </c>
+      <c r="AC8" s="16">
+        <v>2.4099999999999998E-3</v>
+      </c>
+      <c r="AD8" s="17">
+        <f t="shared" ref="AD8:AD10" si="17">M8*AC8</f>
+        <v>35.219739999999994</v>
+      </c>
+      <c r="AE8" s="26">
+        <f>IF(M8&gt;0,(AG8+AP8)/M8,0)</f>
+        <v>2.4521158341316547E-3</v>
+      </c>
+      <c r="AF8" s="16">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG8" s="23">
+        <f t="shared" ref="AG8:AG10" si="18">AF8*M8</f>
+        <v>3.9457800000000001</v>
+      </c>
+      <c r="AH8" s="114">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="AI8" s="29">
+        <f t="shared" ref="AI8:AI10" si="19">AL8*(1-AM8)*AH8</f>
+        <v>31.206837599999997</v>
+      </c>
+      <c r="AJ8" s="27">
+        <f t="shared" ref="AJ8:AJ10" si="20">IF(AND(AH8&gt;0,AF8&gt;0,AC8&gt;0),((AC8-AF8)*AH8)/((AH8-AF8)*AC8),0)</f>
+        <v>0.88910831351300734</v>
+      </c>
+      <c r="AK8" s="59">
+        <f t="shared" si="6"/>
+        <v>0.89101047319287685</v>
+      </c>
+      <c r="AL8" s="11">
+        <v>162</v>
+      </c>
+      <c r="AM8" s="13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AN8" s="14">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="AO8" s="130">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="AP8" s="29">
+        <f>AL8*(1-AM8)*AN8</f>
+        <v>31.889440799999999</v>
+      </c>
+      <c r="AQ8" s="131">
+        <f t="shared" ref="AQ8:AQ15" si="21">AL8*(1-AM8)*AO8</f>
+        <v>31.5184608</v>
+      </c>
+      <c r="AR8" s="18">
+        <v>1.55</v>
+      </c>
+      <c r="AS8" s="18"/>
+      <c r="AT8" s="98">
+        <f>AT6+AL8-AS8</f>
+        <v>1685.9199999999998</v>
+      </c>
+      <c r="AU8" s="99"/>
+      <c r="AV8" s="11"/>
+      <c r="AW8" s="30"/>
+      <c r="AX8" s="19"/>
+      <c r="AY8" s="19"/>
+      <c r="AZ8" s="19"/>
+      <c r="BA8" s="19"/>
+    </row>
+    <row r="9" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="183"/>
+      <c r="B9" s="32">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="33">
+        <v>19410</v>
+      </c>
+      <c r="E9" s="33">
+        <v>3</v>
+      </c>
+      <c r="F9" s="33">
+        <v>19184</v>
+      </c>
+      <c r="G9" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="H9" s="34">
+        <v>5.7</v>
+      </c>
+      <c r="I9" s="33">
+        <v>18743</v>
+      </c>
+      <c r="J9" s="34">
+        <v>2</v>
+      </c>
+      <c r="K9" s="33">
+        <v>15583</v>
+      </c>
+      <c r="L9" s="35">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="M9" s="36">
+        <f>ROUND(K9*(1-L9),0)</f>
+        <v>14679</v>
+      </c>
+      <c r="N9" s="37">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="O9" s="24">
+        <f t="shared" si="11"/>
+        <v>9761.5349999999999</v>
+      </c>
+      <c r="P9" s="35">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q9" s="24">
+        <f t="shared" si="12"/>
+        <v>4110.1200000000008</v>
+      </c>
+      <c r="R9" s="38">
+        <v>5.5E-2</v>
+      </c>
+      <c r="S9" s="134">
+        <v>0.1825</v>
+      </c>
+      <c r="T9" s="24">
+        <f t="shared" si="13"/>
+        <v>807.34500000000003</v>
+      </c>
+      <c r="U9" s="27">
+        <v>0.189</v>
+      </c>
+      <c r="V9" s="24">
+        <f t="shared" si="14"/>
+        <v>2774.3310000000001</v>
+      </c>
+      <c r="W9" s="38">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="X9" s="24">
+        <f t="shared" si="15"/>
+        <v>7677.1170000000002</v>
+      </c>
+      <c r="Y9" s="38">
+        <v>0.39</v>
+      </c>
+      <c r="Z9" s="24">
+        <f t="shared" si="16"/>
+        <v>5724.81</v>
+      </c>
+      <c r="AA9" s="146">
+        <v>2.4299999999999999E-3</v>
+      </c>
+      <c r="AB9" s="18">
+        <f t="shared" ref="AB9:AB10" si="22">M9*AA9</f>
+        <v>35.669969999999999</v>
+      </c>
+      <c r="AC9" s="39">
+        <v>2.4299999999999999E-3</v>
+      </c>
+      <c r="AD9" s="17">
+        <f t="shared" si="17"/>
+        <v>35.669969999999999</v>
+      </c>
+      <c r="AE9" s="26">
+        <f>IF(M9&gt;0,(AG9+AP9)/M9,0)</f>
+        <v>2.6671968935213569E-3</v>
+      </c>
+      <c r="AF9" s="39">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="AG9" s="36">
+        <f t="shared" si="18"/>
+        <v>4.1101199999999993</v>
+      </c>
+      <c r="AH9" s="27">
+        <v>0.2172</v>
+      </c>
+      <c r="AI9" s="40">
+        <f t="shared" si="19"/>
+        <v>34.145577600000003</v>
+      </c>
+      <c r="AJ9" s="27">
+        <f t="shared" si="20"/>
+        <v>0.88591572702458443</v>
+      </c>
+      <c r="AK9" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89614658480947706</v>
+      </c>
+      <c r="AL9" s="33">
+        <v>172</v>
+      </c>
+      <c r="AM9" s="35">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AN9" s="37">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="AO9" s="132">
+        <v>0.2203</v>
+      </c>
+      <c r="AP9" s="40">
+        <f>AL9*(1-AM9)*AN9</f>
+        <v>35.041663199999995</v>
+      </c>
+      <c r="AQ9" s="133">
+        <f t="shared" si="21"/>
+        <v>34.632922399999998</v>
+      </c>
+      <c r="AR9" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="AS9" s="41"/>
+      <c r="AT9" s="110">
+        <f>AT8+AL9-AS9</f>
+        <v>1857.9199999999998</v>
+      </c>
+      <c r="AU9" s="101"/>
+      <c r="AV9" s="42"/>
+      <c r="AW9" s="43"/>
+      <c r="AX9" s="44"/>
+      <c r="AY9" s="44"/>
+      <c r="AZ9" s="44"/>
+      <c r="BA9" s="44"/>
+    </row>
+    <row r="10" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="183"/>
+      <c r="B10" s="32">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="42">
+        <v>18356</v>
+      </c>
+      <c r="E10" s="42">
+        <v>1</v>
+      </c>
+      <c r="F10" s="42">
+        <v>16869</v>
+      </c>
+      <c r="G10" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="36">
+        <v>6.4</v>
+      </c>
+      <c r="I10" s="42">
+        <v>16105</v>
+      </c>
+      <c r="J10" s="36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K10" s="42">
+        <v>15699</v>
+      </c>
+      <c r="L10" s="38">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="M10" s="36">
+        <f>ROUND(K10*(1-L10),0)</f>
+        <v>14804</v>
+      </c>
+      <c r="N10" s="27">
+        <v>0.629</v>
+      </c>
+      <c r="O10" s="24">
+        <f t="shared" si="11"/>
+        <v>9311.7160000000003</v>
+      </c>
+      <c r="P10" s="38">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="Q10" s="24">
+        <f t="shared" si="12"/>
+        <v>4041.4920000000002</v>
+      </c>
+      <c r="R10" s="38">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="S10" s="134">
+        <v>0.17760000000000001</v>
+      </c>
+      <c r="T10" s="24">
+        <f t="shared" si="13"/>
+        <v>1450.7920000000001</v>
+      </c>
+      <c r="U10" s="27">
+        <v>0.185</v>
+      </c>
+      <c r="V10" s="24">
+        <f t="shared" si="14"/>
+        <v>2738.74</v>
+      </c>
+      <c r="W10" s="38">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="X10" s="24">
+        <f t="shared" si="15"/>
+        <v>7683.2759999999998</v>
+      </c>
+      <c r="Y10" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="Z10" s="24">
+        <f t="shared" si="16"/>
+        <v>5921.6</v>
+      </c>
+      <c r="AA10" s="147">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="AB10" s="148">
+        <f t="shared" si="22"/>
+        <v>37.454120000000003</v>
+      </c>
+      <c r="AC10" s="46">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="AD10" s="17">
+        <f t="shared" si="17"/>
+        <v>36.121760000000002</v>
+      </c>
+      <c r="AE10" s="26">
+        <f>IF(M10&gt;0,(AG10+AP10)/M10,0)</f>
+        <v>2.6220147932991085E-3</v>
+      </c>
+      <c r="AF10" s="46">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG10" s="36">
+        <f t="shared" si="18"/>
+        <v>3.99708</v>
+      </c>
+      <c r="AH10" s="27">
+        <v>0.20780000000000001</v>
+      </c>
+      <c r="AI10" s="40">
+        <f t="shared" si="19"/>
+        <v>33.083838000000007</v>
+      </c>
+      <c r="AJ10" s="27">
+        <f t="shared" si="20"/>
+        <v>0.89050131405058564</v>
+      </c>
+      <c r="AK10" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89813456070407471</v>
+      </c>
+      <c r="AL10" s="42">
+        <v>174</v>
+      </c>
+      <c r="AM10" s="38">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN10" s="27">
+        <v>0.21870000000000001</v>
+      </c>
+      <c r="AO10" s="134">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="AP10" s="40">
+        <f>AL10*(1-AM10)*AN10</f>
+        <v>34.819227000000005</v>
+      </c>
+      <c r="AQ10" s="135">
+        <f t="shared" si="21"/>
+        <v>34.532649000000006</v>
+      </c>
+      <c r="AR10" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS10" s="17"/>
+      <c r="AT10" s="110">
+        <f>AT9+AL10-AS10</f>
+        <v>2031.9199999999998</v>
+      </c>
+      <c r="AU10" s="101"/>
+      <c r="AV10" s="42"/>
+      <c r="AW10" s="47"/>
+      <c r="AX10" s="40"/>
+      <c r="AY10" s="40"/>
+      <c r="AZ10" s="40"/>
+      <c r="BA10" s="40"/>
+    </row>
+    <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="184"/>
+      <c r="B11" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50">
+        <f t="shared" ref="D11" si="23">SUM(D8:D10)</f>
+        <v>54766</v>
+      </c>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50">
+        <f t="shared" ref="F11" si="24">SUM(F8:F10)</f>
+        <v>54101</v>
+      </c>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="50">
+        <f t="shared" ref="I11:K11" si="25">SUM(I8:I10)</f>
+        <v>52443</v>
+      </c>
+      <c r="J11" s="51"/>
+      <c r="K11" s="50">
+        <f t="shared" si="25"/>
+        <v>46730</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" ref="L11" si="26">IF(K11&gt;0,(K8*L8+K9*L9+K10*L10)/K11,0)</f>
+        <v>5.6341729081960203E-2</v>
+      </c>
+      <c r="M11" s="51">
+        <f t="shared" ref="M11" si="27">M8+M9+M10</f>
+        <v>44097</v>
+      </c>
+      <c r="N11" s="52">
+        <f t="shared" ref="N11" si="28">IF(M11&gt;0,O11/M11,0)</f>
+        <v>0.65954239517427493</v>
+      </c>
+      <c r="O11" s="53">
+        <f t="shared" ref="O11" si="29">O8+O9+O10</f>
+        <v>29083.841</v>
+      </c>
+      <c r="P11" s="20">
+        <f t="shared" ref="P11" si="30">IF(M11&gt;0,Q11/M11,0)</f>
+        <v>0.27764999886613606</v>
+      </c>
+      <c r="Q11" s="53">
+        <f t="shared" ref="Q11" si="31">Q8+Q9+Q10</f>
+        <v>12243.532000000001</v>
+      </c>
+      <c r="R11" s="20">
+        <f t="shared" ref="R11" si="32">IF(M11&gt;0,T11/M11,0)</f>
+        <v>6.2807605959589091E-2</v>
+      </c>
+      <c r="S11" s="136"/>
+      <c r="T11" s="53">
+        <f t="shared" ref="T11" si="33">T8+T9+T10</f>
+        <v>2769.6270000000004</v>
+      </c>
+      <c r="U11" s="20">
+        <f t="shared" ref="U11" si="34">IF(M11&gt;0,V11/M11,0)</f>
+        <v>0.18831995373834953</v>
+      </c>
+      <c r="V11" s="53">
+        <f t="shared" ref="V11" si="35">V8+V9+V10</f>
+        <v>8304.3449999999993</v>
+      </c>
+      <c r="W11" s="20">
+        <f t="shared" ref="W11" si="36">IF(M11&gt;0,X11/M11,0)</f>
+        <v>0.51801167879901122</v>
+      </c>
+      <c r="X11" s="53">
+        <f t="shared" ref="X11" si="37">X8+X9+X10</f>
+        <v>22842.760999999999</v>
+      </c>
+      <c r="Y11" s="20">
+        <f t="shared" ref="Y11" si="38">IF(M11&gt;0,Z11/M11,0)</f>
+        <v>0.39667120212259344</v>
+      </c>
+      <c r="Z11" s="53">
+        <f t="shared" ref="Z11" si="39">Z8+Z9+Z10</f>
+        <v>17492.010000000002</v>
+      </c>
+      <c r="AA11" s="152">
+        <f>IF(M11&gt;0,AB11/M11,0)</f>
+        <v>2.4967120212259341E-3</v>
+      </c>
+      <c r="AB11" s="55">
+        <f t="shared" ref="AB11" si="40">SUM(AB8:AB10)</f>
+        <v>110.09751000000001</v>
+      </c>
+      <c r="AC11" s="54">
+        <f t="shared" ref="AC11" si="41">IF(M11&gt;0,AD11/M11,0)</f>
+        <v>2.426729029185659E-3</v>
+      </c>
+      <c r="AD11" s="55">
+        <f t="shared" ref="AD11" si="42">SUM(AD8:AD10)</f>
+        <v>107.01147</v>
+      </c>
+      <c r="AE11" s="54">
+        <f t="shared" ref="AE11" si="43">IF(M11&gt;0,(AE8*M8+AE9*M9+AE10*M10)/M11,0)</f>
+        <v>2.5807495067691681E-3</v>
+      </c>
+      <c r="AF11" s="54">
+        <f t="shared" ref="AF11" si="44">IF(K11&gt;0,(K8*AF8+K9*AF9+K10*AF10)/K11,0)</f>
+        <v>2.7333468863684999E-4</v>
+      </c>
+      <c r="AG11" s="51">
+        <f t="shared" ref="AG11" si="45">SUM(AG8:AG10)</f>
+        <v>12.05298</v>
+      </c>
+      <c r="AH11" s="52">
+        <f t="shared" ref="AH11" si="46">IF(K11&gt;0,(K8*AH8+K9*AH9+K10*AH10)/K11,0)</f>
+        <v>0.21176105713674301</v>
+      </c>
+      <c r="AI11" s="57">
+        <f t="shared" ref="AI11" si="47">SUM(AI8:AI10)</f>
+        <v>98.43625320000001</v>
+      </c>
+      <c r="AJ11" s="52">
+        <f t="shared" ref="AJ11" si="48">IF(AND(AD11&gt;0),((AD8*AJ8+AD9*AJ9+AD10*AJ10)/AD11),0)</f>
+        <v>0.88851434136061858</v>
+      </c>
+      <c r="AK11" s="56">
+        <f t="shared" si="6"/>
+        <v>0.89520519403989141</v>
+      </c>
+      <c r="AL11" s="50">
+        <f t="shared" ref="AL11" si="49">SUM(AL8:AL10)</f>
+        <v>508</v>
+      </c>
+      <c r="AM11" s="20">
+        <f t="shared" ref="AM11" si="50">IF(AL11&gt;0,(AM8*AL8+AM9*AL9+AM10*AL10)/AL11,0)</f>
+        <v>8.5019685039370074E-2</v>
+      </c>
+      <c r="AN11" s="52">
+        <f>IF(K11&gt;0,(AN8*K8+AN9*K9+AN10*K10)/K11,0)</f>
+        <v>0.21884436550395892</v>
+      </c>
+      <c r="AO11" s="136">
+        <f>IF(K11&gt;0,(AO8*K8+AO9*K9+AO10*K10)/K11,0)</f>
+        <v>0.2165461844639418</v>
+      </c>
+      <c r="AP11" s="57">
+        <f t="shared" ref="AP11" si="51">SUM(AP8:AP10)</f>
+        <v>101.75033099999999</v>
+      </c>
+      <c r="AQ11" s="137">
+        <f t="shared" ref="AQ11:AQ15" si="52">SUM(AQ8:AQ10)</f>
+        <v>100.6840322</v>
+      </c>
+      <c r="AR11" s="55"/>
+      <c r="AS11" s="55">
+        <f t="shared" ref="AS11" si="53">SUM(AS8:AS10)</f>
+        <v>0</v>
+      </c>
+      <c r="AT11" s="102"/>
+      <c r="AU11" s="103">
+        <f>AT10</f>
+        <v>2031.9199999999998</v>
+      </c>
+      <c r="AV11" s="50">
+        <f t="shared" ref="AV11" si="54">SUM(AV8:AV10)</f>
+        <v>0</v>
+      </c>
+      <c r="AW11" s="58"/>
+      <c r="AX11" s="57"/>
+      <c r="AY11" s="57"/>
+      <c r="AZ11" s="57"/>
+      <c r="BA11" s="57"/>
+    </row>
+    <row r="12" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="182">
+        <v>3</v>
+      </c>
+      <c r="B12" s="22">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="11">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>14206</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="H12" s="12">
+        <v>7.8</v>
+      </c>
+      <c r="I12" s="11">
+        <v>13586</v>
+      </c>
+      <c r="J12" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K12" s="11">
+        <v>15878</v>
+      </c>
+      <c r="L12" s="13">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M12" s="23">
+        <f>ROUND(K12*(1-L12),0)</f>
+        <v>14941</v>
+      </c>
+      <c r="N12" s="14">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="O12" s="24">
+        <f t="shared" ref="O12:O14" si="55">M12*N12</f>
+        <v>8591.0749999999989</v>
+      </c>
+      <c r="P12" s="13">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="Q12" s="24">
+        <f t="shared" ref="Q12:Q14" si="56">M12*P12</f>
+        <v>4049.0110000000004</v>
+      </c>
+      <c r="R12" s="15">
+        <v>0.154</v>
+      </c>
+      <c r="S12" s="143">
+        <v>0.1883</v>
+      </c>
+      <c r="T12" s="24">
+        <f t="shared" ref="T12:T14" si="57">M12*R12</f>
+        <v>2300.9139999999998</v>
+      </c>
+      <c r="U12" s="25">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="V12" s="24">
+        <f t="shared" ref="V12:V14" si="58">M12*U12</f>
+        <v>2973.259</v>
+      </c>
+      <c r="W12" s="15">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="X12" s="24">
+        <f t="shared" ref="X12:X14" si="59">M12*W12</f>
+        <v>7590.0280000000002</v>
+      </c>
+      <c r="Y12" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="Z12" s="24">
+        <f t="shared" ref="Z12:Z14" si="60">Y12*M12</f>
+        <v>5976.4000000000005</v>
+      </c>
+      <c r="AA12" s="145">
+        <v>2.47E-3</v>
+      </c>
+      <c r="AB12" s="18">
+        <f t="shared" ref="AB12:AB15" si="61">M12*AA12</f>
+        <v>36.904269999999997</v>
+      </c>
+      <c r="AC12" s="16">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="AD12" s="17">
+        <f t="shared" ref="AD12:AD14" si="62">M12*AC12</f>
+        <v>35.858399999999996</v>
+      </c>
+      <c r="AE12" s="26">
+        <f>IF(M12&gt;0,(AG12+AP12)/M12,0)</f>
+        <v>2.4513728398366909E-3</v>
+      </c>
+      <c r="AF12" s="16">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="AG12" s="23">
+        <f t="shared" ref="AG12:AG14" si="63">AF12*M12</f>
+        <v>3.8846599999999998</v>
+      </c>
+      <c r="AH12" s="114">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="AI12" s="29">
+        <f t="shared" ref="AI12:AI14" si="64">AL12*(1-AM12)*AH12</f>
+        <v>31.092352200000004</v>
+      </c>
+      <c r="AJ12" s="27">
+        <f t="shared" ref="AJ12:AJ14" si="65">IF(AND(AH12&gt;0,AF12&gt;0,AC12&gt;0),((AC12-AF12)*AH12)/((AH12-AF12)*AC12),0)</f>
+        <v>0.89277570480928703</v>
+      </c>
+      <c r="AK12" s="59">
+        <f t="shared" si="6"/>
+        <v>0.89499278177486474</v>
+      </c>
+      <c r="AL12" s="11">
+        <v>162</v>
+      </c>
+      <c r="AM12" s="13">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="AN12" s="14">
+        <v>0.22040000000000001</v>
+      </c>
+      <c r="AO12" s="130">
+        <v>0.2233</v>
+      </c>
+      <c r="AP12" s="29">
+        <f>AL12*(1-AM12)*AN12</f>
+        <v>32.7413016</v>
+      </c>
+      <c r="AQ12" s="131">
+        <f t="shared" ref="AQ12" si="66">AL12*(1-AM12)*AO12</f>
+        <v>33.172108199999997</v>
+      </c>
+      <c r="AR12" s="18">
+        <v>1.55</v>
+      </c>
+      <c r="AS12" s="18"/>
+      <c r="AT12" s="98">
+        <f>AT10+AL12-AS12</f>
+        <v>2193.92</v>
+      </c>
+      <c r="AU12" s="99"/>
+      <c r="AV12" s="11"/>
+      <c r="AW12" s="30"/>
+      <c r="AX12" s="19"/>
+      <c r="AY12" s="19"/>
+      <c r="AZ12" s="19"/>
+      <c r="BA12" s="19"/>
+    </row>
+    <row r="13" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="183"/>
+      <c r="B13" s="32">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="33">
+        <v>20300</v>
+      </c>
+      <c r="E13" s="33">
+        <v>3</v>
+      </c>
+      <c r="F13" s="33">
+        <v>17555</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="H13" s="34">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I13" s="33">
+        <v>17177</v>
+      </c>
+      <c r="J13" s="34">
+        <v>2</v>
+      </c>
+      <c r="K13" s="33">
+        <v>15996</v>
+      </c>
+      <c r="L13" s="35">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="M13" s="36">
+        <f>ROUND(K13*(1-L13),0)</f>
+        <v>15148</v>
+      </c>
+      <c r="N13" s="37">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="O13" s="24">
+        <f t="shared" si="55"/>
+        <v>10164.308000000001</v>
+      </c>
+      <c r="P13" s="35">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="Q13" s="24">
+        <f t="shared" si="56"/>
+        <v>4044.5160000000001</v>
+      </c>
+      <c r="R13" s="38">
+        <v>6.2E-2</v>
+      </c>
+      <c r="S13" s="134">
+        <v>0.18590000000000001</v>
+      </c>
+      <c r="T13" s="24">
+        <f t="shared" si="57"/>
+        <v>939.17600000000004</v>
+      </c>
+      <c r="U13" s="27">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="V13" s="24">
+        <f t="shared" si="58"/>
+        <v>3196.2280000000001</v>
+      </c>
+      <c r="W13" s="38">
+        <v>0.503</v>
+      </c>
+      <c r="X13" s="24">
+        <f t="shared" si="59"/>
+        <v>7619.4440000000004</v>
+      </c>
+      <c r="Y13" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="Z13" s="24">
+        <f t="shared" si="60"/>
+        <v>6059.2000000000007</v>
+      </c>
+      <c r="AA13" s="146"/>
+      <c r="AB13" s="18">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="39">
+        <v>2.4499999999999999E-3</v>
+      </c>
+      <c r="AD13" s="17">
+        <f t="shared" si="62"/>
+        <v>37.1126</v>
+      </c>
+      <c r="AE13" s="26">
+        <f>IF(M13&gt;0,(AG13+AP13)/M13,0)</f>
+        <v>2.6098444151043038E-3</v>
+      </c>
+      <c r="AF13" s="39">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="AG13" s="36">
+        <f t="shared" si="63"/>
+        <v>3.9384799999999998</v>
+      </c>
+      <c r="AH13" s="27">
+        <v>0.2175</v>
+      </c>
+      <c r="AI13" s="40">
+        <f t="shared" si="64"/>
+        <v>35.579084999999999</v>
+      </c>
+      <c r="AJ13" s="27">
+        <f t="shared" si="65"/>
+        <v>0.89494737316764317</v>
+      </c>
+      <c r="AK13" s="28">
+        <f t="shared" si="6"/>
+        <v>0.90145430847263552</v>
+      </c>
+      <c r="AL13" s="33">
+        <v>178</v>
+      </c>
+      <c r="AM13" s="35">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AN13" s="37">
+        <v>0.21759999999999999</v>
+      </c>
+      <c r="AO13" s="132"/>
+      <c r="AP13" s="40">
+        <f>AL13*(1-AM13)*AN13</f>
+        <v>35.595443199999998</v>
+      </c>
+      <c r="AQ13" s="133">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AR13" s="41">
+        <v>1.55</v>
+      </c>
+      <c r="AS13" s="41"/>
+      <c r="AT13" s="110">
+        <f>AT12+AL13-AS13</f>
+        <v>2371.92</v>
+      </c>
+      <c r="AU13" s="101"/>
+      <c r="AV13" s="42"/>
+      <c r="AW13" s="43"/>
+      <c r="AX13" s="44"/>
+      <c r="AY13" s="44"/>
+      <c r="AZ13" s="44"/>
+      <c r="BA13" s="44"/>
+    </row>
+    <row r="14" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="183"/>
+      <c r="B14" s="32">
+        <v>3</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="42">
+        <v>17879</v>
+      </c>
+      <c r="E14" s="42">
+        <v>1</v>
+      </c>
+      <c r="F14" s="42">
+        <v>18694</v>
+      </c>
+      <c r="G14" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="36">
+        <v>7.2</v>
+      </c>
+      <c r="I14" s="42">
+        <v>18039</v>
+      </c>
+      <c r="J14" s="36">
+        <v>1.6</v>
+      </c>
+      <c r="K14" s="42">
+        <v>15758</v>
+      </c>
+      <c r="L14" s="38">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="M14" s="36">
+        <f>ROUND(K14*(1-L14),0)</f>
+        <v>14844</v>
+      </c>
+      <c r="N14" s="27">
+        <v>0.65</v>
+      </c>
+      <c r="O14" s="24">
+        <f t="shared" si="55"/>
+        <v>9648.6</v>
+      </c>
+      <c r="P14" s="38">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="Q14" s="24">
+        <f t="shared" si="56"/>
+        <v>4230.54</v>
+      </c>
+      <c r="R14" s="38">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="S14" s="134">
+        <v>0.1802</v>
+      </c>
+      <c r="T14" s="24">
+        <f t="shared" si="57"/>
+        <v>964.86</v>
+      </c>
+      <c r="U14" s="27"/>
+      <c r="V14" s="24">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="38"/>
+      <c r="X14" s="24">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z14" s="24">
+        <f t="shared" si="60"/>
+        <v>6086.04</v>
+      </c>
+      <c r="AA14" s="147"/>
+      <c r="AB14" s="148">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="46">
+        <v>2.4099999999999998E-3</v>
+      </c>
+      <c r="AD14" s="17">
+        <f t="shared" si="62"/>
+        <v>35.774039999999999</v>
+      </c>
+      <c r="AE14" s="26">
+        <f>IF(M14&gt;0,(AG14+AP14)/M14,0)</f>
+        <v>2.7E-4</v>
+      </c>
+      <c r="AF14" s="46">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG14" s="36">
+        <f t="shared" si="63"/>
+        <v>4.0078800000000001</v>
+      </c>
+      <c r="AH14" s="27">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="AI14" s="40">
+        <f t="shared" si="64"/>
+        <v>34.171728000000002</v>
+      </c>
+      <c r="AJ14" s="27">
+        <f t="shared" si="65"/>
+        <v>0.88910722755140936</v>
+      </c>
+      <c r="AK14" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AL14" s="42">
+        <v>178</v>
+      </c>
+      <c r="AM14" s="38">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="AN14" s="27"/>
+      <c r="AO14" s="134"/>
+      <c r="AP14" s="40">
+        <f>AL14*(1-AM14)*AN14</f>
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="135">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AR14" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS14" s="17"/>
+      <c r="AT14" s="110">
+        <f>AT13+AL14-AS14</f>
+        <v>2549.92</v>
+      </c>
+      <c r="AU14" s="101"/>
+      <c r="AV14" s="42"/>
+      <c r="AW14" s="47"/>
+      <c r="AX14" s="40"/>
+      <c r="AY14" s="40"/>
+      <c r="AZ14" s="40"/>
+      <c r="BA14" s="40"/>
+    </row>
+    <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="184"/>
+      <c r="B15" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50">
+        <f t="shared" ref="D15" si="67">SUM(D12:D14)</f>
+        <v>50179</v>
+      </c>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50">
+        <f t="shared" ref="F15" si="68">SUM(F12:F14)</f>
+        <v>50455</v>
+      </c>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="50">
+        <f t="shared" ref="I15:K15" si="69">SUM(I12:I14)</f>
+        <v>48802</v>
+      </c>
+      <c r="J15" s="51"/>
+      <c r="K15" s="50">
+        <f t="shared" si="69"/>
+        <v>47632</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" ref="L15" si="70">IF(K15&gt;0,(K12*L12+K13*L13+K14*L14)/K15,0)</f>
+        <v>5.6654224051058112E-2</v>
+      </c>
+      <c r="M15" s="51">
+        <f t="shared" ref="M15" si="71">M12+M13+M14</f>
+        <v>44933</v>
+      </c>
+      <c r="N15" s="52">
+        <f t="shared" ref="N15" si="72">IF(M15&gt;0,O15/M15,0)</f>
+        <v>0.63214080964992325</v>
+      </c>
+      <c r="O15" s="53">
+        <f t="shared" ref="O15" si="73">O12+O13+O14</f>
+        <v>28403.983</v>
+      </c>
+      <c r="P15" s="20">
+        <f t="shared" ref="P15" si="74">IF(M15&gt;0,Q15/M15,0)</f>
+        <v>0.27427652282286957</v>
+      </c>
+      <c r="Q15" s="53">
+        <f t="shared" ref="Q15" si="75">Q12+Q13+Q14</f>
+        <v>12324.066999999999</v>
+      </c>
+      <c r="R15" s="20">
+        <f t="shared" ref="R15" si="76">IF(M15&gt;0,T15/M15,0)</f>
+        <v>9.3582667527207175E-2</v>
+      </c>
+      <c r="S15" s="136"/>
+      <c r="T15" s="53">
+        <f t="shared" ref="T15" si="77">T12+T13+T14</f>
+        <v>4204.95</v>
+      </c>
+      <c r="U15" s="20">
+        <f t="shared" ref="U15" si="78">IF(M15&gt;0,V15/M15,0)</f>
+        <v>0.1373041417221196</v>
+      </c>
+      <c r="V15" s="53">
+        <f t="shared" ref="V15" si="79">V12+V13+V14</f>
+        <v>6169.4870000000001</v>
+      </c>
+      <c r="W15" s="20">
+        <f t="shared" ref="W15" si="80">IF(M15&gt;0,X15/M15,0)</f>
+        <v>0.33849224400774491</v>
+      </c>
+      <c r="X15" s="53">
+        <f t="shared" ref="X15" si="81">X12+X13+X14</f>
+        <v>15209.472000000002</v>
+      </c>
+      <c r="Y15" s="20">
+        <f t="shared" ref="Y15" si="82">IF(M15&gt;0,Z15/M15,0)</f>
+        <v>0.40330358533817023</v>
+      </c>
+      <c r="Z15" s="53">
+        <f t="shared" ref="Z15" si="83">Z12+Z13+Z14</f>
+        <v>18121.640000000003</v>
+      </c>
+      <c r="AA15" s="152">
+        <f>IF(M15&gt;0,AB15/M15,0)</f>
+        <v>8.2131773974584369E-4</v>
+      </c>
+      <c r="AB15" s="55">
+        <f t="shared" ref="AB15" si="84">SUM(AB12:AB14)</f>
+        <v>36.904269999999997</v>
+      </c>
+      <c r="AC15" s="54">
+        <f t="shared" ref="AC15" si="85">IF(M15&gt;0,AD15/M15,0)</f>
+        <v>2.420159793470278E-3</v>
+      </c>
+      <c r="AD15" s="55">
+        <f t="shared" ref="AD15" si="86">SUM(AD12:AD14)</f>
+        <v>108.74504</v>
+      </c>
+      <c r="AE15" s="54">
+        <f t="shared" ref="AE15" si="87">IF(M15&gt;0,(AE12*M12+AE13*M13+AE14*M14)/M15,0)</f>
+        <v>1.7841623038746576E-3</v>
+      </c>
+      <c r="AF15" s="54">
+        <f t="shared" ref="AF15" si="88">IF(K15&gt;0,(K12*AF12+K13*AF13+K14*AF14)/K15,0)</f>
+        <v>2.6330828014779978E-4</v>
+      </c>
+      <c r="AG15" s="51">
+        <f t="shared" ref="AG15" si="89">SUM(AG12:AG14)</f>
+        <v>11.831019999999999</v>
+      </c>
+      <c r="AH15" s="52">
+        <f t="shared" ref="AH15" si="90">IF(K15&gt;0,(K12*AH12+K13*AH13+K14*AH14)/K15,0)</f>
+        <v>0.21245075579442393</v>
+      </c>
+      <c r="AI15" s="57">
+        <f t="shared" ref="AI15" si="91">SUM(AI12:AI14)</f>
+        <v>100.8431652</v>
+      </c>
+      <c r="AJ15" s="52">
+        <f t="shared" ref="AJ15" si="92">IF(AND(AD15&gt;0),((AD12*AJ12+AD13*AJ13+AD14*AJ14)/AD15),0)</f>
+        <v>0.89231002846169372</v>
+      </c>
+      <c r="AK15" s="56">
+        <f t="shared" si="6"/>
+        <v>0.85395345861968397</v>
+      </c>
+      <c r="AL15" s="50">
+        <f t="shared" ref="AL15" si="93">SUM(AL12:AL14)</f>
+        <v>518</v>
+      </c>
+      <c r="AM15" s="20">
+        <f t="shared" ref="AM15" si="94">IF(AL15&gt;0,(AM12*AL12+AM13*AL13+AM14*AL14)/AL15,0)</f>
+        <v>8.403088803088804E-2</v>
+      </c>
+      <c r="AN15" s="52">
+        <f>IF(K15&gt;0,(AN12*K12+AN13*K13+AN14*K14)/K15,0)</f>
+        <v>0.14654519650655021</v>
+      </c>
+      <c r="AO15" s="136">
+        <f>IF(K15&gt;0,(AO12*K12+AO13*K13+AO14*K14)/K15,0)</f>
+        <v>7.4436458683238158E-2</v>
+      </c>
+      <c r="AP15" s="57">
+        <f t="shared" ref="AP15" si="95">SUM(AP12:AP14)</f>
+        <v>68.336744799999991</v>
+      </c>
+      <c r="AQ15" s="137">
+        <f t="shared" si="52"/>
+        <v>33.172108199999997</v>
+      </c>
+      <c r="AR15" s="55"/>
+      <c r="AS15" s="55">
+        <f t="shared" ref="AS15" si="96">SUM(AS12:AS14)</f>
+        <v>0</v>
+      </c>
+      <c r="AT15" s="102"/>
+      <c r="AU15" s="103">
+        <f>AT14</f>
+        <v>2549.92</v>
+      </c>
+      <c r="AV15" s="50">
+        <f t="shared" ref="AV15" si="97">SUM(AV12:AV14)</f>
+        <v>0</v>
+      </c>
+      <c r="AW15" s="58"/>
+      <c r="AX15" s="57"/>
+      <c r="AY15" s="57"/>
+      <c r="AZ15" s="57"/>
+      <c r="BA15" s="57"/>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="Q1:Q3 V1:V3 X1:X3 Z1:Z3 AP1:AQ15 O1:O3 T1:T3 AG1:AG3 AK1:AK15 AD1:AE3 M1:M15" name="Range1_1_1_1_1_1_1_1_1"/>
+    <protectedRange sqref="AH3:AJ3 AH7:AJ7 AI1:AJ2 AH4:AI6 AH11:AJ11 AH15:AJ15 AH8:AI10 AH12:AI14" name="Range1_1_1_1_1_1_1"/>
+    <protectedRange sqref="AJ4:AJ6 AJ8:AJ10 AJ12:AJ14" name="Range1_1_1_1"/>
+    <protectedRange sqref="AD7:AE7 AD4:AD6 AD11:AE11 AD8:AD10 AD15:AE15 AD12:AD14" name="Range1_1_1_1_1_2_2_1"/>
+    <protectedRange sqref="O4:O15" name="Range1_1_1_1_1_5_1_1"/>
+    <protectedRange sqref="Q4:Q15" name="Range1_1_1_1_1_7_1_1"/>
+    <protectedRange sqref="T4:T15" name="Range1_1_1_1_1_8_1_1"/>
+    <protectedRange sqref="V4:V15" name="Range1_1_1_1_1_10_1_1"/>
+    <protectedRange sqref="X4:X15" name="Range1_1_1_1_1_12_1_1"/>
+    <protectedRange sqref="Z4:Z15" name="Range1_1_1_1_1_16_1_1"/>
+    <protectedRange sqref="AG4:AG15" name="Range1_1_1_1_1_18_1_1"/>
+    <protectedRange sqref="AE4:AE6" name="Range1_1_1_1_1_2_1_31_1_1"/>
+    <protectedRange sqref="AE8:AE10" name="Range1_1_1_1_1_2_1_1_2_1_1"/>
+    <protectedRange sqref="AE12:AE14" name="Range1_1_1_1_1_2_1_2_1_1_1"/>
+    <protectedRange sqref="AA3:AB3" name="Range1_1_1_1_1_1_1_1_1_1_2"/>
+    <protectedRange sqref="AB4:AB15" name="Range1_1_1_1_1_2_2_1_1_1"/>
+    <protectedRange sqref="AB1" name="Range1_1_1_1_1_1_1_1_1_1_1_1"/>
+  </protectedRanges>
+  <mergeCells count="8">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="A4:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing the target trend PV
</commit_message>
<xml_diff>
--- a/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
+++ b/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7821C385-163F-4051-ADD6-1EF91D4DCF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B22EF-423A-40D9-BA99-F1CD05A9273D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="70">
   <si>
     <t xml:space="preserve">Подадена руда
  от МГТЛ 
@@ -1688,6 +1688,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1695,6 +1698,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1714,12 +1720,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1770,7 +1770,7 @@
       <sheetData sheetId="6">
         <row r="127">
           <cell r="AU127">
-            <v>1478.34</v>
+            <v>1519.34</v>
           </cell>
         </row>
       </sheetData>
@@ -2139,13 +2139,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -2274,19 +2274,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -2639,7 +2639,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -2799,7 +2799,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -3294,7 +3294,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -3454,7 +3454,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -3614,7 +3614,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -3785,7 +3785,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -3949,7 +3949,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -4109,7 +4109,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -4269,7 +4269,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182">
+      <c r="A16" s="183">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -4604,7 +4604,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="183"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -4764,7 +4764,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="183"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -4924,7 +4924,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="184"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -5095,7 +5095,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182">
+      <c r="A20" s="183">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -5259,7 +5259,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="183"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -5419,7 +5419,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="183"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="184"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182">
+      <c r="A24" s="183">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -5916,7 +5916,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -6076,7 +6076,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="183"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -6236,7 +6236,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
+      <c r="A27" s="185"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -6407,7 +6407,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="182">
+      <c r="A28" s="183">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -6569,7 +6569,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="183"/>
+      <c r="A29" s="184"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -6729,7 +6729,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="183"/>
+      <c r="A30" s="184"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="184"/>
+      <c r="A31" s="185"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -7060,7 +7060,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="182">
+      <c r="A32" s="183">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -7222,7 +7222,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="183"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="183"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -7542,7 +7542,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="184"/>
+      <c r="A35" s="185"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -7713,7 +7713,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182">
+      <c r="A36" s="183">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -7877,7 +7877,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="183"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -8037,7 +8037,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="183"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -8197,7 +8197,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="184"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -8368,7 +8368,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="182">
+      <c r="A40" s="183">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -8532,7 +8532,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="183"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -8692,7 +8692,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="183"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -8852,7 +8852,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="182">
+      <c r="A44" s="183">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -9187,7 +9187,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="183"/>
+      <c r="A45" s="184"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -9347,7 +9347,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="183"/>
+      <c r="A46" s="184"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -9507,7 +9507,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="184"/>
+      <c r="A47" s="185"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="182">
+      <c r="A48" s="183">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -9844,7 +9844,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="183"/>
+      <c r="A49" s="184"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -10004,7 +10004,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="183"/>
+      <c r="A50" s="184"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -10164,7 +10164,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
+      <c r="A51" s="185"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -10335,7 +10335,7 @@
       <c r="BA51" s="57"/>
     </row>
     <row r="52" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="182">
+      <c r="A52" s="183">
         <v>13</v>
       </c>
       <c r="B52" s="22">
@@ -10499,7 +10499,7 @@
       <c r="BA52" s="19"/>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A53" s="183"/>
+      <c r="A53" s="184"/>
       <c r="B53" s="32">
         <v>2</v>
       </c>
@@ -10659,7 +10659,7 @@
       <c r="BA53" s="44"/>
     </row>
     <row r="54" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A54" s="183"/>
+      <c r="A54" s="184"/>
       <c r="B54" s="32">
         <v>3</v>
       </c>
@@ -10819,7 +10819,7 @@
       <c r="BA54" s="40"/>
     </row>
     <row r="55" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="184"/>
+      <c r="A55" s="185"/>
       <c r="B55" s="48" t="s">
         <v>35</v>
       </c>
@@ -10990,7 +10990,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="182">
+      <c r="A56" s="183">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -11152,7 +11152,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="183"/>
+      <c r="A57" s="184"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -11312,7 +11312,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="183"/>
+      <c r="A58" s="184"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -11472,7 +11472,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
+      <c r="A59" s="185"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -11643,7 +11643,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="182">
+      <c r="A60" s="183">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -11805,7 +11805,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="183"/>
+      <c r="A61" s="184"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -11965,7 +11965,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="183"/>
+      <c r="A62" s="184"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -12125,7 +12125,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
+      <c r="A63" s="185"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -12296,7 +12296,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="182">
+      <c r="A64" s="183">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -12460,7 +12460,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="183"/>
+      <c r="A65" s="184"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -12620,7 +12620,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="183"/>
+      <c r="A66" s="184"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -12780,7 +12780,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
+      <c r="A67" s="185"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -12951,7 +12951,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="182">
+      <c r="A68" s="183">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -13115,7 +13115,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="183"/>
+      <c r="A69" s="184"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -13275,7 +13275,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="183"/>
+      <c r="A70" s="184"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -13435,7 +13435,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="184"/>
+      <c r="A71" s="185"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -13606,7 +13606,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="182">
+      <c r="A72" s="183">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -13772,7 +13772,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="183"/>
+      <c r="A73" s="184"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -13932,7 +13932,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="183"/>
+      <c r="A74" s="184"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -14092,7 +14092,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="184"/>
+      <c r="A75" s="185"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -14263,7 +14263,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="182">
+      <c r="A76" s="183">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -14427,7 +14427,7 @@
       <c r="BA76" s="175"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="183"/>
+      <c r="A77" s="184"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -14587,7 +14587,7 @@
       <c r="BA77" s="176"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="183"/>
+      <c r="A78" s="184"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -14747,7 +14747,7 @@
       <c r="BA78" s="177"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="184"/>
+      <c r="A79" s="185"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -14918,7 +14918,7 @@
       <c r="BA79" s="179"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="183">
+      <c r="A80" s="184">
         <v>20</v>
       </c>
       <c r="B80" s="32">
@@ -15084,7 +15084,7 @@
       <c r="BA80" s="168"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="183"/>
+      <c r="A81" s="184"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -15244,7 +15244,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="183"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -15404,7 +15404,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="184"/>
+      <c r="A83" s="185"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -15575,7 +15575,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="182">
+      <c r="A84" s="183">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -15737,7 +15737,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="183"/>
+      <c r="A85" s="184"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -15897,7 +15897,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="183"/>
+      <c r="A86" s="184"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -16057,7 +16057,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="184"/>
+      <c r="A87" s="185"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -16228,7 +16228,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182">
+      <c r="A88" s="183">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -16390,7 +16390,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="183"/>
+      <c r="A89" s="184"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -16550,7 +16550,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="183"/>
+      <c r="A90" s="184"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -16710,7 +16710,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="184"/>
+      <c r="A91" s="185"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -16881,7 +16881,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="182">
+      <c r="A92" s="183">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -17045,7 +17045,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="183"/>
+      <c r="A93" s="184"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -17205,7 +17205,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="183"/>
+      <c r="A94" s="184"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -17365,7 +17365,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="184"/>
+      <c r="A95" s="185"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -17536,7 +17536,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182">
+      <c r="A96" s="183">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -17702,7 +17702,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="183"/>
+      <c r="A97" s="184"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -17862,7 +17862,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="183"/>
+      <c r="A98" s="184"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -18022,7 +18022,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="184"/>
+      <c r="A99" s="185"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -18190,7 +18190,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="192">
+      <c r="A100" s="186">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -18356,7 +18356,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="192"/>
+      <c r="A101" s="186"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -18516,7 +18516,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="192"/>
+      <c r="A102" s="186"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -18676,7 +18676,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="192"/>
+      <c r="A103" s="186"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -18847,7 +18847,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="182">
+      <c r="A104" s="183">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -19013,7 +19013,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="183"/>
+      <c r="A105" s="184"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -19173,7 +19173,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="183"/>
+      <c r="A106" s="184"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -19333,7 +19333,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="184"/>
+      <c r="A107" s="185"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -19504,7 +19504,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="182">
+      <c r="A108" s="183">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -19670,7 +19670,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="183"/>
+      <c r="A109" s="184"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -19830,7 +19830,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="183"/>
+      <c r="A110" s="184"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -19990,7 +19990,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="184"/>
+      <c r="A111" s="185"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -20161,7 +20161,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182">
+      <c r="A112" s="183">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -20323,7 +20323,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="183"/>
+      <c r="A113" s="184"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -20483,7 +20483,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="183"/>
+      <c r="A114" s="184"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -20643,7 +20643,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="184"/>
+      <c r="A115" s="185"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -20814,7 +20814,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="183">
+      <c r="A116" s="184">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -20976,7 +20976,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="183"/>
+      <c r="A117" s="184"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -21136,7 +21136,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="183"/>
+      <c r="A118" s="184"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -21296,7 +21296,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="184"/>
+      <c r="A119" s="185"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -21467,7 +21467,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="182">
+      <c r="A120" s="183">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -21633,7 +21633,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="183"/>
+      <c r="A121" s="184"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -21793,7 +21793,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="183"/>
+      <c r="A122" s="184"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -21953,7 +21953,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
+      <c r="A123" s="185"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -22124,7 +22124,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="182">
+      <c r="A124" s="183">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -22234,7 +22234,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="183"/>
+      <c r="A125" s="184"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -22342,7 +22342,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="183"/>
+      <c r="A126" s="184"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -22450,7 +22450,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
+      <c r="A127" s="185"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -22843,6 +22843,26 @@
     <protectedRange sqref="AB1" name="Range1_1_1_1_1_1_1_1_1_1_1"/>
   </protectedRanges>
   <mergeCells count="36">
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A100:A103"/>
@@ -22859,26 +22879,6 @@
     <mergeCell ref="A68:A71"/>
     <mergeCell ref="A84:A87"/>
     <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -22956,13 +22956,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -23091,19 +23091,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -23294,7 +23294,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -23458,7 +23458,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -23617,7 +23617,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -23776,7 +23776,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -23947,7 +23947,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -24111,7 +24111,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -24271,7 +24271,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -24431,7 +24431,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -24602,7 +24602,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -24764,7 +24764,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -24924,7 +24924,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -25084,7 +25084,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -25255,7 +25255,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182">
+      <c r="A16" s="183">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -25417,7 +25417,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="183"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -25577,7 +25577,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="183"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -25737,7 +25737,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="184"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -25908,7 +25908,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182">
+      <c r="A20" s="183">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -26070,7 +26070,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="183"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -26230,7 +26230,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="183"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -26390,7 +26390,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="184"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -26561,7 +26561,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182">
+      <c r="A24" s="183">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -26723,7 +26723,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -26883,7 +26883,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="183"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -27043,7 +27043,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
+      <c r="A27" s="185"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -27214,7 +27214,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="182">
+      <c r="A28" s="183">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -27378,7 +27378,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="183"/>
+      <c r="A29" s="184"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -27536,7 +27536,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="183"/>
+      <c r="A30" s="184"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -27694,7 +27694,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="184"/>
+      <c r="A31" s="185"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -27865,7 +27865,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="182">
+      <c r="A32" s="183">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -28029,7 +28029,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="183"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -28189,7 +28189,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="183"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -28349,7 +28349,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="184"/>
+      <c r="A35" s="185"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -28520,7 +28520,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182">
+      <c r="A36" s="183">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -28684,7 +28684,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="183"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -28844,7 +28844,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="183"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -29004,7 +29004,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="184"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -29175,7 +29175,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="182">
+      <c r="A40" s="183">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -29339,7 +29339,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="183"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -29495,7 +29495,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="183"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -29643,7 +29643,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -29814,7 +29814,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="182">
+      <c r="A44" s="183">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -29976,7 +29976,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="183"/>
+      <c r="A45" s="184"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -30136,7 +30136,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="183"/>
+      <c r="A46" s="184"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -30296,7 +30296,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="184"/>
+      <c r="A47" s="185"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -30467,7 +30467,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="182">
+      <c r="A48" s="183">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -30629,7 +30629,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="183"/>
+      <c r="A49" s="184"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -30789,7 +30789,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="183"/>
+      <c r="A50" s="184"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -30949,7 +30949,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
+      <c r="A51" s="185"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -31754,7 +31754,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="182">
+      <c r="A56" s="183">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -31918,7 +31918,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="183"/>
+      <c r="A57" s="184"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -32078,7 +32078,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="183"/>
+      <c r="A58" s="184"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -32238,7 +32238,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
+      <c r="A59" s="185"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -32409,7 +32409,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="182">
+      <c r="A60" s="183">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -32573,7 +32573,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="183"/>
+      <c r="A61" s="184"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -32733,7 +32733,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="183"/>
+      <c r="A62" s="184"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -32893,7 +32893,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
+      <c r="A63" s="185"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -33064,7 +33064,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="182">
+      <c r="A64" s="183">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -33230,7 +33230,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="183"/>
+      <c r="A65" s="184"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -33390,7 +33390,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="183"/>
+      <c r="A66" s="184"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -33550,7 +33550,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
+      <c r="A67" s="185"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -33721,7 +33721,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="182">
+      <c r="A68" s="183">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -33885,7 +33885,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="183"/>
+      <c r="A69" s="184"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -34045,7 +34045,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="183"/>
+      <c r="A70" s="184"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -34205,7 +34205,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="184"/>
+      <c r="A71" s="185"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -34376,7 +34376,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="182">
+      <c r="A72" s="183">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -34540,7 +34540,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="183"/>
+      <c r="A73" s="184"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -34700,7 +34700,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="183"/>
+      <c r="A74" s="184"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -34860,7 +34860,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="184"/>
+      <c r="A75" s="185"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -35031,7 +35031,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="182">
+      <c r="A76" s="183">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -35193,7 +35193,7 @@
       <c r="BA76" s="19"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="183"/>
+      <c r="A77" s="184"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -35353,7 +35353,7 @@
       <c r="BA77" s="44"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="183"/>
+      <c r="A78" s="184"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -35513,7 +35513,7 @@
       <c r="BA78" s="40"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="184"/>
+      <c r="A79" s="185"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -35684,7 +35684,7 @@
       <c r="BA79" s="57"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="182">
+      <c r="A80" s="183">
         <v>20</v>
       </c>
       <c r="B80" s="22">
@@ -35846,7 +35846,7 @@
       <c r="BA80" s="19"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="183"/>
+      <c r="A81" s="184"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -36006,7 +36006,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="183"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -36166,7 +36166,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="184"/>
+      <c r="A83" s="185"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -36337,7 +36337,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="182">
+      <c r="A84" s="183">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -36501,7 +36501,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="183"/>
+      <c r="A85" s="184"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -36661,7 +36661,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="183"/>
+      <c r="A86" s="184"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -36821,7 +36821,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="184"/>
+      <c r="A87" s="185"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -36992,7 +36992,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182">
+      <c r="A88" s="183">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -37156,7 +37156,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="183"/>
+      <c r="A89" s="184"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -37316,7 +37316,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="183"/>
+      <c r="A90" s="184"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -37476,7 +37476,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="184"/>
+      <c r="A91" s="185"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -37647,7 +37647,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="182">
+      <c r="A92" s="183">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -37811,7 +37811,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="183"/>
+      <c r="A93" s="184"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -37969,7 +37969,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="183"/>
+      <c r="A94" s="184"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -38123,7 +38123,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="184"/>
+      <c r="A95" s="185"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -38294,7 +38294,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182">
+      <c r="A96" s="183">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -38458,7 +38458,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="183"/>
+      <c r="A97" s="184"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -38618,7 +38618,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="183"/>
+      <c r="A98" s="184"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -38778,7 +38778,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="184"/>
+      <c r="A99" s="185"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -38949,7 +38949,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="192">
+      <c r="A100" s="186">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -39113,7 +39113,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="192"/>
+      <c r="A101" s="186"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -39273,7 +39273,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="192"/>
+      <c r="A102" s="186"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -39433,7 +39433,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="192"/>
+      <c r="A103" s="186"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -39604,7 +39604,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="182">
+      <c r="A104" s="183">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -39766,7 +39766,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="183"/>
+      <c r="A105" s="184"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -39926,7 +39926,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="183"/>
+      <c r="A106" s="184"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -40086,7 +40086,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="184"/>
+      <c r="A107" s="185"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -40257,7 +40257,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="182">
+      <c r="A108" s="183">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -40419,7 +40419,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="183"/>
+      <c r="A109" s="184"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -40575,7 +40575,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="183"/>
+      <c r="A110" s="184"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -40725,7 +40725,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="184"/>
+      <c r="A111" s="185"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -40896,7 +40896,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182">
+      <c r="A112" s="183">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -41060,7 +41060,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="183"/>
+      <c r="A113" s="184"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -41220,7 +41220,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="183"/>
+      <c r="A114" s="184"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -41380,7 +41380,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="184"/>
+      <c r="A115" s="185"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -41551,7 +41551,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="183">
+      <c r="A116" s="184">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -41715,7 +41715,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="183"/>
+      <c r="A117" s="184"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -41875,7 +41875,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="183"/>
+      <c r="A118" s="184"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -42035,7 +42035,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="184"/>
+      <c r="A119" s="185"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -42206,7 +42206,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="182">
+      <c r="A120" s="183">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -42370,7 +42370,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="183"/>
+      <c r="A121" s="184"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -42530,7 +42530,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="183"/>
+      <c r="A122" s="184"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -42690,7 +42690,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
+      <c r="A123" s="185"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -42861,7 +42861,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="182">
+      <c r="A124" s="183">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -43025,7 +43025,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="183"/>
+      <c r="A125" s="184"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -43181,7 +43181,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="183"/>
+      <c r="A126" s="184"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -43331,7 +43331,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
+      <c r="A127" s="185"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -43767,18 +43767,16 @@
     <protectedRange sqref="AB112:AB127" name="Range1_1_1_1_1_2_2_1_1_4"/>
   </protectedRanges>
   <mergeCells count="35">
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A111"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A35"/>
@@ -43792,16 +43790,18 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43811,22 +43811,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6555BB66-49A2-4157-88D4-D9BD7AEDD16F}">
-  <dimension ref="A1:BA15"/>
+  <dimension ref="A1:BA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -43955,19 +43955,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -44147,7 +44147,7 @@
       <c r="AS3" s="96"/>
       <c r="AT3" s="119">
         <f>[1]Юли!AU127</f>
-        <v>1478.34</v>
+        <v>1519.34</v>
       </c>
       <c r="AU3" s="97"/>
       <c r="AV3" s="88"/>
@@ -44158,7 +44158,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -44280,7 +44280,7 @@
         <v>0.89341832658664044</v>
       </c>
       <c r="AK4" s="59">
-        <f t="shared" ref="AK4:AK15" si="6">IF(AND(AE4&gt;0,AN4&gt;0,AF4&gt;0),((AN4*(AE4-AF4))/(AE4*(AN4-AF4))),0)</f>
+        <f t="shared" ref="AK4:AK27" si="6">IF(AND(AE4&gt;0,AN4&gt;0,AF4&gt;0),((AN4*(AE4-AF4))/(AE4*(AN4-AF4))),0)</f>
         <v>0.89517063729570767</v>
       </c>
       <c r="AL4" s="11">
@@ -44311,7 +44311,7 @@
       </c>
       <c r="AT4" s="110">
         <f>AT3+AL4-AS4</f>
-        <v>1167.9199999999998</v>
+        <v>1208.9199999999998</v>
       </c>
       <c r="AU4" s="99"/>
       <c r="AV4" s="11"/>
@@ -44322,7 +44322,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -44471,7 +44471,7 @@
       <c r="AS5" s="41"/>
       <c r="AT5" s="110">
         <f>AT4+AL5-AS5</f>
-        <v>1338.9199999999998</v>
+        <v>1379.9199999999998</v>
       </c>
       <c r="AU5" s="100"/>
       <c r="AV5" s="42"/>
@@ -44482,7 +44482,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -44631,7 +44631,7 @@
       <c r="AS6" s="17"/>
       <c r="AT6" s="110">
         <f>AT5+AL6-AS6</f>
-        <v>1523.9199999999998</v>
+        <v>1564.9199999999998</v>
       </c>
       <c r="AU6" s="101"/>
       <c r="AV6" s="42"/>
@@ -44642,7 +44642,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -44800,7 +44800,7 @@
       <c r="AT7" s="102"/>
       <c r="AU7" s="103">
         <f>AT6</f>
-        <v>1523.9199999999998</v>
+        <v>1564.9199999999998</v>
       </c>
       <c r="AV7" s="50">
         <f>SUM(AV4:AV6)</f>
@@ -44813,7 +44813,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -44955,7 +44955,7 @@
         <v>31.889440799999999</v>
       </c>
       <c r="AQ8" s="131">
-        <f t="shared" ref="AQ8:AQ15" si="21">AL8*(1-AM8)*AO8</f>
+        <f t="shared" ref="AQ8:AQ14" si="21">AL8*(1-AM8)*AO8</f>
         <v>31.5184608</v>
       </c>
       <c r="AR8" s="18">
@@ -44964,7 +44964,7 @@
       <c r="AS8" s="18"/>
       <c r="AT8" s="98">
         <f>AT6+AL8-AS8</f>
-        <v>1685.9199999999998</v>
+        <v>1726.9199999999998</v>
       </c>
       <c r="AU8" s="99"/>
       <c r="AV8" s="11"/>
@@ -44975,7 +44975,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -45124,7 +45124,7 @@
       <c r="AS9" s="41"/>
       <c r="AT9" s="110">
         <f>AT8+AL9-AS9</f>
-        <v>1857.9199999999998</v>
+        <v>1898.9199999999998</v>
       </c>
       <c r="AU9" s="101"/>
       <c r="AV9" s="42"/>
@@ -45135,7 +45135,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -45284,7 +45284,7 @@
       <c r="AS10" s="17"/>
       <c r="AT10" s="110">
         <f>AT9+AL10-AS10</f>
-        <v>2031.9199999999998</v>
+        <v>2072.92</v>
       </c>
       <c r="AU10" s="101"/>
       <c r="AV10" s="42"/>
@@ -45295,7 +45295,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -45453,7 +45453,7 @@
       <c r="AT11" s="102"/>
       <c r="AU11" s="103">
         <f>AT10</f>
-        <v>2031.9199999999998</v>
+        <v>2072.92</v>
       </c>
       <c r="AV11" s="50">
         <f t="shared" ref="AV11" si="54">SUM(AV8:AV10)</f>
@@ -45466,7 +45466,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -45555,7 +45555,7 @@
         <v>2.47E-3</v>
       </c>
       <c r="AB12" s="18">
-        <f t="shared" ref="AB12:AB15" si="61">M12*AA12</f>
+        <f t="shared" ref="AB12:AB14" si="61">M12*AA12</f>
         <v>36.904269999999997</v>
       </c>
       <c r="AC12" s="16">
@@ -45617,7 +45617,7 @@
       <c r="AS12" s="18"/>
       <c r="AT12" s="98">
         <f>AT10+AL12-AS12</f>
-        <v>2193.92</v>
+        <v>2234.92</v>
       </c>
       <c r="AU12" s="99"/>
       <c r="AV12" s="11"/>
@@ -45628,7 +45628,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -45773,7 +45773,7 @@
       <c r="AS13" s="41"/>
       <c r="AT13" s="110">
         <f>AT12+AL13-AS13</f>
-        <v>2371.92</v>
+        <v>2412.92</v>
       </c>
       <c r="AU13" s="101"/>
       <c r="AV13" s="42"/>
@@ -45784,7 +45784,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -45923,7 +45923,7 @@
       <c r="AS14" s="17"/>
       <c r="AT14" s="110">
         <f>AT13+AL14-AS14</f>
-        <v>2549.92</v>
+        <v>2590.92</v>
       </c>
       <c r="AU14" s="101"/>
       <c r="AV14" s="42"/>
@@ -45934,7 +45934,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -46092,7 +46092,7 @@
       <c r="AT15" s="102"/>
       <c r="AU15" s="103">
         <f>AT14</f>
-        <v>2549.92</v>
+        <v>2590.92</v>
       </c>
       <c r="AV15" s="50">
         <f t="shared" ref="AV15" si="97">SUM(AV12:AV14)</f>
@@ -46103,6 +46103,1957 @@
       <c r="AY15" s="57"/>
       <c r="AZ15" s="57"/>
       <c r="BA15" s="57"/>
+    </row>
+    <row r="16" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="183">
+        <v>4</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="11">
+        <v>4000</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>9268</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="H16" s="12">
+        <v>5.4</v>
+      </c>
+      <c r="I16" s="11">
+        <v>9219</v>
+      </c>
+      <c r="J16" s="12">
+        <v>3.9</v>
+      </c>
+      <c r="K16" s="11">
+        <v>15811</v>
+      </c>
+      <c r="L16" s="13">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M16" s="23">
+        <f>ROUND(K16*(1-L16),0)</f>
+        <v>14878</v>
+      </c>
+      <c r="N16" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="O16" s="24">
+        <f t="shared" ref="O16:O18" si="98">M16*N16</f>
+        <v>9819.48</v>
+      </c>
+      <c r="P16" s="13">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="Q16" s="24">
+        <f t="shared" ref="Q16:Q18" si="99">M16*P16</f>
+        <v>4136.0840000000007</v>
+      </c>
+      <c r="R16" s="15">
+        <v>6.2E-2</v>
+      </c>
+      <c r="S16" s="143">
+        <v>0.18140000000000001</v>
+      </c>
+      <c r="T16" s="24">
+        <f t="shared" ref="T16:T18" si="100">M16*R16</f>
+        <v>922.43600000000004</v>
+      </c>
+      <c r="U16" s="25">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="V16" s="24">
+        <f t="shared" ref="V16:V18" si="101">M16*U16</f>
+        <v>2901.21</v>
+      </c>
+      <c r="W16" s="15">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="X16" s="24">
+        <f t="shared" ref="X16:X18" si="102">M16*W16</f>
+        <v>7647.2920000000004</v>
+      </c>
+      <c r="Y16" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="Z16" s="24">
+        <f t="shared" ref="Z16:Z18" si="103">Y16*M16</f>
+        <v>5951.2000000000007</v>
+      </c>
+      <c r="AA16" s="145">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="AB16" s="18">
+        <f t="shared" ref="AB16:AB26" si="104">M16*AA16</f>
+        <v>36.302320000000002</v>
+      </c>
+      <c r="AC16" s="16">
+        <v>2.33E-3</v>
+      </c>
+      <c r="AD16" s="17">
+        <f t="shared" ref="AD16:AD18" si="105">M16*AC16</f>
+        <v>34.66574</v>
+      </c>
+      <c r="AE16" s="26">
+        <f>IF(M16&gt;0,(AG16+AP16)/M16,0)</f>
+        <v>2.3499799166554645E-3</v>
+      </c>
+      <c r="AF16" s="16">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG16" s="23">
+        <f t="shared" ref="AG16:AG18" si="106">AF16*M16</f>
+        <v>4.0170599999999999</v>
+      </c>
+      <c r="AH16" s="114">
+        <v>0.2084</v>
+      </c>
+      <c r="AI16" s="29">
+        <f t="shared" ref="AI16:AI18" si="107">AL16*(1-AM16)*AH16</f>
+        <v>30.9459412</v>
+      </c>
+      <c r="AJ16" s="27">
+        <f t="shared" ref="AJ16:AJ18" si="108">IF(AND(AH16&gt;0,AF16&gt;0,AC16&gt;0),((AC16-AF16)*AH16)/((AH16-AF16)*AC16),0)</f>
+        <v>0.8852671108289244</v>
+      </c>
+      <c r="AK16" s="59">
+        <f t="shared" si="6"/>
+        <v>0.88625361833736738</v>
+      </c>
+      <c r="AL16" s="11">
+        <v>163</v>
+      </c>
+      <c r="AM16" s="13">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="AN16" s="14">
+        <v>0.2084</v>
+      </c>
+      <c r="AO16" s="130">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="AP16" s="29">
+        <f>AL16*(1-AM16)*AN16</f>
+        <v>30.9459412</v>
+      </c>
+      <c r="AQ16" s="131">
+        <f t="shared" ref="AQ16:AQ26" si="109">AL16*(1-AM16)*AO16</f>
+        <v>31.257776499999999</v>
+      </c>
+      <c r="AR16" s="18">
+        <v>1.55</v>
+      </c>
+      <c r="AS16" s="18">
+        <v>1049.24</v>
+      </c>
+      <c r="AT16" s="98">
+        <f>AT14+AL16-AS16</f>
+        <v>1704.68</v>
+      </c>
+      <c r="AU16" s="99"/>
+      <c r="AV16" s="11"/>
+      <c r="AW16" s="30"/>
+      <c r="AX16" s="19"/>
+      <c r="AY16" s="19"/>
+      <c r="AZ16" s="19"/>
+      <c r="BA16" s="19"/>
+    </row>
+    <row r="17" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="184"/>
+      <c r="B17" s="32">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="33">
+        <v>20500</v>
+      </c>
+      <c r="E17" s="33">
+        <v>3</v>
+      </c>
+      <c r="F17" s="33">
+        <v>16898</v>
+      </c>
+      <c r="G17" s="34">
+        <v>1.3</v>
+      </c>
+      <c r="H17" s="34">
+        <v>10.8</v>
+      </c>
+      <c r="I17" s="33">
+        <v>16942</v>
+      </c>
+      <c r="J17" s="34">
+        <v>2.7</v>
+      </c>
+      <c r="K17" s="33">
+        <v>15868</v>
+      </c>
+      <c r="L17" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="M17" s="36">
+        <f>ROUND(K17*(1-L17),0)</f>
+        <v>15075</v>
+      </c>
+      <c r="N17" s="37">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="O17" s="24">
+        <f t="shared" si="98"/>
+        <v>8683.1999999999989</v>
+      </c>
+      <c r="P17" s="35">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="Q17" s="24">
+        <f t="shared" si="99"/>
+        <v>5773.7250000000004</v>
+      </c>
+      <c r="R17" s="38">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="S17" s="134">
+        <v>0.1817</v>
+      </c>
+      <c r="T17" s="24">
+        <f t="shared" si="100"/>
+        <v>618.07500000000005</v>
+      </c>
+      <c r="U17" s="27">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="V17" s="24">
+        <f t="shared" si="101"/>
+        <v>3180.8249999999998</v>
+      </c>
+      <c r="W17" s="38">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="X17" s="24">
+        <f t="shared" si="102"/>
+        <v>7205.8499999999995</v>
+      </c>
+      <c r="Y17" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="Z17" s="24">
+        <f t="shared" si="103"/>
+        <v>6030</v>
+      </c>
+      <c r="AA17" s="146">
+        <v>2.4199999999999998E-3</v>
+      </c>
+      <c r="AB17" s="18">
+        <f t="shared" si="104"/>
+        <v>36.481499999999997</v>
+      </c>
+      <c r="AC17" s="39">
+        <v>2.31E-3</v>
+      </c>
+      <c r="AD17" s="17">
+        <f t="shared" si="105"/>
+        <v>34.823250000000002</v>
+      </c>
+      <c r="AE17" s="26">
+        <f>IF(M17&gt;0,(AG17+AP17)/M17,0)</f>
+        <v>2.4951113499170814E-3</v>
+      </c>
+      <c r="AF17" s="39">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG17" s="36">
+        <f t="shared" si="106"/>
+        <v>4.0702499999999997</v>
+      </c>
+      <c r="AH17" s="27">
+        <v>0.21160000000000001</v>
+      </c>
+      <c r="AI17" s="40">
+        <f t="shared" si="107"/>
+        <v>32.175049600000001</v>
+      </c>
+      <c r="AJ17" s="27">
+        <f t="shared" si="108"/>
+        <v>0.88424517327181418</v>
+      </c>
+      <c r="AK17" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89288122486936006</v>
+      </c>
+      <c r="AL17" s="33">
+        <v>166</v>
+      </c>
+      <c r="AM17" s="35">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AN17" s="37">
+        <v>0.22059999999999999</v>
+      </c>
+      <c r="AO17" s="132">
+        <v>0.2203</v>
+      </c>
+      <c r="AP17" s="40">
+        <f>AL17*(1-AM17)*AN17</f>
+        <v>33.543553600000003</v>
+      </c>
+      <c r="AQ17" s="133">
+        <f t="shared" si="109"/>
+        <v>33.497936800000005</v>
+      </c>
+      <c r="AR17" s="41">
+        <v>1.55</v>
+      </c>
+      <c r="AS17" s="41"/>
+      <c r="AT17" s="110">
+        <f>AT16+AL17-AS17</f>
+        <v>1870.68</v>
+      </c>
+      <c r="AU17" s="101"/>
+      <c r="AV17" s="42"/>
+      <c r="AW17" s="43"/>
+      <c r="AX17" s="44"/>
+      <c r="AY17" s="44"/>
+      <c r="AZ17" s="44"/>
+      <c r="BA17" s="44"/>
+    </row>
+    <row r="18" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="184"/>
+      <c r="B18" s="32">
+        <v>3</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="42">
+        <v>19750</v>
+      </c>
+      <c r="E18" s="42">
+        <v>1</v>
+      </c>
+      <c r="F18" s="42">
+        <v>19317</v>
+      </c>
+      <c r="G18" s="36">
+        <v>1.3</v>
+      </c>
+      <c r="H18" s="36">
+        <v>7.6</v>
+      </c>
+      <c r="I18" s="42">
+        <v>18773</v>
+      </c>
+      <c r="J18" s="36">
+        <v>1.2</v>
+      </c>
+      <c r="K18" s="42">
+        <v>15715</v>
+      </c>
+      <c r="L18" s="38">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="M18" s="36">
+        <f>ROUND(K18*(1-L18),0)</f>
+        <v>14662</v>
+      </c>
+      <c r="N18" s="27">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="O18" s="24">
+        <f t="shared" si="98"/>
+        <v>8034.7760000000007</v>
+      </c>
+      <c r="P18" s="38">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q18" s="24">
+        <f t="shared" si="99"/>
+        <v>6289.9979999999996</v>
+      </c>
+      <c r="R18" s="38">
+        <v>2.3E-2</v>
+      </c>
+      <c r="S18" s="134">
+        <v>0.1757</v>
+      </c>
+      <c r="T18" s="24">
+        <f t="shared" si="100"/>
+        <v>337.226</v>
+      </c>
+      <c r="U18" s="27">
+        <v>0.19</v>
+      </c>
+      <c r="V18" s="24">
+        <f t="shared" si="101"/>
+        <v>2785.78</v>
+      </c>
+      <c r="W18" s="38">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="X18" s="24">
+        <f t="shared" si="102"/>
+        <v>7506.9440000000004</v>
+      </c>
+      <c r="Y18" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z18" s="24">
+        <f t="shared" si="103"/>
+        <v>6011.42</v>
+      </c>
+      <c r="AA18" s="147">
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="AB18" s="148">
+        <f t="shared" si="104"/>
+        <v>32.9895</v>
+      </c>
+      <c r="AC18" s="46">
+        <v>2.31E-3</v>
+      </c>
+      <c r="AD18" s="17">
+        <f t="shared" si="105"/>
+        <v>33.869219999999999</v>
+      </c>
+      <c r="AE18" s="26">
+        <f>IF(M18&gt;0,(AG18+AP18)/M18,0)</f>
+        <v>2.4519773223298327E-3</v>
+      </c>
+      <c r="AF18" s="46">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG18" s="36">
+        <f t="shared" si="106"/>
+        <v>3.9587400000000001</v>
+      </c>
+      <c r="AH18" s="27">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="AI18" s="40">
+        <f t="shared" si="107"/>
+        <v>30.915562500000004</v>
+      </c>
+      <c r="AJ18" s="27">
+        <f t="shared" si="108"/>
+        <v>0.88424038855174891</v>
+      </c>
+      <c r="AK18" s="28">
+        <f t="shared" si="6"/>
+        <v>0.8909787602806194</v>
+      </c>
+      <c r="AL18" s="42">
+        <v>159</v>
+      </c>
+      <c r="AM18" s="38">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN18" s="27">
+        <v>0.21990000000000001</v>
+      </c>
+      <c r="AO18" s="134">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="AP18" s="40">
+        <f>AL18*(1-AM18)*AN18</f>
+        <v>31.992151500000006</v>
+      </c>
+      <c r="AQ18" s="135">
+        <f t="shared" si="109"/>
+        <v>31.686633</v>
+      </c>
+      <c r="AR18" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS18" s="17"/>
+      <c r="AT18" s="110">
+        <f>AT17+AL18-AS18</f>
+        <v>2029.68</v>
+      </c>
+      <c r="AU18" s="101"/>
+      <c r="AV18" s="42"/>
+      <c r="AW18" s="47"/>
+      <c r="AX18" s="40"/>
+      <c r="AY18" s="40"/>
+      <c r="AZ18" s="40"/>
+      <c r="BA18" s="40"/>
+    </row>
+    <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="185"/>
+      <c r="B19" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50">
+        <f t="shared" ref="D19" si="110">SUM(D16:D18)</f>
+        <v>44250</v>
+      </c>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50">
+        <f t="shared" ref="F19" si="111">SUM(F16:F18)</f>
+        <v>45483</v>
+      </c>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="50">
+        <f t="shared" ref="I19:K19" si="112">SUM(I16:I18)</f>
+        <v>44934</v>
+      </c>
+      <c r="J19" s="51"/>
+      <c r="K19" s="50">
+        <f t="shared" si="112"/>
+        <v>47394</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" ref="L19" si="113">IF(K19&gt;0,(K16*L16+K17*L17+K18*L18)/K19,0)</f>
+        <v>5.8639363632527322E-2</v>
+      </c>
+      <c r="M19" s="51">
+        <f t="shared" ref="M19" si="114">M16+M17+M18</f>
+        <v>44615</v>
+      </c>
+      <c r="N19" s="52">
+        <f t="shared" ref="N19" si="115">IF(M19&gt;0,O19/M19,0)</f>
+        <v>0.59481017594979269</v>
+      </c>
+      <c r="O19" s="53">
+        <f t="shared" ref="O19" si="116">O16+O17+O18</f>
+        <v>26537.456000000002</v>
+      </c>
+      <c r="P19" s="20">
+        <f t="shared" ref="P19" si="117">IF(M19&gt;0,Q19/M19,0)</f>
+        <v>0.36310225260562595</v>
+      </c>
+      <c r="Q19" s="53">
+        <f t="shared" ref="Q19" si="118">Q16+Q17+Q18</f>
+        <v>16199.807000000001</v>
+      </c>
+      <c r="R19" s="20">
+        <f t="shared" ref="R19" si="119">IF(M19&gt;0,T19/M19,0)</f>
+        <v>4.2087571444581418E-2</v>
+      </c>
+      <c r="S19" s="136"/>
+      <c r="T19" s="53">
+        <f t="shared" ref="T19" si="120">T16+T17+T18</f>
+        <v>1877.7370000000001</v>
+      </c>
+      <c r="U19" s="20">
+        <f t="shared" ref="U19" si="121">IF(M19&gt;0,V19/M19,0)</f>
+        <v>0.19876308416451868</v>
+      </c>
+      <c r="V19" s="53">
+        <f t="shared" ref="V19" si="122">V16+V17+V18</f>
+        <v>8867.8150000000005</v>
+      </c>
+      <c r="W19" s="20">
+        <f t="shared" ref="W19" si="123">IF(M19&gt;0,X19/M19,0)</f>
+        <v>0.50117866188501625</v>
+      </c>
+      <c r="X19" s="53">
+        <f t="shared" ref="X19" si="124">X16+X17+X18</f>
+        <v>22360.085999999999</v>
+      </c>
+      <c r="Y19" s="20">
+        <f t="shared" ref="Y19" si="125">IF(M19&gt;0,Z19/M19,0)</f>
+        <v>0.40328633867533348</v>
+      </c>
+      <c r="Z19" s="53">
+        <f t="shared" ref="Z19" si="126">Z16+Z17+Z18</f>
+        <v>17992.620000000003</v>
+      </c>
+      <c r="AA19" s="152">
+        <f>IF(M19&gt;0,AB19/M19,0)</f>
+        <v>2.3708017482909332E-3</v>
+      </c>
+      <c r="AB19" s="55">
+        <f t="shared" ref="AB19" si="127">SUM(AB16:AB18)</f>
+        <v>105.77331999999998</v>
+      </c>
+      <c r="AC19" s="54">
+        <f t="shared" ref="AC19" si="128">IF(M19&gt;0,AD19/M19,0)</f>
+        <v>2.3166695057716016E-3</v>
+      </c>
+      <c r="AD19" s="55">
+        <f t="shared" ref="AD19" si="129">SUM(AD16:AD18)</f>
+        <v>103.35821</v>
+      </c>
+      <c r="AE19" s="54">
+        <f t="shared" ref="AE19" si="130">IF(M19&gt;0,(AE16*M16+AE17*M17+AE18*M18)/M19,0)</f>
+        <v>2.4325383010198364E-3</v>
+      </c>
+      <c r="AF19" s="54">
+        <f t="shared" ref="AF19" si="131">IF(K19&gt;0,(K16*AF16+K17*AF17+K18*AF18)/K19,0)</f>
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG19" s="51">
+        <f t="shared" ref="AG19" si="132">SUM(AG16:AG18)</f>
+        <v>12.046049999999999</v>
+      </c>
+      <c r="AH19" s="52">
+        <f t="shared" ref="AH19" si="133">IF(K19&gt;0,(K16*AH16+K17*AH17+K18*AH18)/K19,0)</f>
+        <v>0.21083087943621556</v>
+      </c>
+      <c r="AI19" s="57">
+        <f t="shared" ref="AI19" si="134">SUM(AI16:AI18)</f>
+        <v>94.036553300000008</v>
+      </c>
+      <c r="AJ19" s="52">
+        <f t="shared" ref="AJ19" si="135">IF(AND(AD19&gt;0),((AD16*AJ16+AD17*AJ17+AD18*AJ18)/AD19),0)</f>
+        <v>0.88458635726594947</v>
+      </c>
+      <c r="AK19" s="56">
+        <f t="shared" si="6"/>
+        <v>0.89011594355178614</v>
+      </c>
+      <c r="AL19" s="50">
+        <f t="shared" ref="AL19" si="136">SUM(AL16:AL18)</f>
+        <v>488</v>
+      </c>
+      <c r="AM19" s="20">
+        <f t="shared" ref="AM19" si="137">IF(AL19&gt;0,(AM16*AL16+AM17*AL17+AM18*AL18)/AL19,0)</f>
+        <v>8.5995901639344258E-2</v>
+      </c>
+      <c r="AN19" s="52">
+        <f>IF(K19&gt;0,(AN16*K16+AN17*K17+AN18*K18)/K19,0)</f>
+        <v>0.216297879478415</v>
+      </c>
+      <c r="AO19" s="136">
+        <f>IF(K19&gt;0,(AO16*K16+AO17*K17+AO18*K18)/K19,0)</f>
+        <v>0.21620169008735282</v>
+      </c>
+      <c r="AP19" s="57">
+        <f t="shared" ref="AP19" si="138">SUM(AP16:AP18)</f>
+        <v>96.481646300000008</v>
+      </c>
+      <c r="AQ19" s="137">
+        <f t="shared" ref="AQ19:AQ27" si="139">SUM(AQ16:AQ18)</f>
+        <v>96.442346299999997</v>
+      </c>
+      <c r="AR19" s="55"/>
+      <c r="AS19" s="55">
+        <f t="shared" ref="AS19" si="140">SUM(AS16:AS18)</f>
+        <v>1049.24</v>
+      </c>
+      <c r="AT19" s="102"/>
+      <c r="AU19" s="103">
+        <f>AT18</f>
+        <v>2029.68</v>
+      </c>
+      <c r="AV19" s="50">
+        <f t="shared" ref="AV19" si="141">SUM(AV16:AV18)</f>
+        <v>0</v>
+      </c>
+      <c r="AW19" s="58"/>
+      <c r="AX19" s="57"/>
+      <c r="AY19" s="57"/>
+      <c r="AZ19" s="57"/>
+      <c r="BA19" s="57"/>
+    </row>
+    <row r="20" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="183">
+        <v>5</v>
+      </c>
+      <c r="B20" s="22">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="11">
+        <v>5628</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>6232</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="H20" s="12">
+        <v>6</v>
+      </c>
+      <c r="I20" s="11">
+        <v>6261</v>
+      </c>
+      <c r="J20" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="K20" s="11">
+        <v>14699</v>
+      </c>
+      <c r="L20" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M20" s="23">
+        <f>ROUND(K20*(1-L20),0)</f>
+        <v>13670</v>
+      </c>
+      <c r="N20" s="14">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="O20" s="24">
+        <f t="shared" ref="O20:O22" si="142">M20*N20</f>
+        <v>9104.2200000000012</v>
+      </c>
+      <c r="P20" s="13">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="Q20" s="24">
+        <f t="shared" ref="Q20:Q22" si="143">M20*P20</f>
+        <v>4183.0199999999995</v>
+      </c>
+      <c r="R20" s="15">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="S20" s="143">
+        <v>0.1915</v>
+      </c>
+      <c r="T20" s="24">
+        <f t="shared" ref="T20:T22" si="144">M20*R20</f>
+        <v>382.76</v>
+      </c>
+      <c r="U20" s="25">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="V20" s="24">
+        <f t="shared" ref="V20:V22" si="145">M20*U20</f>
+        <v>2665.65</v>
+      </c>
+      <c r="W20" s="15">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="X20" s="24">
+        <f t="shared" ref="X20:X22" si="146">M20*W20</f>
+        <v>7135.7400000000007</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="Z20" s="24">
+        <f t="shared" ref="Z20:Z22" si="147">Y20*M20</f>
+        <v>5468</v>
+      </c>
+      <c r="AA20" s="145">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AB20" s="18">
+        <f t="shared" ref="AB20" si="148">M20*AA20</f>
+        <v>34.174999999999997</v>
+      </c>
+      <c r="AC20" s="16">
+        <v>2.3900000000000002E-3</v>
+      </c>
+      <c r="AD20" s="17">
+        <f t="shared" ref="AD20:AD22" si="149">M20*AC20</f>
+        <v>32.671300000000002</v>
+      </c>
+      <c r="AE20" s="26">
+        <f>IF(M20&gt;0,(AG20+AP20)/M20,0)</f>
+        <v>2.4940054864667155E-3</v>
+      </c>
+      <c r="AF20" s="16">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="AG20" s="23">
+        <f t="shared" ref="AG20:AG22" si="150">AF20*M20</f>
+        <v>3.8275999999999994</v>
+      </c>
+      <c r="AH20" s="114">
+        <v>0.2132</v>
+      </c>
+      <c r="AI20" s="29">
+        <f t="shared" ref="AI20:AI22" si="151">AL20*(1-AM20)*AH20</f>
+        <v>30.237090000000002</v>
+      </c>
+      <c r="AJ20" s="27">
+        <f t="shared" ref="AJ20:AJ22" si="152">IF(AND(AH20&gt;0,AF20&gt;0,AC20&gt;0),((AC20-AF20)*AH20)/((AH20-AF20)*AC20),0)</f>
+        <v>0.88400617200009135</v>
+      </c>
+      <c r="AK20" s="59">
+        <f t="shared" si="6"/>
+        <v>0.88889711329361265</v>
+      </c>
+      <c r="AL20" s="11">
+        <v>155</v>
+      </c>
+      <c r="AM20" s="13">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN20" s="14">
+        <v>0.21340000000000001</v>
+      </c>
+      <c r="AO20" s="130">
+        <v>0.21160000000000001</v>
+      </c>
+      <c r="AP20" s="29">
+        <f>AL20*(1-AM20)*AN20</f>
+        <v>30.265455000000003</v>
+      </c>
+      <c r="AQ20" s="131">
+        <f t="shared" ref="AQ20" si="153">AL20*(1-AM20)*AO20</f>
+        <v>30.010170000000006</v>
+      </c>
+      <c r="AR20" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="AS20" s="18">
+        <v>1009.52</v>
+      </c>
+      <c r="AT20" s="98">
+        <f>AT18+AL20-AS20</f>
+        <v>1175.1600000000003</v>
+      </c>
+      <c r="AU20" s="99"/>
+      <c r="AV20" s="11"/>
+      <c r="AW20" s="30"/>
+      <c r="AX20" s="19"/>
+      <c r="AY20" s="19"/>
+      <c r="AZ20" s="19"/>
+      <c r="BA20" s="19"/>
+    </row>
+    <row r="21" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="184"/>
+      <c r="B21" s="32">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="33">
+        <v>20800</v>
+      </c>
+      <c r="E21" s="33">
+        <v>2</v>
+      </c>
+      <c r="F21" s="33">
+        <v>19506</v>
+      </c>
+      <c r="G21" s="34">
+        <v>1</v>
+      </c>
+      <c r="H21" s="34">
+        <v>9.1</v>
+      </c>
+      <c r="I21" s="33">
+        <v>18803</v>
+      </c>
+      <c r="J21" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="K21" s="33">
+        <v>14484</v>
+      </c>
+      <c r="L21" s="35">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M21" s="36">
+        <f>ROUND(K21*(1-L21),0)</f>
+        <v>13600</v>
+      </c>
+      <c r="N21" s="37">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="O21" s="24">
+        <f t="shared" si="142"/>
+        <v>9479.1999999999989</v>
+      </c>
+      <c r="P21" s="35">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="Q21" s="24">
+        <f t="shared" si="143"/>
+        <v>3196</v>
+      </c>
+      <c r="R21" s="38">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="S21" s="134">
+        <v>0.18909999999999999</v>
+      </c>
+      <c r="T21" s="24">
+        <f t="shared" si="144"/>
+        <v>924.80000000000007</v>
+      </c>
+      <c r="U21" s="27">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="V21" s="24">
+        <f t="shared" si="145"/>
+        <v>2747.2000000000003</v>
+      </c>
+      <c r="W21" s="38">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="X21" s="24">
+        <f t="shared" si="146"/>
+        <v>7099.2</v>
+      </c>
+      <c r="Y21" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z21" s="24">
+        <f t="shared" si="147"/>
+        <v>5576</v>
+      </c>
+      <c r="AA21" s="146">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="AB21" s="18">
+        <f t="shared" si="104"/>
+        <v>33.183999999999997</v>
+      </c>
+      <c r="AC21" s="39">
+        <v>2.4099999999999998E-3</v>
+      </c>
+      <c r="AD21" s="17">
+        <f t="shared" si="149"/>
+        <v>32.775999999999996</v>
+      </c>
+      <c r="AE21" s="26">
+        <f>IF(M21&gt;0,(AG21+AP21)/M21,0)</f>
+        <v>2.5449681250000003E-3</v>
+      </c>
+      <c r="AF21" s="39">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="AG21" s="36">
+        <f t="shared" si="150"/>
+        <v>3.8079999999999998</v>
+      </c>
+      <c r="AH21" s="27">
+        <v>0.20569999999999999</v>
+      </c>
+      <c r="AI21" s="40">
+        <f t="shared" si="151"/>
+        <v>30.302695499999999</v>
+      </c>
+      <c r="AJ21" s="27">
+        <f t="shared" si="152"/>
+        <v>0.88502212449263951</v>
+      </c>
+      <c r="AK21" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89117231976138456</v>
+      </c>
+      <c r="AL21" s="33">
+        <v>161</v>
+      </c>
+      <c r="AM21" s="35">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN21" s="37">
+        <v>0.20910000000000001</v>
+      </c>
+      <c r="AO21" s="132">
+        <v>0.2077</v>
+      </c>
+      <c r="AP21" s="40">
+        <f>AL21*(1-AM21)*AN21</f>
+        <v>30.803566500000002</v>
+      </c>
+      <c r="AQ21" s="133">
+        <f t="shared" si="109"/>
+        <v>30.5973255</v>
+      </c>
+      <c r="AR21" s="41">
+        <v>1.55</v>
+      </c>
+      <c r="AS21" s="41"/>
+      <c r="AT21" s="117">
+        <f>AT20+AL21-AS21</f>
+        <v>1336.1600000000003</v>
+      </c>
+      <c r="AU21" s="101"/>
+      <c r="AV21" s="42"/>
+      <c r="AW21" s="43"/>
+      <c r="AX21" s="44"/>
+      <c r="AY21" s="44"/>
+      <c r="AZ21" s="44"/>
+      <c r="BA21" s="44"/>
+    </row>
+    <row r="22" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="184"/>
+      <c r="B22" s="32">
+        <v>3</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="42">
+        <v>17822</v>
+      </c>
+      <c r="E22" s="42">
+        <v>1</v>
+      </c>
+      <c r="F22" s="42">
+        <v>18635</v>
+      </c>
+      <c r="G22" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H22" s="36">
+        <v>7.2</v>
+      </c>
+      <c r="I22" s="42">
+        <v>18157</v>
+      </c>
+      <c r="J22" s="36">
+        <v>1.3</v>
+      </c>
+      <c r="K22" s="42">
+        <v>14796</v>
+      </c>
+      <c r="L22" s="38">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="M22" s="36">
+        <f>ROUND(K22*(1-L22),0)</f>
+        <v>13731</v>
+      </c>
+      <c r="N22" s="27">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="O22" s="24">
+        <f t="shared" si="142"/>
+        <v>7510.8570000000009</v>
+      </c>
+      <c r="P22" s="38">
+        <v>0.435</v>
+      </c>
+      <c r="Q22" s="24">
+        <f t="shared" si="143"/>
+        <v>5972.9849999999997</v>
+      </c>
+      <c r="R22" s="38">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="S22" s="134">
+        <v>0.1835</v>
+      </c>
+      <c r="T22" s="24">
+        <f t="shared" si="144"/>
+        <v>247.15799999999999</v>
+      </c>
+      <c r="U22" s="27">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="V22" s="24">
+        <f t="shared" si="145"/>
+        <v>2787.393</v>
+      </c>
+      <c r="W22" s="38">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="X22" s="24">
+        <f t="shared" si="146"/>
+        <v>7249.9680000000008</v>
+      </c>
+      <c r="Y22" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z22" s="24">
+        <f t="shared" si="147"/>
+        <v>5629.71</v>
+      </c>
+      <c r="AA22" s="147">
+        <v>2.4299999999999999E-3</v>
+      </c>
+      <c r="AB22" s="148">
+        <f t="shared" si="104"/>
+        <v>33.366329999999998</v>
+      </c>
+      <c r="AC22" s="46">
+        <v>2.5200000000000001E-3</v>
+      </c>
+      <c r="AD22" s="17">
+        <f t="shared" si="149"/>
+        <v>34.602119999999999</v>
+      </c>
+      <c r="AE22" s="26">
+        <f>IF(M22&gt;0,(AG22+AP22)/M22,0)</f>
+        <v>2.483840106328745E-3</v>
+      </c>
+      <c r="AF22" s="46">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="AG22" s="36">
+        <f t="shared" si="150"/>
+        <v>3.8446799999999999</v>
+      </c>
+      <c r="AH22" s="27">
+        <v>0.2135</v>
+      </c>
+      <c r="AI22" s="40">
+        <f t="shared" si="151"/>
+        <v>29.433750499999999</v>
+      </c>
+      <c r="AJ22" s="27">
+        <f t="shared" si="152"/>
+        <v>0.89005617567666162</v>
+      </c>
+      <c r="AK22" s="28">
+        <f t="shared" si="6"/>
+        <v>0.8884045990314372</v>
+      </c>
+      <c r="AL22" s="42">
+        <v>151</v>
+      </c>
+      <c r="AM22" s="38">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="AN22" s="27">
+        <v>0.2195</v>
+      </c>
+      <c r="AO22" s="134">
+        <v>0.2135</v>
+      </c>
+      <c r="AP22" s="40">
+        <f>AL22*(1-AM22)*AN22</f>
+        <v>30.260928499999999</v>
+      </c>
+      <c r="AQ22" s="135">
+        <f t="shared" si="109"/>
+        <v>29.433750499999999</v>
+      </c>
+      <c r="AR22" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS22" s="17"/>
+      <c r="AT22" s="117">
+        <f>AT21+AL22-AS22</f>
+        <v>1487.1600000000003</v>
+      </c>
+      <c r="AU22" s="101"/>
+      <c r="AV22" s="42"/>
+      <c r="AW22" s="47"/>
+      <c r="AX22" s="40"/>
+      <c r="AY22" s="40"/>
+      <c r="AZ22" s="40"/>
+      <c r="BA22" s="40"/>
+    </row>
+    <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="185"/>
+      <c r="B23" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50">
+        <f t="shared" ref="D23" si="154">SUM(D20:D22)</f>
+        <v>44250</v>
+      </c>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50">
+        <f t="shared" ref="F23" si="155">SUM(F20:F22)</f>
+        <v>44373</v>
+      </c>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="50">
+        <f t="shared" ref="I23:K23" si="156">SUM(I20:I22)</f>
+        <v>43221</v>
+      </c>
+      <c r="J23" s="51"/>
+      <c r="K23" s="50">
+        <f t="shared" si="156"/>
+        <v>43979</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" ref="L23" si="157">IF(K23&gt;0,(K20*L20+K21*L21+K22*L22)/K23,0)</f>
+        <v>6.7708815571068018E-2</v>
+      </c>
+      <c r="M23" s="51">
+        <f t="shared" ref="M23" si="158">M20+M21+M22</f>
+        <v>41001</v>
+      </c>
+      <c r="N23" s="52">
+        <f t="shared" ref="N23" si="159">IF(M23&gt;0,O23/M23,0)</f>
+        <v>0.63643025779859019</v>
+      </c>
+      <c r="O23" s="53">
+        <f t="shared" ref="O23" si="160">O20+O21+O22</f>
+        <v>26094.276999999998</v>
+      </c>
+      <c r="P23" s="20">
+        <f t="shared" ref="P23" si="161">IF(M23&gt;0,Q23/M23,0)</f>
+        <v>0.32565071583619909</v>
+      </c>
+      <c r="Q23" s="53">
+        <f t="shared" ref="Q23" si="162">Q20+Q21+Q22</f>
+        <v>13352.004999999999</v>
+      </c>
+      <c r="R23" s="20">
+        <f t="shared" ref="R23" si="163">IF(M23&gt;0,T23/M23,0)</f>
+        <v>3.7919026365210599E-2</v>
+      </c>
+      <c r="S23" s="136"/>
+      <c r="T23" s="53">
+        <f t="shared" ref="T23" si="164">T20+T21+T22</f>
+        <v>1554.7179999999998</v>
+      </c>
+      <c r="U23" s="20">
+        <f t="shared" ref="U23" si="165">IF(M23&gt;0,V23/M23,0)</f>
+        <v>0.20000104875490843</v>
+      </c>
+      <c r="V23" s="53">
+        <f t="shared" ref="V23" si="166">V20+V21+V22</f>
+        <v>8200.2430000000004</v>
+      </c>
+      <c r="W23" s="20">
+        <f t="shared" ref="W23" si="167">IF(M23&gt;0,X23/M23,0)</f>
+        <v>0.52400936562522871</v>
+      </c>
+      <c r="X23" s="53">
+        <f t="shared" ref="X23" si="168">X20+X21+X22</f>
+        <v>21484.908000000003</v>
+      </c>
+      <c r="Y23" s="20">
+        <f t="shared" ref="Y23" si="169">IF(M23&gt;0,Z23/M23,0)</f>
+        <v>0.40666593497719566</v>
+      </c>
+      <c r="Z23" s="53">
+        <f t="shared" ref="Z23" si="170">Z20+Z21+Z22</f>
+        <v>16673.71</v>
+      </c>
+      <c r="AA23" s="152">
+        <f>IF(M23&gt;0,AB23/M23,0)</f>
+        <v>2.4566554474281114E-3</v>
+      </c>
+      <c r="AB23" s="55">
+        <f t="shared" ref="AB23" si="171">SUM(AB20:AB22)</f>
+        <v>100.72532999999999</v>
+      </c>
+      <c r="AC23" s="54">
+        <f t="shared" ref="AC23" si="172">IF(M23&gt;0,AD23/M23,0)</f>
+        <v>2.4401702397502498E-3</v>
+      </c>
+      <c r="AD23" s="55">
+        <f t="shared" ref="AD23" si="173">SUM(AD20:AD22)</f>
+        <v>100.04942</v>
+      </c>
+      <c r="AE23" s="54">
+        <f t="shared" ref="AE23" si="174">IF(M23&gt;0,(AE20*M20+AE21*M21+AE22*M22)/M23,0)</f>
+        <v>2.5075054266969097E-3</v>
+      </c>
+      <c r="AF23" s="54">
+        <f t="shared" ref="AF23" si="175">IF(K23&gt;0,(K20*AF20+K21*AF21+K22*AF22)/K23,0)</f>
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="AG23" s="51">
+        <f t="shared" ref="AG23" si="176">SUM(AG20:AG22)</f>
+        <v>11.480279999999999</v>
+      </c>
+      <c r="AH23" s="52">
+        <f t="shared" ref="AH23" si="177">IF(K23&gt;0,(K20*AH20+K21*AH21+K22*AH22)/K23,0)</f>
+        <v>0.21083088746901932</v>
+      </c>
+      <c r="AI23" s="57">
+        <f t="shared" ref="AI23" si="178">SUM(AI20:AI22)</f>
+        <v>89.973535999999996</v>
+      </c>
+      <c r="AJ23" s="52">
+        <f t="shared" ref="AJ23" si="179">IF(AND(AD23&gt;0),((AD20*AJ20+AD21*AJ21+AD22*AJ22)/AD23),0)</f>
+        <v>0.8864313915777049</v>
+      </c>
+      <c r="AK23" s="56">
+        <f t="shared" si="6"/>
+        <v>0.8894988707605691</v>
+      </c>
+      <c r="AL23" s="50">
+        <f t="shared" ref="AL23" si="180">SUM(AL20:AL22)</f>
+        <v>467</v>
+      </c>
+      <c r="AM23" s="20">
+        <f t="shared" ref="AM23" si="181">IF(AL23&gt;0,(AM20*AL20+AM21*AL21+AM22*AL22)/AL23,0)</f>
+        <v>8.5646680942184153E-2</v>
+      </c>
+      <c r="AN23" s="52">
+        <f>IF(K23&gt;0,(AN20*K20+AN21*K21+AN22*K22)/K23,0)</f>
+        <v>0.21403608540439756</v>
+      </c>
+      <c r="AO23" s="136">
+        <f>IF(K23&gt;0,(AO20*K20+AO21*K21+AO22*K22)/K23,0)</f>
+        <v>0.21095480115509677</v>
+      </c>
+      <c r="AP23" s="57">
+        <f t="shared" ref="AP23" si="182">SUM(AP20:AP22)</f>
+        <v>91.329949999999997</v>
+      </c>
+      <c r="AQ23" s="137">
+        <f t="shared" si="139"/>
+        <v>90.041246000000001</v>
+      </c>
+      <c r="AR23" s="55"/>
+      <c r="AS23" s="55">
+        <f t="shared" ref="AS23" si="183">SUM(AS20:AS22)</f>
+        <v>1009.52</v>
+      </c>
+      <c r="AT23" s="102"/>
+      <c r="AU23" s="103">
+        <f>AT22</f>
+        <v>1487.1600000000003</v>
+      </c>
+      <c r="AV23" s="50">
+        <f t="shared" ref="AV23" si="184">SUM(AV20:AV22)</f>
+        <v>0</v>
+      </c>
+      <c r="AW23" s="58"/>
+      <c r="AX23" s="57"/>
+      <c r="AY23" s="57"/>
+      <c r="AZ23" s="57"/>
+      <c r="BA23" s="57"/>
+    </row>
+    <row r="24" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="183">
+        <v>6</v>
+      </c>
+      <c r="B24" s="22">
+        <v>1</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="11">
+        <v>3003</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <v>6116</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="H24" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="I24" s="11">
+        <v>6113</v>
+      </c>
+      <c r="J24" s="12">
+        <v>5.4</v>
+      </c>
+      <c r="K24" s="11">
+        <v>14834</v>
+      </c>
+      <c r="L24" s="13">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M24" s="23">
+        <f>ROUND(K24*(1-L24),0)</f>
+        <v>13885</v>
+      </c>
+      <c r="N24" s="14">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="O24" s="24">
+        <f t="shared" ref="O24:O26" si="185">M24*N24</f>
+        <v>8206.0349999999999</v>
+      </c>
+      <c r="P24" s="13">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="Q24" s="24">
+        <f t="shared" ref="Q24:Q26" si="186">M24*P24</f>
+        <v>4818.0949999999993</v>
+      </c>
+      <c r="R24" s="15">
+        <v>6.2E-2</v>
+      </c>
+      <c r="S24" s="143">
+        <v>0.19789999999999999</v>
+      </c>
+      <c r="T24" s="24">
+        <f t="shared" ref="T24:T26" si="187">M24*R24</f>
+        <v>860.87</v>
+      </c>
+      <c r="U24" s="25">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="V24" s="24">
+        <f t="shared" ref="V24:V26" si="188">M24*U24</f>
+        <v>2846.4249999999997</v>
+      </c>
+      <c r="W24" s="15">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="X24" s="24">
+        <f t="shared" ref="X24:X26" si="189">M24*W24</f>
+        <v>7164.66</v>
+      </c>
+      <c r="Y24" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="Z24" s="24">
+        <f t="shared" ref="Z24:Z26" si="190">Y24*M24</f>
+        <v>5831.7</v>
+      </c>
+      <c r="AA24" s="145">
+        <v>2.5300000000000001E-3</v>
+      </c>
+      <c r="AB24" s="18">
+        <f t="shared" ref="AB24" si="191">M24*AA24</f>
+        <v>35.129049999999999</v>
+      </c>
+      <c r="AC24" s="16">
+        <v>2.5500000000000002E-3</v>
+      </c>
+      <c r="AD24" s="17">
+        <f t="shared" ref="AD24:AD26" si="192">M24*AC24</f>
+        <v>35.406750000000002</v>
+      </c>
+      <c r="AE24" s="26">
+        <f>IF(M24&gt;0,(AG24+AP24)/M24,0)</f>
+        <v>2.6065172488296726E-3</v>
+      </c>
+      <c r="AF24" s="16">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG24" s="23">
+        <f t="shared" ref="AG24:AG26" si="193">AF24*M24</f>
+        <v>3.7489500000000002</v>
+      </c>
+      <c r="AH24" s="114">
+        <v>0.218</v>
+      </c>
+      <c r="AI24" s="29">
+        <f t="shared" ref="AI24:AI26" si="194">AL24*(1-AM24)*AH24</f>
+        <v>32.442542000000003</v>
+      </c>
+      <c r="AJ24" s="27">
+        <f t="shared" ref="AJ24:AJ26" si="195">IF(AND(AH24&gt;0,AF24&gt;0,AC24&gt;0),((AC24-AF24)*AH24)/((AH24-AF24)*AC24),0)</f>
+        <v>0.89522641371801548</v>
+      </c>
+      <c r="AK24" s="59">
+        <f t="shared" si="6"/>
+        <v>0.8975251132871912</v>
+      </c>
+      <c r="AL24" s="11">
+        <v>163</v>
+      </c>
+      <c r="AM24" s="13">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="AN24" s="14">
+        <v>0.218</v>
+      </c>
+      <c r="AO24" s="130">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="AP24" s="29">
+        <f>AL24*(1-AM24)*AN24</f>
+        <v>32.442542000000003</v>
+      </c>
+      <c r="AQ24" s="131">
+        <f t="shared" ref="AQ24" si="196">AL24*(1-AM24)*AO24</f>
+        <v>32.278841100000008</v>
+      </c>
+      <c r="AR24" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="AS24" s="18">
+        <v>1015.94</v>
+      </c>
+      <c r="AT24" s="98">
+        <f>AT22+AL24-AS24</f>
+        <v>634.22000000000025</v>
+      </c>
+      <c r="AU24" s="99"/>
+      <c r="AV24" s="11"/>
+      <c r="AW24" s="30"/>
+      <c r="AX24" s="19"/>
+      <c r="AY24" s="19"/>
+      <c r="AZ24" s="19"/>
+      <c r="BA24" s="19"/>
+    </row>
+    <row r="25" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="184"/>
+      <c r="B25" s="32">
+        <v>2</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="33">
+        <v>18900</v>
+      </c>
+      <c r="E25" s="33">
+        <v>1</v>
+      </c>
+      <c r="F25" s="33">
+        <v>15628</v>
+      </c>
+      <c r="G25" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="H25" s="34">
+        <v>7.3</v>
+      </c>
+      <c r="I25" s="33">
+        <v>15274</v>
+      </c>
+      <c r="J25" s="34">
+        <v>3.6</v>
+      </c>
+      <c r="K25" s="33">
+        <v>14827</v>
+      </c>
+      <c r="L25" s="35">
+        <v>6.2E-2</v>
+      </c>
+      <c r="M25" s="36">
+        <f>ROUND(K25*(1-L25),0)</f>
+        <v>13908</v>
+      </c>
+      <c r="N25" s="37">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="O25" s="24">
+        <f t="shared" si="185"/>
+        <v>9234.9120000000003</v>
+      </c>
+      <c r="P25" s="35">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="Q25" s="24">
+        <f t="shared" si="186"/>
+        <v>3796.8840000000005</v>
+      </c>
+      <c r="R25" s="38">
+        <v>6.3E-2</v>
+      </c>
+      <c r="S25" s="134">
+        <v>0.20619999999999999</v>
+      </c>
+      <c r="T25" s="24">
+        <f t="shared" si="187"/>
+        <v>876.20399999999995</v>
+      </c>
+      <c r="U25" s="27">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="V25" s="24">
+        <f t="shared" si="188"/>
+        <v>2865.0479999999998</v>
+      </c>
+      <c r="W25" s="38">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="X25" s="24">
+        <f t="shared" si="189"/>
+        <v>7176.5280000000002</v>
+      </c>
+      <c r="Y25" s="38">
+        <v>0.42</v>
+      </c>
+      <c r="Z25" s="24">
+        <f t="shared" si="190"/>
+        <v>5841.36</v>
+      </c>
+      <c r="AA25" s="146"/>
+      <c r="AB25" s="18">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="39">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AD25" s="17">
+        <f t="shared" si="192"/>
+        <v>34.770000000000003</v>
+      </c>
+      <c r="AE25" s="26">
+        <f>IF(M25&gt;0,(AG25+AP25)/M25,0)</f>
+        <v>2.5755921052631582E-3</v>
+      </c>
+      <c r="AF25" s="39">
+        <v>2.7E-4</v>
+      </c>
+      <c r="AG25" s="36">
+        <f t="shared" si="193"/>
+        <v>3.7551600000000001</v>
+      </c>
+      <c r="AH25" s="27">
+        <v>0.2072</v>
+      </c>
+      <c r="AI25" s="40">
+        <f t="shared" si="194"/>
+        <v>30.902844000000002</v>
+      </c>
+      <c r="AJ25" s="27">
+        <f t="shared" si="195"/>
+        <v>0.8931638718407191</v>
+      </c>
+      <c r="AK25" s="28">
+        <f t="shared" si="6"/>
+        <v>0.89629531630095682</v>
+      </c>
+      <c r="AL25" s="33">
+        <v>163</v>
+      </c>
+      <c r="AM25" s="35">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN25" s="37">
+        <v>0.215</v>
+      </c>
+      <c r="AO25" s="132"/>
+      <c r="AP25" s="40">
+        <f>AL25*(1-AM25)*AN25</f>
+        <v>32.066175000000001</v>
+      </c>
+      <c r="AQ25" s="133">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="AR25" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="AS25" s="41"/>
+      <c r="AT25" s="117">
+        <f>AT24+AL25-AS25</f>
+        <v>797.22000000000025</v>
+      </c>
+      <c r="AU25" s="101"/>
+      <c r="AV25" s="42"/>
+      <c r="AW25" s="43"/>
+      <c r="AX25" s="44"/>
+      <c r="AY25" s="44"/>
+      <c r="AZ25" s="44"/>
+      <c r="BA25" s="44"/>
+    </row>
+    <row r="26" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="184"/>
+      <c r="B26" s="32">
+        <v>3</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="42">
+        <v>16000</v>
+      </c>
+      <c r="E26" s="42">
+        <v>0</v>
+      </c>
+      <c r="F26" s="42">
+        <v>18490</v>
+      </c>
+      <c r="G26" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="H26" s="36">
+        <v>5.7</v>
+      </c>
+      <c r="I26" s="42">
+        <v>17390</v>
+      </c>
+      <c r="J26" s="36">
+        <v>3</v>
+      </c>
+      <c r="K26" s="42">
+        <v>15540</v>
+      </c>
+      <c r="L26" s="38">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="M26" s="36">
+        <f>ROUND(K26*(1-L26),0)</f>
+        <v>14530</v>
+      </c>
+      <c r="N26" s="27">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="O26" s="24">
+        <f t="shared" si="185"/>
+        <v>10359.89</v>
+      </c>
+      <c r="P26" s="38">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="Q26" s="24">
+        <f t="shared" si="186"/>
+        <v>3864.98</v>
+      </c>
+      <c r="R26" s="38">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="S26" s="134">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="T26" s="24">
+        <f t="shared" si="187"/>
+        <v>305.13</v>
+      </c>
+      <c r="U26" s="27"/>
+      <c r="V26" s="24">
+        <f t="shared" si="188"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="38"/>
+      <c r="X26" s="24">
+        <f t="shared" si="189"/>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="38">
+        <v>0.41</v>
+      </c>
+      <c r="Z26" s="24">
+        <f t="shared" si="190"/>
+        <v>5957.2999999999993</v>
+      </c>
+      <c r="AA26" s="147"/>
+      <c r="AB26" s="148">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="46">
+        <v>2.5899999999999999E-3</v>
+      </c>
+      <c r="AD26" s="17">
+        <f t="shared" si="192"/>
+        <v>37.6327</v>
+      </c>
+      <c r="AE26" s="26">
+        <f>IF(M26&gt;0,(AG26+AP26)/M26,0)</f>
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="AF26" s="46">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="AG26" s="36">
+        <f t="shared" si="193"/>
+        <v>3.7777999999999996</v>
+      </c>
+      <c r="AH26" s="27">
+        <v>0.2094</v>
+      </c>
+      <c r="AI26" s="40">
+        <f t="shared" si="194"/>
+        <v>32.799578400000001</v>
+      </c>
+      <c r="AJ26" s="27">
+        <f t="shared" si="195"/>
+        <v>0.90073228736325239</v>
+      </c>
+      <c r="AK26" s="28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AL26" s="42">
+        <v>171</v>
+      </c>
+      <c r="AM26" s="38">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="134"/>
+      <c r="AP26" s="40">
+        <f>AL26*(1-AM26)*AN26</f>
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="135">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="AR26" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="AS26" s="17"/>
+      <c r="AT26" s="117">
+        <f>AT25+AL26-AS26</f>
+        <v>968.22000000000025</v>
+      </c>
+      <c r="AU26" s="101"/>
+      <c r="AV26" s="42"/>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="40"/>
+      <c r="AY26" s="40"/>
+      <c r="AZ26" s="40"/>
+      <c r="BA26" s="40"/>
+    </row>
+    <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="185"/>
+      <c r="B27" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50">
+        <f t="shared" ref="D27" si="197">SUM(D24:D26)</f>
+        <v>37903</v>
+      </c>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50">
+        <f t="shared" ref="F27" si="198">SUM(F24:F26)</f>
+        <v>40234</v>
+      </c>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="50">
+        <f t="shared" ref="I27:K27" si="199">SUM(I24:I26)</f>
+        <v>38777</v>
+      </c>
+      <c r="J27" s="51"/>
+      <c r="K27" s="50">
+        <f t="shared" si="199"/>
+        <v>45201</v>
+      </c>
+      <c r="L27" s="20">
+        <f t="shared" ref="L27" si="200">IF(K27&gt;0,(K24*L24+K25*L25+K26*L26)/K27,0)</f>
+        <v>6.36877502710117E-2</v>
+      </c>
+      <c r="M27" s="51">
+        <f t="shared" ref="M27" si="201">M24+M25+M26</f>
+        <v>42323</v>
+      </c>
+      <c r="N27" s="52">
+        <f t="shared" ref="N27" si="202">IF(M27&gt;0,O27/M27,0)</f>
+        <v>0.65687302412399873</v>
+      </c>
+      <c r="O27" s="53">
+        <f t="shared" ref="O27" si="203">O24+O25+O26</f>
+        <v>27800.837</v>
+      </c>
+      <c r="P27" s="20">
+        <f t="shared" ref="P27" si="204">IF(M27&gt;0,Q27/M27,0)</f>
+        <v>0.29487415825910257</v>
+      </c>
+      <c r="Q27" s="53">
+        <f t="shared" ref="Q27" si="205">Q24+Q25+Q26</f>
+        <v>12479.958999999999</v>
+      </c>
+      <c r="R27" s="20">
+        <f t="shared" ref="R27" si="206">IF(M27&gt;0,T27/M27,0)</f>
+        <v>4.8252817616898619E-2</v>
+      </c>
+      <c r="S27" s="136"/>
+      <c r="T27" s="53">
+        <f t="shared" ref="T27" si="207">T24+T25+T26</f>
+        <v>2042.2040000000002</v>
+      </c>
+      <c r="U27" s="20">
+        <f t="shared" ref="U27" si="208">IF(M27&gt;0,V27/M27,0)</f>
+        <v>0.13494962549913758</v>
+      </c>
+      <c r="V27" s="53">
+        <f t="shared" ref="V27" si="209">V24+V25+V26</f>
+        <v>5711.473</v>
+      </c>
+      <c r="W27" s="20">
+        <f t="shared" ref="W27" si="210">IF(M27&gt;0,X27/M27,0)</f>
+        <v>0.33885093211728845</v>
+      </c>
+      <c r="X27" s="53">
+        <f t="shared" ref="X27" si="211">X24+X25+X26</f>
+        <v>14341.188</v>
+      </c>
+      <c r="Y27" s="20">
+        <f t="shared" ref="Y27" si="212">IF(M27&gt;0,Z27/M27,0)</f>
+        <v>0.41656687852940483</v>
+      </c>
+      <c r="Z27" s="53">
+        <f t="shared" ref="Z27" si="213">Z24+Z25+Z26</f>
+        <v>17630.36</v>
+      </c>
+      <c r="AA27" s="152">
+        <f>IF(M27&gt;0,AB27/M27,0)</f>
+        <v>8.3002268270207687E-4</v>
+      </c>
+      <c r="AB27" s="55">
+        <f t="shared" ref="AB27" si="214">SUM(AB24:AB26)</f>
+        <v>35.129049999999999</v>
+      </c>
+      <c r="AC27" s="54">
+        <f t="shared" ref="AC27" si="215">IF(M27&gt;0,AD27/M27,0)</f>
+        <v>2.5473017035654373E-3</v>
+      </c>
+      <c r="AD27" s="55">
+        <f t="shared" ref="AD27" si="216">SUM(AD24:AD26)</f>
+        <v>107.80945</v>
+      </c>
+      <c r="AE27" s="54">
+        <f t="shared" ref="AE27" si="217">IF(M27&gt;0,(AE24*M24+AE25*M25+AE26*M26)/M27,0)</f>
+        <v>1.790766887980531E-3</v>
+      </c>
+      <c r="AF27" s="54">
+        <f t="shared" ref="AF27" si="218">IF(K27&gt;0,(K24*AF24+K25*AF25+K26*AF26)/K27,0)</f>
+        <v>2.6656202296409371E-4</v>
+      </c>
+      <c r="AG27" s="51">
+        <f t="shared" ref="AG27" si="219">SUM(AG24:AG26)</f>
+        <v>11.28191</v>
+      </c>
+      <c r="AH27" s="52">
+        <f t="shared" ref="AH27" si="220">IF(K27&gt;0,(K24*AH24+K25*AH25+K26*AH26)/K27,0)</f>
+        <v>0.21150068361319435</v>
+      </c>
+      <c r="AI27" s="57">
+        <f t="shared" ref="AI27" si="221">SUM(AI24:AI26)</f>
+        <v>96.144964400000006</v>
+      </c>
+      <c r="AJ27" s="52">
+        <f t="shared" ref="AJ27" si="222">IF(AND(AD27&gt;0),((AD24*AJ24+AD25*AJ25+AD26*AJ26)/AD27),0)</f>
+        <v>0.89648313388545464</v>
+      </c>
+      <c r="AK27" s="56">
+        <f t="shared" si="6"/>
+        <v>0.85274644875895866</v>
+      </c>
+      <c r="AL27" s="50">
+        <f t="shared" ref="AL27" si="223">SUM(AL24:AL26)</f>
+        <v>497</v>
+      </c>
+      <c r="AM27" s="20">
+        <f t="shared" ref="AM27" si="224">IF(AL27&gt;0,(AM24*AL24+AM25*AL25+AM26*AL26)/AL27,0)</f>
+        <v>8.5311871227364194E-2</v>
+      </c>
+      <c r="AN27" s="52">
+        <f>IF(K27&gt;0,(AN24*K24+AN25*K25+AN26*K26)/K27,0)</f>
+        <v>0.1420680294683746</v>
+      </c>
+      <c r="AO27" s="136">
+        <f>IF(K27&gt;0,(AO24*K24+AO25*K25+AO26*K26)/K27,0)</f>
+        <v>7.1181934028008223E-2</v>
+      </c>
+      <c r="AP27" s="57">
+        <f t="shared" ref="AP27" si="225">SUM(AP24:AP26)</f>
+        <v>64.508717000000004</v>
+      </c>
+      <c r="AQ27" s="137">
+        <f t="shared" si="139"/>
+        <v>32.278841100000008</v>
+      </c>
+      <c r="AR27" s="55"/>
+      <c r="AS27" s="55">
+        <f t="shared" ref="AS27" si="226">SUM(AS24:AS26)</f>
+        <v>1015.94</v>
+      </c>
+      <c r="AT27" s="102"/>
+      <c r="AU27" s="103">
+        <f>AT26</f>
+        <v>968.22000000000025</v>
+      </c>
+      <c r="AV27" s="50">
+        <f t="shared" ref="AV27" si="227">SUM(AV24:AV26)</f>
+        <v>0</v>
+      </c>
+      <c r="AW27" s="58"/>
+      <c r="AX27" s="57"/>
+      <c r="AY27" s="57"/>
+      <c r="AZ27" s="57"/>
+      <c r="BA27" s="57"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -46123,16 +48074,34 @@
     <protectedRange sqref="AA3:AB3" name="Range1_1_1_1_1_1_1_1_1_1_2"/>
     <protectedRange sqref="AB4:AB15" name="Range1_1_1_1_1_2_2_1_1_1"/>
     <protectedRange sqref="AB1" name="Range1_1_1_1_1_1_1_1_1_1_1_1"/>
+    <protectedRange sqref="AP16:AQ27 AK16:AK27 M16:M27" name="Range1_1_1_1_1_1_1_1_1_1"/>
+    <protectedRange sqref="AH19:AJ19 AH23:AJ23 AH27:AJ27 AH16:AI18 AH20:AI22 AH24:AI26" name="Range1_1_1_1_1_1_1_1"/>
+    <protectedRange sqref="AJ16:AJ18 AJ20:AJ22 AJ24:AJ26" name="Range1_1_1_1_1"/>
+    <protectedRange sqref="AD19:AE19 AD16:AD18 AD23:AE23 AD20:AD22 AD27:AE27 AD24:AD26" name="Range1_1_1_1_1_2_2_1_1"/>
+    <protectedRange sqref="O16:O27" name="Range1_1_1_1_1_5_1_1_1"/>
+    <protectedRange sqref="Q16:Q27" name="Range1_1_1_1_1_7_1_1_1"/>
+    <protectedRange sqref="T16:T27" name="Range1_1_1_1_1_8_1_1_1"/>
+    <protectedRange sqref="V16:V27" name="Range1_1_1_1_1_10_1_1_1"/>
+    <protectedRange sqref="X16:X27" name="Range1_1_1_1_1_12_1_1_1"/>
+    <protectedRange sqref="Z16:Z27" name="Range1_1_1_1_1_16_1_1_1"/>
+    <protectedRange sqref="AG16:AG27" name="Range1_1_1_1_1_18_1_1_1"/>
+    <protectedRange sqref="AE16:AE18" name="Range1_1_1_1_1_2_1_3_1_1_1"/>
+    <protectedRange sqref="AE20:AE22" name="Range1_1_1_1_1_2_1_4_1_1_1"/>
+    <protectedRange sqref="AE24:AE26" name="Range1_1_1_1_1_2_1_5_1_1_1"/>
+    <protectedRange sqref="AB16:AB27" name="Range1_1_1_1_1_2_2_1_1_1_1"/>
   </protectedRanges>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="A4:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
swapping of key/val for self.sql_tags
</commit_message>
<xml_diff>
--- a/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
+++ b/dispatchers_rep/Doklad_Dispecheri_2025!.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E761D1-2FF6-44A8-B593-C2167EBE6562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC8499B-7B68-45A9-94B0-68EE160B5804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,12 +681,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="AU44" authorId="0" shapeId="0" xr:uid="{41A52672-E3F2-47AC-9339-BF8901AF3B67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+корекция на концентрат
+след замер на 
+автомобилна везна</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="70">
   <si>
     <t xml:space="preserve">Подадена руда
  от МГТЛ 
@@ -1763,6 +1789,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1770,6 +1799,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1789,12 +1821,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2214,13 +2240,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -2349,19 +2375,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -2552,7 +2578,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -2714,7 +2740,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -2874,7 +2900,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -3034,7 +3060,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -3205,7 +3231,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -3369,7 +3395,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -3529,7 +3555,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -3689,7 +3715,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -3860,7 +3886,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -4024,7 +4050,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -4184,7 +4210,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -4344,7 +4370,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -4515,7 +4541,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182">
+      <c r="A16" s="183">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -4679,7 +4705,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="183"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -4839,7 +4865,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="183"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -4999,7 +5025,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="184"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -5170,7 +5196,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182">
+      <c r="A20" s="183">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -5334,7 +5360,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="183"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -5494,7 +5520,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="183"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -5654,7 +5680,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="184"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -5825,7 +5851,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182">
+      <c r="A24" s="183">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -5991,7 +6017,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -6151,7 +6177,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="183"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -6311,7 +6337,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
+      <c r="A27" s="185"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -6482,7 +6508,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="182">
+      <c r="A28" s="183">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -6644,7 +6670,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="183"/>
+      <c r="A29" s="184"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -6804,7 +6830,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="183"/>
+      <c r="A30" s="184"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -6964,7 +6990,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="184"/>
+      <c r="A31" s="185"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -7135,7 +7161,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="182">
+      <c r="A32" s="183">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -7297,7 +7323,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="183"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -7457,7 +7483,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="183"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -7617,7 +7643,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="184"/>
+      <c r="A35" s="185"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -7788,7 +7814,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182">
+      <c r="A36" s="183">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -7952,7 +7978,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="183"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -8112,7 +8138,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="183"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -8272,7 +8298,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="184"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -8443,7 +8469,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="182">
+      <c r="A40" s="183">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -8607,7 +8633,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="183"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -8767,7 +8793,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="183"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -8927,7 +8953,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -9098,7 +9124,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="182">
+      <c r="A44" s="183">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -9262,7 +9288,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="183"/>
+      <c r="A45" s="184"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -9422,7 +9448,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="183"/>
+      <c r="A46" s="184"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -9582,7 +9608,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="184"/>
+      <c r="A47" s="185"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -9753,7 +9779,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="182">
+      <c r="A48" s="183">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -9919,7 +9945,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="183"/>
+      <c r="A49" s="184"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -10079,7 +10105,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="183"/>
+      <c r="A50" s="184"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -10239,7 +10265,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
+      <c r="A51" s="185"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -10410,7 +10436,7 @@
       <c r="BA51" s="57"/>
     </row>
     <row r="52" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="182">
+      <c r="A52" s="183">
         <v>13</v>
       </c>
       <c r="B52" s="22">
@@ -10574,7 +10600,7 @@
       <c r="BA52" s="19"/>
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A53" s="183"/>
+      <c r="A53" s="184"/>
       <c r="B53" s="32">
         <v>2</v>
       </c>
@@ -10734,7 +10760,7 @@
       <c r="BA53" s="44"/>
     </row>
     <row r="54" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A54" s="183"/>
+      <c r="A54" s="184"/>
       <c r="B54" s="32">
         <v>3</v>
       </c>
@@ -10894,7 +10920,7 @@
       <c r="BA54" s="40"/>
     </row>
     <row r="55" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="184"/>
+      <c r="A55" s="185"/>
       <c r="B55" s="48" t="s">
         <v>35</v>
       </c>
@@ -11065,7 +11091,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="182">
+      <c r="A56" s="183">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -11227,7 +11253,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="183"/>
+      <c r="A57" s="184"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -11387,7 +11413,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="183"/>
+      <c r="A58" s="184"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -11547,7 +11573,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
+      <c r="A59" s="185"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -11718,7 +11744,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="182">
+      <c r="A60" s="183">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -11880,7 +11906,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="183"/>
+      <c r="A61" s="184"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -12040,7 +12066,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="183"/>
+      <c r="A62" s="184"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -12200,7 +12226,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
+      <c r="A63" s="185"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -12371,7 +12397,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="182">
+      <c r="A64" s="183">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -12535,7 +12561,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="183"/>
+      <c r="A65" s="184"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -12695,7 +12721,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="183"/>
+      <c r="A66" s="184"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -12855,7 +12881,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
+      <c r="A67" s="185"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -13026,7 +13052,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="182">
+      <c r="A68" s="183">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -13190,7 +13216,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="183"/>
+      <c r="A69" s="184"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -13350,7 +13376,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="183"/>
+      <c r="A70" s="184"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -13510,7 +13536,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="184"/>
+      <c r="A71" s="185"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -13681,7 +13707,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="182">
+      <c r="A72" s="183">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -13847,7 +13873,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="183"/>
+      <c r="A73" s="184"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -14007,7 +14033,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="183"/>
+      <c r="A74" s="184"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -14167,7 +14193,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="184"/>
+      <c r="A75" s="185"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -14338,7 +14364,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="182">
+      <c r="A76" s="183">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -14502,7 +14528,7 @@
       <c r="BA76" s="175"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="183"/>
+      <c r="A77" s="184"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -14662,7 +14688,7 @@
       <c r="BA77" s="176"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="183"/>
+      <c r="A78" s="184"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -14822,7 +14848,7 @@
       <c r="BA78" s="177"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="184"/>
+      <c r="A79" s="185"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -14993,7 +15019,7 @@
       <c r="BA79" s="179"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="183">
+      <c r="A80" s="184">
         <v>20</v>
       </c>
       <c r="B80" s="32">
@@ -15159,7 +15185,7 @@
       <c r="BA80" s="168"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="183"/>
+      <c r="A81" s="184"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -15319,7 +15345,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="183"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -15479,7 +15505,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="184"/>
+      <c r="A83" s="185"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -15650,7 +15676,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="182">
+      <c r="A84" s="183">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -15812,7 +15838,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="183"/>
+      <c r="A85" s="184"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -15972,7 +15998,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="183"/>
+      <c r="A86" s="184"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -16132,7 +16158,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="184"/>
+      <c r="A87" s="185"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -16303,7 +16329,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182">
+      <c r="A88" s="183">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -16465,7 +16491,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="183"/>
+      <c r="A89" s="184"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -16625,7 +16651,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="183"/>
+      <c r="A90" s="184"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -16785,7 +16811,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="184"/>
+      <c r="A91" s="185"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -16956,7 +16982,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="182">
+      <c r="A92" s="183">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -17120,7 +17146,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="183"/>
+      <c r="A93" s="184"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -17280,7 +17306,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="183"/>
+      <c r="A94" s="184"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -17440,7 +17466,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="184"/>
+      <c r="A95" s="185"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -17611,7 +17637,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182">
+      <c r="A96" s="183">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -17777,7 +17803,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="183"/>
+      <c r="A97" s="184"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -17937,7 +17963,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="183"/>
+      <c r="A98" s="184"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -18097,7 +18123,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="184"/>
+      <c r="A99" s="185"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -18265,7 +18291,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="192">
+      <c r="A100" s="186">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -18431,7 +18457,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="192"/>
+      <c r="A101" s="186"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -18591,7 +18617,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="192"/>
+      <c r="A102" s="186"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -18751,7 +18777,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="192"/>
+      <c r="A103" s="186"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -18922,7 +18948,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="182">
+      <c r="A104" s="183">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -19088,7 +19114,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="183"/>
+      <c r="A105" s="184"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -19248,7 +19274,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="183"/>
+      <c r="A106" s="184"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -19408,7 +19434,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="184"/>
+      <c r="A107" s="185"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -19579,7 +19605,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="182">
+      <c r="A108" s="183">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -19745,7 +19771,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="183"/>
+      <c r="A109" s="184"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -19905,7 +19931,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="183"/>
+      <c r="A110" s="184"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -20065,7 +20091,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="184"/>
+      <c r="A111" s="185"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -20236,7 +20262,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182">
+      <c r="A112" s="183">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -20398,7 +20424,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="183"/>
+      <c r="A113" s="184"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -20558,7 +20584,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="183"/>
+      <c r="A114" s="184"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -20718,7 +20744,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="184"/>
+      <c r="A115" s="185"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -20889,7 +20915,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="183">
+      <c r="A116" s="184">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -21051,7 +21077,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="183"/>
+      <c r="A117" s="184"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -21211,7 +21237,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="183"/>
+      <c r="A118" s="184"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -21371,7 +21397,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="184"/>
+      <c r="A119" s="185"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -21542,7 +21568,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="182">
+      <c r="A120" s="183">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -21708,7 +21734,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="183"/>
+      <c r="A121" s="184"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -21868,7 +21894,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="183"/>
+      <c r="A122" s="184"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -22028,7 +22054,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
+      <c r="A123" s="185"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -22199,7 +22225,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="182">
+      <c r="A124" s="183">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -22309,7 +22335,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="183"/>
+      <c r="A125" s="184"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -22417,7 +22443,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="183"/>
+      <c r="A126" s="184"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -22525,7 +22551,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
+      <c r="A127" s="185"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -22918,6 +22944,26 @@
     <protectedRange sqref="AB1" name="Range1_1_1_1_1_1_1_1_1_1_1"/>
   </protectedRanges>
   <mergeCells count="36">
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A100:A103"/>
@@ -22934,26 +22980,6 @@
     <mergeCell ref="A68:A71"/>
     <mergeCell ref="A84:A87"/>
     <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23031,13 +23057,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -23166,19 +23192,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -23369,7 +23395,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -23533,7 +23559,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -23692,7 +23718,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -23851,7 +23877,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -24022,7 +24048,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -24186,7 +24212,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -24346,7 +24372,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -24506,7 +24532,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -24677,7 +24703,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -24839,7 +24865,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -24999,7 +25025,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -25159,7 +25185,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -25330,7 +25356,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182">
+      <c r="A16" s="183">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -25492,7 +25518,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="183"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -25652,7 +25678,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="183"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -25812,7 +25838,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="184"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -25983,7 +26009,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182">
+      <c r="A20" s="183">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -26145,7 +26171,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="183"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -26305,7 +26331,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="183"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -26465,7 +26491,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="184"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -26636,7 +26662,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182">
+      <c r="A24" s="183">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -26798,7 +26824,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -26958,7 +26984,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A26" s="183"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -27118,7 +27144,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
+      <c r="A27" s="185"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -27289,7 +27315,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="182">
+      <c r="A28" s="183">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -27453,7 +27479,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A29" s="183"/>
+      <c r="A29" s="184"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -27611,7 +27637,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A30" s="183"/>
+      <c r="A30" s="184"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -27769,7 +27795,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="184"/>
+      <c r="A31" s="185"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -27940,7 +27966,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="182">
+      <c r="A32" s="183">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -28104,7 +28130,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A33" s="183"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -28264,7 +28290,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A34" s="183"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -28424,7 +28450,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="184"/>
+      <c r="A35" s="185"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -28595,7 +28621,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182">
+      <c r="A36" s="183">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -28759,7 +28785,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A37" s="183"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -28919,7 +28945,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A38" s="183"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -29079,7 +29105,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="184"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -29250,7 +29276,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="182">
+      <c r="A40" s="183">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -29414,7 +29440,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A41" s="183"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -29570,7 +29596,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A42" s="183"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -29718,7 +29744,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -29889,7 +29915,7 @@
       <c r="BA43" s="57"/>
     </row>
     <row r="44" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="182">
+      <c r="A44" s="183">
         <v>11</v>
       </c>
       <c r="B44" s="22">
@@ -30051,7 +30077,7 @@
       <c r="BA44" s="19"/>
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A45" s="183"/>
+      <c r="A45" s="184"/>
       <c r="B45" s="32">
         <v>2</v>
       </c>
@@ -30211,7 +30237,7 @@
       <c r="BA45" s="44"/>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A46" s="183"/>
+      <c r="A46" s="184"/>
       <c r="B46" s="32">
         <v>3</v>
       </c>
@@ -30371,7 +30397,7 @@
       <c r="BA46" s="40"/>
     </row>
     <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="184"/>
+      <c r="A47" s="185"/>
       <c r="B47" s="48" t="s">
         <v>35</v>
       </c>
@@ -30542,7 +30568,7 @@
       <c r="BA47" s="57"/>
     </row>
     <row r="48" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="182">
+      <c r="A48" s="183">
         <v>12</v>
       </c>
       <c r="B48" s="22">
@@ -30704,7 +30730,7 @@
       <c r="BA48" s="19"/>
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A49" s="183"/>
+      <c r="A49" s="184"/>
       <c r="B49" s="32">
         <v>2</v>
       </c>
@@ -30864,7 +30890,7 @@
       <c r="BA49" s="44"/>
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A50" s="183"/>
+      <c r="A50" s="184"/>
       <c r="B50" s="32">
         <v>3</v>
       </c>
@@ -31024,7 +31050,7 @@
       <c r="BA50" s="40"/>
     </row>
     <row r="51" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
+      <c r="A51" s="185"/>
       <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
@@ -31829,7 +31855,7 @@
       <c r="BA55" s="57"/>
     </row>
     <row r="56" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="182">
+      <c r="A56" s="183">
         <v>14</v>
       </c>
       <c r="B56" s="22">
@@ -31993,7 +32019,7 @@
       <c r="BA56" s="19"/>
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A57" s="183"/>
+      <c r="A57" s="184"/>
       <c r="B57" s="32">
         <v>2</v>
       </c>
@@ -32153,7 +32179,7 @@
       <c r="BA57" s="44"/>
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A58" s="183"/>
+      <c r="A58" s="184"/>
       <c r="B58" s="32">
         <v>3</v>
       </c>
@@ -32313,7 +32339,7 @@
       <c r="BA58" s="40"/>
     </row>
     <row r="59" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
+      <c r="A59" s="185"/>
       <c r="B59" s="48" t="s">
         <v>35</v>
       </c>
@@ -32484,7 +32510,7 @@
       <c r="BA59" s="57"/>
     </row>
     <row r="60" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="182">
+      <c r="A60" s="183">
         <v>15</v>
       </c>
       <c r="B60" s="22">
@@ -32648,7 +32674,7 @@
       <c r="BA60" s="19"/>
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A61" s="183"/>
+      <c r="A61" s="184"/>
       <c r="B61" s="32">
         <v>2</v>
       </c>
@@ -32808,7 +32834,7 @@
       <c r="BA61" s="44"/>
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A62" s="183"/>
+      <c r="A62" s="184"/>
       <c r="B62" s="32">
         <v>3</v>
       </c>
@@ -32968,7 +32994,7 @@
       <c r="BA62" s="40"/>
     </row>
     <row r="63" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
+      <c r="A63" s="185"/>
       <c r="B63" s="48" t="s">
         <v>35</v>
       </c>
@@ -33139,7 +33165,7 @@
       <c r="BA63" s="57"/>
     </row>
     <row r="64" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="182">
+      <c r="A64" s="183">
         <v>16</v>
       </c>
       <c r="B64" s="22">
@@ -33305,7 +33331,7 @@
       <c r="BA64" s="19"/>
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A65" s="183"/>
+      <c r="A65" s="184"/>
       <c r="B65" s="32">
         <v>2</v>
       </c>
@@ -33465,7 +33491,7 @@
       <c r="BA65" s="44"/>
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A66" s="183"/>
+      <c r="A66" s="184"/>
       <c r="B66" s="32">
         <v>3</v>
       </c>
@@ -33625,7 +33651,7 @@
       <c r="BA66" s="40"/>
     </row>
     <row r="67" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
+      <c r="A67" s="185"/>
       <c r="B67" s="48" t="s">
         <v>35</v>
       </c>
@@ -33796,7 +33822,7 @@
       <c r="BA67" s="57"/>
     </row>
     <row r="68" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="182">
+      <c r="A68" s="183">
         <v>17</v>
       </c>
       <c r="B68" s="22">
@@ -33960,7 +33986,7 @@
       <c r="BA68" s="19"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A69" s="183"/>
+      <c r="A69" s="184"/>
       <c r="B69" s="32">
         <v>2</v>
       </c>
@@ -34120,7 +34146,7 @@
       <c r="BA69" s="44"/>
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A70" s="183"/>
+      <c r="A70" s="184"/>
       <c r="B70" s="32">
         <v>3</v>
       </c>
@@ -34280,7 +34306,7 @@
       <c r="BA70" s="40"/>
     </row>
     <row r="71" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="184"/>
+      <c r="A71" s="185"/>
       <c r="B71" s="48" t="s">
         <v>35</v>
       </c>
@@ -34451,7 +34477,7 @@
       <c r="BA71" s="57"/>
     </row>
     <row r="72" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="182">
+      <c r="A72" s="183">
         <v>18</v>
       </c>
       <c r="B72" s="22">
@@ -34615,7 +34641,7 @@
       <c r="BA72" s="19"/>
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A73" s="183"/>
+      <c r="A73" s="184"/>
       <c r="B73" s="32">
         <v>2</v>
       </c>
@@ -34775,7 +34801,7 @@
       <c r="BA73" s="44"/>
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A74" s="183"/>
+      <c r="A74" s="184"/>
       <c r="B74" s="32">
         <v>3</v>
       </c>
@@ -34935,7 +34961,7 @@
       <c r="BA74" s="40"/>
     </row>
     <row r="75" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="184"/>
+      <c r="A75" s="185"/>
       <c r="B75" s="48" t="s">
         <v>35</v>
       </c>
@@ -35106,7 +35132,7 @@
       <c r="BA75" s="57"/>
     </row>
     <row r="76" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="182">
+      <c r="A76" s="183">
         <v>19</v>
       </c>
       <c r="B76" s="22">
@@ -35268,7 +35294,7 @@
       <c r="BA76" s="19"/>
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A77" s="183"/>
+      <c r="A77" s="184"/>
       <c r="B77" s="32">
         <v>2</v>
       </c>
@@ -35428,7 +35454,7 @@
       <c r="BA77" s="44"/>
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A78" s="183"/>
+      <c r="A78" s="184"/>
       <c r="B78" s="32">
         <v>3</v>
       </c>
@@ -35588,7 +35614,7 @@
       <c r="BA78" s="40"/>
     </row>
     <row r="79" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="184"/>
+      <c r="A79" s="185"/>
       <c r="B79" s="48" t="s">
         <v>35</v>
       </c>
@@ -35759,7 +35785,7 @@
       <c r="BA79" s="57"/>
     </row>
     <row r="80" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="182">
+      <c r="A80" s="183">
         <v>20</v>
       </c>
       <c r="B80" s="22">
@@ -35921,7 +35947,7 @@
       <c r="BA80" s="19"/>
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A81" s="183"/>
+      <c r="A81" s="184"/>
       <c r="B81" s="32">
         <v>2</v>
       </c>
@@ -36081,7 +36107,7 @@
       <c r="BA81" s="44"/>
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A82" s="183"/>
+      <c r="A82" s="184"/>
       <c r="B82" s="32">
         <v>3</v>
       </c>
@@ -36241,7 +36267,7 @@
       <c r="BA82" s="40"/>
     </row>
     <row r="83" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="184"/>
+      <c r="A83" s="185"/>
       <c r="B83" s="48" t="s">
         <v>35</v>
       </c>
@@ -36412,7 +36438,7 @@
       <c r="BA83" s="57"/>
     </row>
     <row r="84" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="182">
+      <c r="A84" s="183">
         <v>21</v>
       </c>
       <c r="B84" s="22">
@@ -36576,7 +36602,7 @@
       <c r="BA84" s="19"/>
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A85" s="183"/>
+      <c r="A85" s="184"/>
       <c r="B85" s="32">
         <v>2</v>
       </c>
@@ -36736,7 +36762,7 @@
       <c r="BA85" s="44"/>
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A86" s="183"/>
+      <c r="A86" s="184"/>
       <c r="B86" s="32">
         <v>3</v>
       </c>
@@ -36896,7 +36922,7 @@
       <c r="BA86" s="40"/>
     </row>
     <row r="87" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="184"/>
+      <c r="A87" s="185"/>
       <c r="B87" s="48" t="s">
         <v>35</v>
       </c>
@@ -37067,7 +37093,7 @@
       <c r="BA87" s="57"/>
     </row>
     <row r="88" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="182">
+      <c r="A88" s="183">
         <v>22</v>
       </c>
       <c r="B88" s="22">
@@ -37231,7 +37257,7 @@
       <c r="BA88" s="19"/>
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A89" s="183"/>
+      <c r="A89" s="184"/>
       <c r="B89" s="32">
         <v>2</v>
       </c>
@@ -37391,7 +37417,7 @@
       <c r="BA89" s="44"/>
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A90" s="183"/>
+      <c r="A90" s="184"/>
       <c r="B90" s="32">
         <v>3</v>
       </c>
@@ -37551,7 +37577,7 @@
       <c r="BA90" s="40"/>
     </row>
     <row r="91" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="184"/>
+      <c r="A91" s="185"/>
       <c r="B91" s="48" t="s">
         <v>35</v>
       </c>
@@ -37722,7 +37748,7 @@
       <c r="BA91" s="57"/>
     </row>
     <row r="92" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="182">
+      <c r="A92" s="183">
         <v>23</v>
       </c>
       <c r="B92" s="22">
@@ -37886,7 +37912,7 @@
       <c r="BA92" s="19"/>
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A93" s="183"/>
+      <c r="A93" s="184"/>
       <c r="B93" s="32">
         <v>2</v>
       </c>
@@ -38044,7 +38070,7 @@
       <c r="BA93" s="44"/>
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A94" s="183"/>
+      <c r="A94" s="184"/>
       <c r="B94" s="32">
         <v>3</v>
       </c>
@@ -38198,7 +38224,7 @@
       <c r="BA94" s="40"/>
     </row>
     <row r="95" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="184"/>
+      <c r="A95" s="185"/>
       <c r="B95" s="48" t="s">
         <v>35</v>
       </c>
@@ -38369,7 +38395,7 @@
       <c r="BA95" s="57"/>
     </row>
     <row r="96" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="182">
+      <c r="A96" s="183">
         <v>24</v>
       </c>
       <c r="B96" s="22">
@@ -38533,7 +38559,7 @@
       <c r="BA96" s="19"/>
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A97" s="183"/>
+      <c r="A97" s="184"/>
       <c r="B97" s="32">
         <v>2</v>
       </c>
@@ -38693,7 +38719,7 @@
       <c r="BA97" s="44"/>
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A98" s="183"/>
+      <c r="A98" s="184"/>
       <c r="B98" s="32">
         <v>3</v>
       </c>
@@ -38853,7 +38879,7 @@
       <c r="BA98" s="40"/>
     </row>
     <row r="99" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="184"/>
+      <c r="A99" s="185"/>
       <c r="B99" s="48" t="s">
         <v>35</v>
       </c>
@@ -39024,7 +39050,7 @@
       <c r="BA99" s="57"/>
     </row>
     <row r="100" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="192">
+      <c r="A100" s="186">
         <v>25</v>
       </c>
       <c r="B100" s="32">
@@ -39188,7 +39214,7 @@
       <c r="BA100" s="19"/>
     </row>
     <row r="101" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A101" s="192"/>
+      <c r="A101" s="186"/>
       <c r="B101" s="32">
         <v>2</v>
       </c>
@@ -39348,7 +39374,7 @@
       <c r="BA101" s="44"/>
     </row>
     <row r="102" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A102" s="192"/>
+      <c r="A102" s="186"/>
       <c r="B102" s="32">
         <v>3</v>
       </c>
@@ -39508,7 +39534,7 @@
       <c r="BA102" s="40"/>
     </row>
     <row r="103" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="192"/>
+      <c r="A103" s="186"/>
       <c r="B103" s="65" t="s">
         <v>35</v>
       </c>
@@ -39679,7 +39705,7 @@
       <c r="BA103" s="57"/>
     </row>
     <row r="104" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="182">
+      <c r="A104" s="183">
         <v>26</v>
       </c>
       <c r="B104" s="22">
@@ -39841,7 +39867,7 @@
       <c r="BA104" s="19"/>
     </row>
     <row r="105" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A105" s="183"/>
+      <c r="A105" s="184"/>
       <c r="B105" s="32">
         <v>2</v>
       </c>
@@ -40001,7 +40027,7 @@
       <c r="BA105" s="44"/>
     </row>
     <row r="106" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A106" s="183"/>
+      <c r="A106" s="184"/>
       <c r="B106" s="32">
         <v>3</v>
       </c>
@@ -40161,7 +40187,7 @@
       <c r="BA106" s="40"/>
     </row>
     <row r="107" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="184"/>
+      <c r="A107" s="185"/>
       <c r="B107" s="48" t="s">
         <v>35</v>
       </c>
@@ -40332,7 +40358,7 @@
       <c r="BA107" s="57"/>
     </row>
     <row r="108" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="182">
+      <c r="A108" s="183">
         <v>27</v>
       </c>
       <c r="B108" s="22">
@@ -40494,7 +40520,7 @@
       <c r="BA108" s="19"/>
     </row>
     <row r="109" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A109" s="183"/>
+      <c r="A109" s="184"/>
       <c r="B109" s="32">
         <v>2</v>
       </c>
@@ -40650,7 +40676,7 @@
       <c r="BA109" s="44"/>
     </row>
     <row r="110" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A110" s="183"/>
+      <c r="A110" s="184"/>
       <c r="B110" s="32">
         <v>3</v>
       </c>
@@ -40800,7 +40826,7 @@
       <c r="BA110" s="40"/>
     </row>
     <row r="111" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="184"/>
+      <c r="A111" s="185"/>
       <c r="B111" s="48" t="s">
         <v>35</v>
       </c>
@@ -40971,7 +40997,7 @@
       <c r="BA111" s="57"/>
     </row>
     <row r="112" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="182">
+      <c r="A112" s="183">
         <v>28</v>
       </c>
       <c r="B112" s="22">
@@ -41135,7 +41161,7 @@
       <c r="BA112" s="19"/>
     </row>
     <row r="113" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A113" s="183"/>
+      <c r="A113" s="184"/>
       <c r="B113" s="32">
         <v>2</v>
       </c>
@@ -41295,7 +41321,7 @@
       <c r="BA113" s="44"/>
     </row>
     <row r="114" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A114" s="183"/>
+      <c r="A114" s="184"/>
       <c r="B114" s="32">
         <v>3</v>
       </c>
@@ -41455,7 +41481,7 @@
       <c r="BA114" s="40"/>
     </row>
     <row r="115" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="184"/>
+      <c r="A115" s="185"/>
       <c r="B115" s="48" t="s">
         <v>35</v>
       </c>
@@ -41626,7 +41652,7 @@
       <c r="BA115" s="57"/>
     </row>
     <row r="116" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="183">
+      <c r="A116" s="184">
         <v>29</v>
       </c>
       <c r="B116" s="32">
@@ -41790,7 +41816,7 @@
       <c r="BA116" s="19"/>
     </row>
     <row r="117" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A117" s="183"/>
+      <c r="A117" s="184"/>
       <c r="B117" s="32">
         <v>2</v>
       </c>
@@ -41950,7 +41976,7 @@
       <c r="BA117" s="44"/>
     </row>
     <row r="118" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A118" s="183"/>
+      <c r="A118" s="184"/>
       <c r="B118" s="32">
         <v>3</v>
       </c>
@@ -42110,7 +42136,7 @@
       <c r="BA118" s="40"/>
     </row>
     <row r="119" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="184"/>
+      <c r="A119" s="185"/>
       <c r="B119" s="48" t="s">
         <v>35</v>
       </c>
@@ -42281,7 +42307,7 @@
       <c r="BA119" s="57"/>
     </row>
     <row r="120" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="182">
+      <c r="A120" s="183">
         <v>30</v>
       </c>
       <c r="B120" s="22">
@@ -42445,7 +42471,7 @@
       <c r="BA120" s="19"/>
     </row>
     <row r="121" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A121" s="183"/>
+      <c r="A121" s="184"/>
       <c r="B121" s="32">
         <v>2</v>
       </c>
@@ -42605,7 +42631,7 @@
       <c r="BA121" s="44"/>
     </row>
     <row r="122" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A122" s="183"/>
+      <c r="A122" s="184"/>
       <c r="B122" s="32">
         <v>3</v>
       </c>
@@ -42765,7 +42791,7 @@
       <c r="BA122" s="40"/>
     </row>
     <row r="123" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="184"/>
+      <c r="A123" s="185"/>
       <c r="B123" s="48" t="s">
         <v>35</v>
       </c>
@@ -42936,7 +42962,7 @@
       <c r="BA123" s="57"/>
     </row>
     <row r="124" spans="1:53" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="182">
+      <c r="A124" s="183">
         <v>31</v>
       </c>
       <c r="B124" s="22">
@@ -43100,7 +43126,7 @@
       <c r="BA124" s="19"/>
     </row>
     <row r="125" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A125" s="183"/>
+      <c r="A125" s="184"/>
       <c r="B125" s="32">
         <v>2</v>
       </c>
@@ -43256,7 +43282,7 @@
       <c r="BA125" s="44"/>
     </row>
     <row r="126" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A126" s="183"/>
+      <c r="A126" s="184"/>
       <c r="B126" s="32">
         <v>3</v>
       </c>
@@ -43406,7 +43432,7 @@
       <c r="BA126" s="40"/>
     </row>
     <row r="127" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="184"/>
+      <c r="A127" s="185"/>
       <c r="B127" s="48" t="s">
         <v>35</v>
       </c>
@@ -43842,18 +43868,16 @@
     <protectedRange sqref="AB112:AB127" name="Range1_1_1_1_1_2_2_1_1_4"/>
   </protectedRanges>
   <mergeCells count="35">
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="A108:A111"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A35"/>
@@ -43867,16 +43891,18 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A124:A127"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="A116:A119"/>
-    <mergeCell ref="A120:A123"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A76:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43886,22 +43912,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6555BB66-49A2-4157-88D4-D9BD7AEDD16F}">
-  <dimension ref="A1:BA43"/>
+  <dimension ref="A1:BA47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:53" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="191" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="187" t="s">
+      <c r="B1" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="185" t="s">
+      <c r="C1" s="187" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="125" t="s">
@@ -44030,19 +44056,19 @@
       <c r="AW1" s="125" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="191" t="s">
+      <c r="AX1" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="AY1" s="191"/>
-      <c r="AZ1" s="191" t="s">
+      <c r="AY1" s="182"/>
+      <c r="AZ1" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BA1" s="191"/>
+      <c r="BA1" s="182"/>
     </row>
     <row r="2" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="190"/>
-      <c r="B2" s="188"/>
-      <c r="C2" s="186"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="188"/>
       <c r="D2" s="5" t="s">
         <v>27</v>
       </c>
@@ -44233,7 +44259,7 @@
       <c r="BA3" s="85"/>
     </row>
     <row r="4" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182">
+      <c r="A4" s="183">
         <v>1</v>
       </c>
       <c r="B4" s="22">
@@ -44355,7 +44381,7 @@
         <v>0.89341832658664044</v>
       </c>
       <c r="AK4" s="59">
-        <f t="shared" ref="AK4:AK43" si="6">IF(AND(AE4&gt;0,AN4&gt;0,AF4&gt;0),((AN4*(AE4-AF4))/(AE4*(AN4-AF4))),0)</f>
+        <f t="shared" ref="AK4:AK47" si="6">IF(AND(AE4&gt;0,AN4&gt;0,AF4&gt;0),((AN4*(AE4-AF4))/(AE4*(AN4-AF4))),0)</f>
         <v>0.89517063729570767</v>
       </c>
       <c r="AL4" s="11">
@@ -44397,7 +44423,7 @@
       <c r="BA4" s="19"/>
     </row>
     <row r="5" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="183"/>
+      <c r="A5" s="184"/>
       <c r="B5" s="32">
         <v>2</v>
       </c>
@@ -44557,7 +44583,7 @@
       <c r="BA5" s="44"/>
     </row>
     <row r="6" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="183"/>
+      <c r="A6" s="184"/>
       <c r="B6" s="32">
         <v>3</v>
       </c>
@@ -44717,7 +44743,7 @@
       <c r="BA6" s="40"/>
     </row>
     <row r="7" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
+      <c r="A7" s="185"/>
       <c r="B7" s="48" t="s">
         <v>35</v>
       </c>
@@ -44888,7 +44914,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182">
+      <c r="A8" s="183">
         <v>2</v>
       </c>
       <c r="B8" s="22">
@@ -45050,7 +45076,7 @@
       <c r="BA8" s="19"/>
     </row>
     <row r="9" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="183"/>
+      <c r="A9" s="184"/>
       <c r="B9" s="32">
         <v>2</v>
       </c>
@@ -45210,7 +45236,7 @@
       <c r="BA9" s="44"/>
     </row>
     <row r="10" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="183"/>
+      <c r="A10" s="184"/>
       <c r="B10" s="32">
         <v>3</v>
       </c>
@@ -45370,7 +45396,7 @@
       <c r="BA10" s="40"/>
     </row>
     <row r="11" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
+      <c r="A11" s="185"/>
       <c r="B11" s="48" t="s">
         <v>35</v>
       </c>
@@ -45541,7 +45567,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182">
+      <c r="A12" s="183">
         <v>3</v>
       </c>
       <c r="B12" s="22">
@@ -45703,7 +45729,7 @@
       <c r="BA12" s="19"/>
     </row>
     <row r="13" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="183"/>
+      <c r="A13" s="184"/>
       <c r="B13" s="32">
         <v>2</v>
       </c>
@@ -45859,7 +45885,7 @@
       <c r="BA13" s="44"/>
     </row>
     <row r="14" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="183"/>
+      <c r="A14" s="184"/>
       <c r="B14" s="32">
         <v>3</v>
       </c>
@@ -46009,7 +46035,7 @@
       <c r="BA14" s="40"/>
     </row>
     <row r="15" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="184"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="48" t="s">
         <v>35</v>
       </c>
@@ -46180,7 +46206,7 @@
       <c r="BA15" s="57"/>
     </row>
     <row r="16" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="182">
+      <c r="A16" s="183">
         <v>4</v>
       </c>
       <c r="B16" s="22">
@@ -46344,7 +46370,7 @@
       <c r="BA16" s="19"/>
     </row>
     <row r="17" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="183"/>
+      <c r="A17" s="184"/>
       <c r="B17" s="32">
         <v>2</v>
       </c>
@@ -46504,7 +46530,7 @@
       <c r="BA17" s="44"/>
     </row>
     <row r="18" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="183"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="32">
         <v>3</v>
       </c>
@@ -46664,7 +46690,7 @@
       <c r="BA18" s="40"/>
     </row>
     <row r="19" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="184"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="48" t="s">
         <v>35</v>
       </c>
@@ -46835,7 +46861,7 @@
       <c r="BA19" s="57"/>
     </row>
     <row r="20" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182">
+      <c r="A20" s="183">
         <v>5</v>
       </c>
       <c r="B20" s="22">
@@ -46999,7 +47025,7 @@
       <c r="BA20" s="19"/>
     </row>
     <row r="21" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="183"/>
+      <c r="A21" s="184"/>
       <c r="B21" s="32">
         <v>2</v>
       </c>
@@ -47159,7 +47185,7 @@
       <c r="BA21" s="44"/>
     </row>
     <row r="22" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="183"/>
+      <c r="A22" s="184"/>
       <c r="B22" s="32">
         <v>3</v>
       </c>
@@ -47319,7 +47345,7 @@
       <c r="BA22" s="40"/>
     </row>
     <row r="23" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="184"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
@@ -47490,7 +47516,7 @@
       <c r="BA23" s="57"/>
     </row>
     <row r="24" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="182">
+      <c r="A24" s="183">
         <v>6</v>
       </c>
       <c r="B24" s="22">
@@ -47654,7 +47680,7 @@
       <c r="BA24" s="19"/>
     </row>
     <row r="25" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="183"/>
+      <c r="A25" s="184"/>
       <c r="B25" s="32">
         <v>2</v>
       </c>
@@ -47810,7 +47836,7 @@
       <c r="BA25" s="44"/>
     </row>
     <row r="26" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="183"/>
+      <c r="A26" s="184"/>
       <c r="B26" s="32">
         <v>3</v>
       </c>
@@ -47960,7 +47986,7 @@
       <c r="BA26" s="40"/>
     </row>
     <row r="27" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
+      <c r="A27" s="185"/>
       <c r="B27" s="48" t="s">
         <v>35</v>
       </c>
@@ -48131,7 +48157,7 @@
       <c r="BA27" s="57"/>
     </row>
     <row r="28" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="182">
+      <c r="A28" s="183">
         <v>7</v>
       </c>
       <c r="B28" s="22">
@@ -48297,7 +48323,7 @@
       <c r="BA28" s="19"/>
     </row>
     <row r="29" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="183"/>
+      <c r="A29" s="184"/>
       <c r="B29" s="32">
         <v>2</v>
       </c>
@@ -48457,7 +48483,7 @@
       <c r="BA29" s="44"/>
     </row>
     <row r="30" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="183"/>
+      <c r="A30" s="184"/>
       <c r="B30" s="32">
         <v>3</v>
       </c>
@@ -48617,7 +48643,7 @@
       <c r="BA30" s="40"/>
     </row>
     <row r="31" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="184"/>
+      <c r="A31" s="185"/>
       <c r="B31" s="48" t="s">
         <v>35</v>
       </c>
@@ -48788,7 +48814,7 @@
       <c r="BA31" s="57"/>
     </row>
     <row r="32" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="182">
+      <c r="A32" s="183">
         <v>8</v>
       </c>
       <c r="B32" s="22">
@@ -48954,7 +48980,7 @@
       <c r="BA32" s="19"/>
     </row>
     <row r="33" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="183"/>
+      <c r="A33" s="184"/>
       <c r="B33" s="32">
         <v>2</v>
       </c>
@@ -49114,7 +49140,7 @@
       <c r="BA33" s="44"/>
     </row>
     <row r="34" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="183"/>
+      <c r="A34" s="184"/>
       <c r="B34" s="32">
         <v>3</v>
       </c>
@@ -49274,7 +49300,7 @@
       <c r="BA34" s="40"/>
     </row>
     <row r="35" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="184"/>
+      <c r="A35" s="185"/>
       <c r="B35" s="48" t="s">
         <v>35</v>
       </c>
@@ -49445,7 +49471,7 @@
       <c r="BA35" s="57"/>
     </row>
     <row r="36" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182">
+      <c r="A36" s="183">
         <v>9</v>
       </c>
       <c r="B36" s="22">
@@ -49607,7 +49633,7 @@
       <c r="BA36" s="19"/>
     </row>
     <row r="37" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="183"/>
+      <c r="A37" s="184"/>
       <c r="B37" s="32">
         <v>2</v>
       </c>
@@ -49767,7 +49793,7 @@
       <c r="BA37" s="44"/>
     </row>
     <row r="38" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="183"/>
+      <c r="A38" s="184"/>
       <c r="B38" s="32">
         <v>3</v>
       </c>
@@ -49927,7 +49953,7 @@
       <c r="BA38" s="40"/>
     </row>
     <row r="39" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="184"/>
+      <c r="A39" s="185"/>
       <c r="B39" s="48" t="s">
         <v>35</v>
       </c>
@@ -50098,7 +50124,7 @@
       <c r="BA39" s="57"/>
     </row>
     <row r="40" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="182">
+      <c r="A40" s="183">
         <v>10</v>
       </c>
       <c r="B40" s="22">
@@ -50260,7 +50286,7 @@
       <c r="BA40" s="19"/>
     </row>
     <row r="41" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="183"/>
+      <c r="A41" s="184"/>
       <c r="B41" s="32">
         <v>2</v>
       </c>
@@ -50416,7 +50442,7 @@
       <c r="BA41" s="44"/>
     </row>
     <row r="42" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="183"/>
+      <c r="A42" s="184"/>
       <c r="B42" s="32">
         <v>3</v>
       </c>
@@ -50566,7 +50592,7 @@
       <c r="BA42" s="40"/>
     </row>
     <row r="43" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
+      <c r="A43" s="185"/>
       <c r="B43" s="48" t="s">
         <v>35</v>
       </c>
@@ -50735,6 +50761,663 @@
       <c r="AY43" s="57"/>
       <c r="AZ43" s="57"/>
       <c r="BA43" s="57"/>
+    </row>
+    <row r="44" spans="1:53" s="31" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="183">
+        <v>11</v>
+      </c>
+      <c r="B44" s="22">
+        <v>1</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="11">
+        <v>3600</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0</v>
+      </c>
+      <c r="F44" s="11">
+        <v>8878</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="H44" s="12">
+        <v>6.9</v>
+      </c>
+      <c r="I44" s="11">
+        <v>9730</v>
+      </c>
+      <c r="J44" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="K44" s="11">
+        <v>16156</v>
+      </c>
+      <c r="L44" s="13">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="M44" s="23">
+        <f>ROUND(K44*(1-L44),0)</f>
+        <v>15090</v>
+      </c>
+      <c r="N44" s="14">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="O44" s="24">
+        <f t="shared" ref="O44:O46" si="405">M44*N44</f>
+        <v>8827.65</v>
+      </c>
+      <c r="P44" s="13">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="Q44" s="24">
+        <f t="shared" ref="Q44:Q46" si="406">M44*P44</f>
+        <v>4149.75</v>
+      </c>
+      <c r="R44" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="S44" s="143">
+        <v>0.2011</v>
+      </c>
+      <c r="T44" s="24">
+        <f t="shared" ref="T44:T46" si="407">M44*R44</f>
+        <v>2112.6000000000004</v>
+      </c>
+      <c r="U44" s="25">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="V44" s="24">
+        <f t="shared" ref="V44:V46" si="408">M44*U44</f>
+        <v>3485.79</v>
+      </c>
+      <c r="W44" s="15">
+        <v>0.503</v>
+      </c>
+      <c r="X44" s="24">
+        <f t="shared" ref="X44:X46" si="409">M44*W44</f>
+        <v>7590.27</v>
+      </c>
+      <c r="Y44" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="Z44" s="24">
+        <f t="shared" ref="Z44:Z46" si="410">Y44*M44</f>
+        <v>6639.6</v>
+      </c>
+      <c r="AA44" s="145">
+        <v>2.4599999999999999E-3</v>
+      </c>
+      <c r="AB44" s="18">
+        <f t="shared" ref="AB44:AB46" si="411">M44*AA44</f>
+        <v>37.121400000000001</v>
+      </c>
+      <c r="AC44" s="16">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="AD44" s="17">
+        <f t="shared" ref="AD44:AD46" si="412">M44*AC44</f>
+        <v>36.215999999999994</v>
+      </c>
+      <c r="AE44" s="26">
+        <f>IF(M44&gt;0,(AG44+AP44)/M44,0)</f>
+        <v>2.5725410205434066E-3</v>
+      </c>
+      <c r="AF44" s="16">
+        <v>3.1E-4</v>
+      </c>
+      <c r="AG44" s="23">
+        <f t="shared" ref="AG44:AG46" si="413">AF44*M44</f>
+        <v>4.6779000000000002</v>
+      </c>
+      <c r="AH44" s="114">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="AI44" s="29">
+        <f t="shared" ref="AI44:AI46" si="414">AL44*(1-AM44)*AH44</f>
+        <v>34.011432000000006</v>
+      </c>
+      <c r="AJ44" s="27">
+        <f t="shared" ref="AJ44:AJ46" si="415">IF(AND(AH44&gt;0,AF44&gt;0,AC44&gt;0),((AC44-AF44)*AH44)/((AH44-AF44)*AC44),0)</f>
+        <v>0.87212815962396284</v>
+      </c>
+      <c r="AK44" s="59">
+        <f t="shared" si="6"/>
+        <v>0.88079928539383623</v>
+      </c>
+      <c r="AL44" s="11">
+        <v>179</v>
+      </c>
+      <c r="AM44" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="AN44" s="14">
+        <v>0.20960000000000001</v>
+      </c>
+      <c r="AO44" s="130">
+        <v>0.2072</v>
+      </c>
+      <c r="AP44" s="29">
+        <f>AL44*(1-AM44)*AN44</f>
+        <v>34.141744000000003</v>
+      </c>
+      <c r="AQ44" s="131">
+        <f t="shared" ref="AQ44:AQ46" si="416">AL44*(1-AM44)*AO44</f>
+        <v>33.750807999999999</v>
+      </c>
+      <c r="AR44" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="AS44" s="18">
+        <v>1018.58</v>
+      </c>
+      <c r="AT44" s="98">
+        <f>AT42+AL44-AS44-AU44</f>
+        <v>642.9000000000002</v>
+      </c>
+      <c r="AU44" s="99">
+        <v>13</v>
+      </c>
+      <c r="AV44" s="11"/>
+      <c r="AW44" s="30"/>
+      <c r="AX44" s="19"/>
+      <c r="AY44" s="19"/>
+      <c r="AZ44" s="19"/>
+      <c r="BA44" s="19"/>
+    </row>
+    <row r="45" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="184"/>
+      <c r="B45" s="32">
+        <v>2</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="33">
+        <v>21700</v>
+      </c>
+      <c r="E45" s="33">
+        <v>3</v>
+      </c>
+      <c r="F45" s="33">
+        <v>17660</v>
+      </c>
+      <c r="G45" s="34">
+        <v>0.9</v>
+      </c>
+      <c r="H45" s="34">
+        <v>10</v>
+      </c>
+      <c r="I45" s="33">
+        <v>17150</v>
+      </c>
+      <c r="J45" s="34">
+        <v>3</v>
+      </c>
+      <c r="K45" s="33">
+        <v>15801</v>
+      </c>
+      <c r="L45" s="35">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M45" s="36">
+        <f>ROUND(K45*(1-L45),0)</f>
+        <v>14695</v>
+      </c>
+      <c r="N45" s="37">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="O45" s="24">
+        <f t="shared" si="405"/>
+        <v>8141.0300000000007</v>
+      </c>
+      <c r="P45" s="35">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="Q45" s="24">
+        <f t="shared" si="406"/>
+        <v>3835.395</v>
+      </c>
+      <c r="R45" s="38">
+        <v>0.185</v>
+      </c>
+      <c r="S45" s="134">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="T45" s="24">
+        <f t="shared" si="407"/>
+        <v>2718.5749999999998</v>
+      </c>
+      <c r="U45" s="27">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="V45" s="24">
+        <f t="shared" si="408"/>
+        <v>3453.3249999999998</v>
+      </c>
+      <c r="W45" s="38">
+        <v>0.499</v>
+      </c>
+      <c r="X45" s="24">
+        <f t="shared" si="409"/>
+        <v>7332.8050000000003</v>
+      </c>
+      <c r="Y45" s="38">
+        <v>0.44</v>
+      </c>
+      <c r="Z45" s="24">
+        <f t="shared" si="410"/>
+        <v>6465.8</v>
+      </c>
+      <c r="AA45" s="146">
+        <v>2.48E-3</v>
+      </c>
+      <c r="AB45" s="18">
+        <f t="shared" si="411"/>
+        <v>36.443600000000004</v>
+      </c>
+      <c r="AC45" s="39">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="AD45" s="17">
+        <f t="shared" si="412"/>
+        <v>35.855799999999995</v>
+      </c>
+      <c r="AE45" s="26">
+        <f>IF(M45&gt;0,(AG45+AP45)/M45,0)</f>
+        <v>2.3899900918679822E-3</v>
+      </c>
+      <c r="AF45" s="39">
+        <v>3.1E-4</v>
+      </c>
+      <c r="AG45" s="36">
+        <f t="shared" si="413"/>
+        <v>4.5554500000000004</v>
+      </c>
+      <c r="AH45" s="27">
+        <v>0.21410000000000001</v>
+      </c>
+      <c r="AI45" s="40">
+        <f t="shared" si="414"/>
+        <v>30.594033600000007</v>
+      </c>
+      <c r="AJ45" s="27">
+        <f t="shared" si="415"/>
+        <v>0.87421661673512929</v>
+      </c>
+      <c r="AK45" s="28">
+        <f t="shared" si="6"/>
+        <v>0.87155547317939197</v>
+      </c>
+      <c r="AL45" s="33">
+        <v>156</v>
+      </c>
+      <c r="AM45" s="35">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AN45" s="37">
+        <v>0.21390000000000001</v>
+      </c>
+      <c r="AO45" s="132">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="AP45" s="40">
+        <f>AL45*(1-AM45)*AN45</f>
+        <v>30.565454400000004</v>
+      </c>
+      <c r="AQ45" s="133">
+        <f t="shared" si="416"/>
+        <v>31.122748800000004</v>
+      </c>
+      <c r="AR45" s="41">
+        <v>1.6</v>
+      </c>
+      <c r="AS45" s="41"/>
+      <c r="AT45" s="117">
+        <f>AT44+AL45-AS45</f>
+        <v>798.9000000000002</v>
+      </c>
+      <c r="AU45" s="101"/>
+      <c r="AV45" s="42"/>
+      <c r="AW45" s="43"/>
+      <c r="AX45" s="44"/>
+      <c r="AY45" s="44"/>
+      <c r="AZ45" s="44"/>
+      <c r="BA45" s="44"/>
+    </row>
+    <row r="46" spans="1:53" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="184"/>
+      <c r="B46" s="32">
+        <v>3</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="42">
+        <v>17670</v>
+      </c>
+      <c r="E46" s="42">
+        <v>1</v>
+      </c>
+      <c r="F46" s="42">
+        <v>19268</v>
+      </c>
+      <c r="G46" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="H46" s="36">
+        <v>9</v>
+      </c>
+      <c r="I46" s="42">
+        <v>19282</v>
+      </c>
+      <c r="J46" s="36">
+        <v>1.6</v>
+      </c>
+      <c r="K46" s="42">
+        <v>16569</v>
+      </c>
+      <c r="L46" s="38">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="M46" s="36">
+        <f>ROUND(K46*(1-L46),0)</f>
+        <v>15426</v>
+      </c>
+      <c r="N46" s="27">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="O46" s="24">
+        <f t="shared" si="405"/>
+        <v>7913.5380000000005</v>
+      </c>
+      <c r="P46" s="38">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="Q46" s="24">
+        <f t="shared" si="406"/>
+        <v>6340.0859999999993</v>
+      </c>
+      <c r="R46" s="38">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="S46" s="134">
+        <v>0.21260000000000001</v>
+      </c>
+      <c r="T46" s="24">
+        <f t="shared" si="407"/>
+        <v>1172.376</v>
+      </c>
+      <c r="U46" s="27">
+        <v>0.253</v>
+      </c>
+      <c r="V46" s="24">
+        <f t="shared" si="408"/>
+        <v>3902.7780000000002</v>
+      </c>
+      <c r="W46" s="38">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="X46" s="24">
+        <f t="shared" si="409"/>
+        <v>7466.1840000000002</v>
+      </c>
+      <c r="Y46" s="38">
+        <v>0.44</v>
+      </c>
+      <c r="Z46" s="24">
+        <f t="shared" si="410"/>
+        <v>6787.44</v>
+      </c>
+      <c r="AA46" s="147">
+        <v>2.6099999999999999E-3</v>
+      </c>
+      <c r="AB46" s="148">
+        <f t="shared" si="411"/>
+        <v>40.261859999999999</v>
+      </c>
+      <c r="AC46" s="46">
+        <v>2.7899999999999999E-3</v>
+      </c>
+      <c r="AD46" s="17">
+        <f t="shared" si="412"/>
+        <v>43.038539999999998</v>
+      </c>
+      <c r="AE46" s="26">
+        <f>IF(M46&gt;0,(AG46+AP46)/M46,0)</f>
+        <v>2.7313980941267991E-3</v>
+      </c>
+      <c r="AF46" s="46">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="AG46" s="36">
+        <f t="shared" si="413"/>
+        <v>4.9363200000000003</v>
+      </c>
+      <c r="AH46" s="27">
+        <v>0.21859999999999999</v>
+      </c>
+      <c r="AI46" s="40">
+        <f t="shared" si="414"/>
+        <v>37.403553000000002</v>
+      </c>
+      <c r="AJ46" s="27">
+        <f t="shared" si="415"/>
+        <v>0.88660252229388048</v>
+      </c>
+      <c r="AK46" s="28">
+        <f t="shared" si="6"/>
+        <v>0.88414529086737415</v>
+      </c>
+      <c r="AL46" s="42">
+        <v>187</v>
+      </c>
+      <c r="AM46" s="38">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN46" s="27">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="AO46" s="134">
+        <v>0.2132</v>
+      </c>
+      <c r="AP46" s="40">
+        <f>AL46*(1-AM46)*AN46</f>
+        <v>37.198227000000003</v>
+      </c>
+      <c r="AQ46" s="135">
+        <f t="shared" si="416"/>
+        <v>36.479586000000005</v>
+      </c>
+      <c r="AR46" s="17">
+        <v>1.6</v>
+      </c>
+      <c r="AS46" s="17"/>
+      <c r="AT46" s="117">
+        <f>AT45+AL46-AS46</f>
+        <v>985.9000000000002</v>
+      </c>
+      <c r="AU46" s="101"/>
+      <c r="AV46" s="42"/>
+      <c r="AW46" s="47"/>
+      <c r="AX46" s="40"/>
+      <c r="AY46" s="40"/>
+      <c r="AZ46" s="40"/>
+      <c r="BA46" s="40"/>
+    </row>
+    <row r="47" spans="1:53" s="21" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="185"/>
+      <c r="B47" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50">
+        <f t="shared" ref="D47" si="417">SUM(D44:D46)</f>
+        <v>42970</v>
+      </c>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50">
+        <f t="shared" ref="F47" si="418">SUM(F44:F46)</f>
+        <v>45806</v>
+      </c>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="50">
+        <f t="shared" ref="I47:K47" si="419">SUM(I44:I46)</f>
+        <v>46162</v>
+      </c>
+      <c r="J47" s="51"/>
+      <c r="K47" s="50">
+        <f t="shared" si="419"/>
+        <v>48526</v>
+      </c>
+      <c r="L47" s="20">
+        <f t="shared" ref="L47" si="420">IF(K47&gt;0,(K44*L44+K45*L45+K46*L46)/K47,0)</f>
+        <v>6.8326814491200608E-2</v>
+      </c>
+      <c r="M47" s="51">
+        <f t="shared" ref="M47" si="421">M44+M45+M46</f>
+        <v>45211</v>
+      </c>
+      <c r="N47" s="52">
+        <f t="shared" ref="N47" si="422">IF(M47&gt;0,O47/M47,0)</f>
+        <v>0.55035761208555445</v>
+      </c>
+      <c r="O47" s="53">
+        <f t="shared" ref="O47" si="423">O44+O45+O46</f>
+        <v>24882.218000000001</v>
+      </c>
+      <c r="P47" s="20">
+        <f t="shared" ref="P47" si="424">IF(M47&gt;0,Q47/M47,0)</f>
+        <v>0.31685277919090488</v>
+      </c>
+      <c r="Q47" s="53">
+        <f t="shared" ref="Q47" si="425">Q44+Q45+Q46</f>
+        <v>14325.231</v>
+      </c>
+      <c r="R47" s="20">
+        <f t="shared" ref="R47" si="426">IF(M47&gt;0,T47/M47,0)</f>
+        <v>0.13278960872354073</v>
+      </c>
+      <c r="S47" s="136"/>
+      <c r="T47" s="53">
+        <f t="shared" ref="T47" si="427">T44+T45+T46</f>
+        <v>6003.5510000000004</v>
+      </c>
+      <c r="U47" s="20">
+        <f t="shared" ref="U47" si="428">IF(M47&gt;0,V47/M47,0)</f>
+        <v>0.23980652938444183</v>
+      </c>
+      <c r="V47" s="53">
+        <f t="shared" ref="V47" si="429">V44+V45+V46</f>
+        <v>10841.893</v>
+      </c>
+      <c r="W47" s="20">
+        <f t="shared" ref="W47" si="430">IF(M47&gt;0,X47/M47,0)</f>
+        <v>0.49521707106677582</v>
+      </c>
+      <c r="X47" s="53">
+        <f t="shared" ref="X47" si="431">X44+X45+X46</f>
+        <v>22389.259000000002</v>
+      </c>
+      <c r="Y47" s="20">
+        <f t="shared" ref="Y47" si="432">IF(M47&gt;0,Z47/M47,0)</f>
+        <v>0.44</v>
+      </c>
+      <c r="Z47" s="53">
+        <f t="shared" ref="Z47" si="433">Z44+Z45+Z46</f>
+        <v>19892.84</v>
+      </c>
+      <c r="AA47" s="152">
+        <f t="shared" ref="AA47" si="434">IF(M47&gt;0,AB47/M47,0)</f>
+        <v>2.5176806529384442E-3</v>
+      </c>
+      <c r="AB47" s="55">
+        <f t="shared" ref="AB47" si="435">SUM(AB44:AB46)</f>
+        <v>113.82686</v>
+      </c>
+      <c r="AC47" s="54">
+        <f t="shared" ref="AC47" si="436">IF(M47&gt;0,AD47/M47,0)</f>
+        <v>2.5460693194134169E-3</v>
+      </c>
+      <c r="AD47" s="55">
+        <f t="shared" ref="AD47" si="437">SUM(AD44:AD46)</f>
+        <v>115.11033999999999</v>
+      </c>
+      <c r="AE47" s="54">
+        <f t="shared" ref="AE47" si="438">IF(M47&gt;0,(AE44*M44+AE45*M45+AE46*M46)/M47,0)</f>
+        <v>2.5674082723231074E-3</v>
+      </c>
+      <c r="AF47" s="54">
+        <f t="shared" ref="AF47" si="439">IF(K47&gt;0,(K44*AF44+K45*AF45+K46*AF46)/K47,0)</f>
+        <v>3.1341445822857849E-4</v>
+      </c>
+      <c r="AG47" s="51">
+        <f t="shared" ref="AG47" si="440">SUM(AG44:AG46)</f>
+        <v>14.169670000000002</v>
+      </c>
+      <c r="AH47" s="52">
+        <f t="shared" ref="AH47" si="441">IF(K47&gt;0,(K44*AH44+K45*AH45+K46*AH46)/K47,0)</f>
+        <v>0.21387195111898777</v>
+      </c>
+      <c r="AI47" s="57">
+        <f t="shared" ref="AI47" si="442">SUM(AI44:AI46)</f>
+        <v>102.00901860000002</v>
+      </c>
+      <c r="AJ47" s="52">
+        <f t="shared" ref="AJ47" si="443">IF(AND(AD47&gt;0),((AD44*AJ44+AD45*AJ45+AD46*AJ46)/AD47),0)</f>
+        <v>0.87819050586697034</v>
+      </c>
+      <c r="AK47" s="56">
+        <f t="shared" si="6"/>
+        <v>0.87921542899595684</v>
+      </c>
+      <c r="AL47" s="50">
+        <f t="shared" ref="AL47" si="444">SUM(AL44:AL46)</f>
+        <v>522</v>
+      </c>
+      <c r="AM47" s="20">
+        <f t="shared" ref="AM47" si="445">IF(AL47&gt;0,(AM44*AL44+AM45*AL45+AM46*AL46)/AL47,0)</f>
+        <v>8.6415708812260544E-2</v>
+      </c>
+      <c r="AN47" s="52">
+        <f>IF(K47&gt;0,(AN44*K44+AN45*K45+AN46*K46)/K47,0)</f>
+        <v>0.21366344021761532</v>
+      </c>
+      <c r="AO47" s="136">
+        <f>IF(L47&gt;0,(AO44*K44+AO45*K45+AO46*K46)/K47,0)</f>
+        <v>0.21270023904710877</v>
+      </c>
+      <c r="AP47" s="57">
+        <f t="shared" ref="AP47" si="446">SUM(AP44:AP46)</f>
+        <v>101.90542540000001</v>
+      </c>
+      <c r="AQ47" s="137">
+        <f t="shared" ref="AQ47" si="447">SUM(AQ44:AQ46)</f>
+        <v>101.3531428</v>
+      </c>
+      <c r="AR47" s="55"/>
+      <c r="AS47" s="55">
+        <f t="shared" ref="AS47" si="448">SUM(AS44:AS46)</f>
+        <v>1018.58</v>
+      </c>
+      <c r="AT47" s="102"/>
+      <c r="AU47" s="103">
+        <f>AT46</f>
+        <v>985.9000000000002</v>
+      </c>
+      <c r="AV47" s="50">
+        <f t="shared" ref="AV47" si="449">SUM(AV44:AV46)</f>
+        <v>0</v>
+      </c>
+      <c r="AW47" s="58"/>
+      <c r="AX47" s="57"/>
+      <c r="AY47" s="57"/>
+      <c r="AZ47" s="57"/>
+      <c r="BA47" s="57"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -50786,13 +51469,22 @@
     <protectedRange sqref="AE36:AE38" name="Range1_1_1_1_1_2_1_8_1_1_1"/>
     <protectedRange sqref="AE40:AE42" name="Range1_1_1_1_1_2_1_9_1_1_1"/>
     <protectedRange sqref="AB28:AB43" name="Range1_1_1_1_1_2_2_1_1_1_2"/>
+    <protectedRange sqref="AP44:AQ47 AK44:AK47 M44:M47" name="Range1_1_1_1_1_1_1_1_1_3"/>
+    <protectedRange sqref="AH47:AJ47 AH44:AI46" name="Range1_1_1_1_1_1_1_3"/>
+    <protectedRange sqref="AJ44:AJ46" name="Range1_1_1_1_3"/>
+    <protectedRange sqref="AD47:AE47 AD44:AD46" name="Range1_1_1_1_1_2_2_1_3"/>
+    <protectedRange sqref="O44:O47" name="Range1_1_1_1_1_5_1_1_3"/>
+    <protectedRange sqref="Q44:Q47" name="Range1_1_1_1_1_7_1_1_3"/>
+    <protectedRange sqref="T44:T47" name="Range1_1_1_1_1_8_1_1_3"/>
+    <protectedRange sqref="V44:V47" name="Range1_1_1_1_1_10_1_1_3"/>
+    <protectedRange sqref="X44:X47" name="Range1_1_1_1_1_12_1_1_3"/>
+    <protectedRange sqref="Z44:Z47" name="Range1_1_1_1_1_16_1_1_3"/>
+    <protectedRange sqref="AG44:AG47" name="Range1_1_1_1_1_18_1_1_3"/>
+    <protectedRange sqref="AE44:AE46" name="Range1_1_1_1_1_2_1_10_1_1_1"/>
+    <protectedRange sqref="AB44:AB47" name="Range1_1_1_1_1_2_2_1_1_1_3"/>
   </protectedRanges>
-  <mergeCells count="15">
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A24:A27"/>
+  <mergeCells count="16">
+    <mergeCell ref="A44:A47"/>
     <mergeCell ref="AX1:AY1"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="A4:A7"/>
@@ -50803,6 +51495,11 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A24:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>